<commit_message>
Issue no. 53 @1337264806
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Template" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$A$3:$J$147</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$A$3:$J$162</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="312">
   <si>
     <t>Konzept</t>
   </si>
@@ -811,9 +811,6 @@
     <t>Handhabung Registry prüfen</t>
   </si>
   <si>
-    <t>Einträge wieder entfernen.</t>
-  </si>
-  <si>
     <t>7118, 7237.</t>
   </si>
   <si>
@@ -961,6 +958,75 @@
   </si>
   <si>
     <t>CatalogDS9 für Contour-Dateien as DS9 eingeführt. Keine Färbung/ Füllung, da innen/ außen nicht ohne weiteres differenzierbar.</t>
+  </si>
+  <si>
+    <t>Einträge wieder entfernen. Push/ pop-Konzept einführen: push entry at index 0/ pop first entry.</t>
+  </si>
+  <si>
+    <t>currentpoint, boundary, quadrant, sign math/ both mit ParserSubstitute lösen</t>
+  </si>
+  <si>
+    <t>Projector, Converter, Baseline überarbeiten</t>
+  </si>
+  <si>
+    <t>Rückgabewerte und Methodenparameter vom Typ List vermeiden</t>
+  </si>
+  <si>
+    <t>Arrays verwenden.</t>
+  </si>
+  <si>
+    <t>Serial-Nummern einführen</t>
+  </si>
+  <si>
+    <t>Obsolet durch fare#135.</t>
+  </si>
+  <si>
+    <t>push/ pop eingeführt durch Stack() in Registry.</t>
+  </si>
+  <si>
+    <t>Einheitlicher Typ für Coordinate</t>
+  </si>
+  <si>
+    <t>HALO-Konzept</t>
+  </si>
+  <si>
+    <t>Unabhängig von ChartAzimuthaltype, applikationsübergreifend</t>
+  </si>
+  <si>
+    <t>ApplicationConstant auflösen</t>
+  </si>
+  <si>
+    <t>LK_/ PK_ lokalisieren.</t>
+  </si>
+  <si>
+    <t>Substitute-Werte überarbeiten</t>
+  </si>
+  <si>
+    <t>double[], Coordinate, CAA[23]Dcoordinate, C-Sequences.</t>
+  </si>
+  <si>
+    <t>CAADate(JD, true) geht 14 Tage nach</t>
+  </si>
+  <si>
+    <t>CAADate() ; Set(JD, true) ; funktioniert.</t>
+  </si>
+  <si>
+    <t>CircleMeridian/ CircleParallel.zenith() vermeiden. PROJ.4, Representations of celestial coordinates in FITS (.pdf in lab/mccm)</t>
+  </si>
+  <si>
+    <t>astrolabe*.properties. In Verbindung mit unregister() können grd (std, grdmin, …) ohne Prefix, da Kontext.</t>
+  </si>
+  <si>
+    <t>getLT() und getST() in HorizonLocal</t>
+  </si>
+  <si>
+    <t>Methoden prüfen und erffs. überarbeiten.</t>
+  </si>
+  <si>
+    <t>GSPaintColor und GSPaintStroke auflösen.</t>
+  </si>
+  <si>
+    <t>Konzept für Postscript GraphicState einführen</t>
   </si>
 </sst>
 </file>
@@ -1115,10 +1181,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1437,7 +1503,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D107" sqref="D107"/>
+      <selection pane="bottomRight" activeCell="B159" sqref="B159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1491,135 +1557,127 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="56.25" hidden="1">
+    <row r="4" spans="2:10">
       <c r="B4" s="5">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="D4" s="6">
-        <v>40959</v>
+        <v>41039</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="G4" s="6">
-        <v>40972</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="I4" s="6"/>
+        <v>310</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:10" ht="33.75" hidden="1">
+    <row r="5" spans="2:10">
       <c r="B5" s="5">
-        <v>115</v>
+        <v>144</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>259</v>
+        <v>308</v>
       </c>
       <c r="D5" s="6">
-        <v>40866</v>
+        <v>41030</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="6">
-        <v>40965</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>280</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B6" s="5">
-        <v>124</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>265</v>
+        <v>9</v>
       </c>
       <c r="D6" s="6">
-        <v>40959</v>
+        <v>39417</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6">
-        <v>40960</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="G6" s="6">
+        <v>40607</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="I6" s="6"/>
       <c r="J6" s="5" t="s">
-        <v>277</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="33.75" hidden="1">
       <c r="B7" s="5">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>268</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6">
-        <v>40959</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>278</v>
+        <v>40</v>
       </c>
       <c r="G7" s="6">
-        <v>40960</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>288</v>
-      </c>
+        <v>39480</v>
+      </c>
+      <c r="H7" s="10"/>
       <c r="I7" s="6"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:10" ht="33.75" hidden="1">
+    <row r="8" spans="2:10" ht="22.5" hidden="1">
       <c r="B8" s="5">
-        <v>103</v>
+        <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>239</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6">
-        <v>40625</v>
+        <v>39417</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>243</v>
+        <v>25</v>
       </c>
       <c r="G8" s="6">
-        <v>40872</v>
+        <v>39480</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
@@ -1627,163 +1685,140 @@
     </row>
     <row r="9" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B9" s="5">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>229</v>
+        <v>11</v>
       </c>
       <c r="D9" s="6">
-        <v>40758</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="F9" s="5" t="s">
-        <v>230</v>
+        <v>39</v>
       </c>
       <c r="G9" s="6">
-        <v>40790</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>235</v>
-      </c>
+        <v>39463</v>
+      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B10" s="5">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="D10" s="6">
-        <v>40625</v>
+        <v>39417</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="G10" s="6">
-        <v>40786</v>
+        <v>39463</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="33.75" hidden="1">
+    <row r="11" spans="2:10" hidden="1">
       <c r="B11" s="5">
-        <v>106</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>228</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C11" s="5"/>
       <c r="D11" s="6">
-        <v>40758</v>
+        <v>39417</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="G11" s="6">
-        <v>40763</v>
+        <v>39463</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:10" ht="22.5" hidden="1">
+    <row r="12" spans="2:10" ht="67.5" hidden="1">
       <c r="B12" s="5">
-        <f>ROW()-3</f>
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>208</v>
-      </c>
+      <c r="C12" s="5"/>
       <c r="D12" s="6">
-        <v>40519</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>39417</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="6">
-        <v>40742</v>
+        <v>39462</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:10" ht="33.75" hidden="1">
+    <row r="13" spans="2:10" ht="78.75" hidden="1">
       <c r="B13" s="5">
-        <f>ROW()-3</f>
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>197</v>
-      </c>
+      <c r="C13" s="5"/>
       <c r="D13" s="6">
-        <v>40519</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="G13" s="6">
-        <v>40607</v>
+        <v>39462</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="2:10" ht="191.25" hidden="1">
+    <row r="14" spans="2:10" ht="33.75" hidden="1">
       <c r="B14" s="5">
-        <f>ROW()-3</f>
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="C14" s="5"/>
       <c r="D14" s="6">
         <v>39417</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="G14" s="6">
-        <v>40607</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>213</v>
-      </c>
+        <v>39462</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="45" hidden="1">
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" ht="33.75" hidden="1">
       <c r="B15" s="5">
-        <v>97</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>211</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C15" s="5"/>
       <c r="D15" s="6">
-        <v>40589</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>212</v>
+        <v>31</v>
       </c>
       <c r="G15" s="6">
-        <v>40600</v>
+        <v>39462</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="6"/>
@@ -1791,23 +1826,20 @@
     </row>
     <row r="16" spans="2:10" ht="45" hidden="1">
       <c r="B16" s="5">
-        <f t="shared" ref="B16:B31" si="0">ROW()-3</f>
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>206</v>
+        <v>29</v>
       </c>
       <c r="D16" s="6">
-        <v>40588</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>60</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>207</v>
+        <v>30</v>
       </c>
       <c r="G16" s="6">
-        <v>40599</v>
+        <v>39462</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
@@ -1815,509 +1847,466 @@
     </row>
     <row r="17" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B17" s="5">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>171</v>
-      </c>
+      <c r="C17" s="5"/>
       <c r="D17" s="6">
-        <v>40239</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>204</v>
+        <v>43</v>
       </c>
       <c r="G17" s="6">
-        <v>40587</v>
+        <v>39462</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10" ht="22.5" hidden="1">
+    <row r="18" spans="2:10" ht="45" hidden="1">
       <c r="B18" s="5">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
       <c r="D18" s="6">
-        <v>39904</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>39417</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="G18" s="6">
-        <v>40587</v>
+        <v>39462</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="6"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10" ht="33.75" hidden="1">
+    <row r="19" spans="2:10" ht="56.25" hidden="1">
       <c r="B19" s="5">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="D19" s="6">
-        <v>39904</v>
+        <v>39417</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="G19" s="6">
-        <v>40587</v>
-      </c>
-      <c r="H19" s="5"/>
+        <v>39456</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="I19" s="6"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10" ht="67.5" hidden="1">
+    <row r="20" spans="2:10" hidden="1">
       <c r="B20" s="5">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D20" s="6">
-        <v>39569</v>
+        <v>39417</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="G20" s="6">
-        <v>40578</v>
+        <v>39456</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>201</v>
+        <v>46</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="2:10" ht="22.5" hidden="1">
       <c r="B21" s="5">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>195</v>
+        <v>23</v>
       </c>
       <c r="D21" s="6">
-        <v>40517</v>
+        <v>39417</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>199</v>
+        <v>24</v>
       </c>
       <c r="G21" s="6">
-        <v>40526</v>
-      </c>
-      <c r="H21" s="5"/>
+        <v>39456</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10" ht="22.5" hidden="1">
+    <row r="22" spans="2:10" hidden="1">
       <c r="B22" s="5">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>194</v>
+        <v>18</v>
       </c>
       <c r="D22" s="6">
-        <v>40461</v>
+        <v>39417</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
       <c r="G22" s="6">
-        <v>40523</v>
+        <v>39456</v>
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="6"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10" ht="168.75" hidden="1">
+    <row r="23" spans="2:10" ht="22.5" hidden="1">
       <c r="B23" s="5">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>170</v>
+        <v>35</v>
       </c>
       <c r="D23" s="6">
-        <v>40239</v>
+        <v>39417</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>196</v>
+        <v>34</v>
       </c>
       <c r="G23" s="6">
-        <v>40517</v>
+        <v>39456</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="6"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10" ht="33.75" hidden="1">
+    <row r="24" spans="2:10" ht="22.5" hidden="1">
       <c r="B24" s="5">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>154</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="6">
-        <v>40098</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>39417</v>
+      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
-        <v>155</v>
+        <v>44</v>
       </c>
       <c r="G24" s="6">
-        <v>40497</v>
+        <v>39452</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10" ht="67.5" hidden="1">
+    <row r="25" spans="2:10" ht="90" hidden="1">
       <c r="B25" s="5">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>150</v>
+        <v>33</v>
       </c>
       <c r="D25" s="6">
-        <v>39904</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>39417</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="G25" s="6">
-        <v>40497</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>192</v>
-      </c>
+        <v>39448</v>
+      </c>
+      <c r="H25" s="5"/>
       <c r="I25" s="6"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10" ht="281.25" hidden="1">
+    <row r="26" spans="2:10" ht="33.75" hidden="1">
       <c r="B26" s="5">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>152</v>
+        <v>26</v>
       </c>
       <c r="D26" s="6">
-        <v>40098</v>
+        <v>39417</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>189</v>
+        <v>27</v>
       </c>
       <c r="G26" s="6">
-        <v>40456</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>190</v>
-      </c>
+        <v>39445</v>
+      </c>
+      <c r="H26" s="5"/>
       <c r="I26" s="6"/>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B27" s="5">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>167</v>
-      </c>
+      <c r="C27" s="5"/>
       <c r="D27" s="6">
-        <v>40228</v>
+        <v>39417</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G27" s="6">
-        <v>40429</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>188</v>
-      </c>
+        <v>39437</v>
+      </c>
+      <c r="H27" s="5"/>
       <c r="I27" s="6"/>
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B28" s="5">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>180</v>
+        <v>36</v>
       </c>
       <c r="D28" s="6">
-        <v>40253</v>
+        <v>39417</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>184</v>
+        <v>37</v>
       </c>
       <c r="G28" s="6">
-        <v>40255</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>185</v>
-      </c>
+        <v>39437</v>
+      </c>
+      <c r="H28" s="5"/>
       <c r="I28" s="6"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="2:10" ht="33.75" hidden="1">
+    <row r="29" spans="2:10" hidden="1">
       <c r="B29" s="5">
-        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
       <c r="D29" s="6">
-        <v>40253</v>
+        <v>39448</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>182</v>
+        <v>50</v>
       </c>
       <c r="G29" s="6">
-        <v>40254</v>
+        <v>39477</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>183</v>
+        <v>62</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10" ht="56.25" hidden="1">
+    <row r="30" spans="2:10" hidden="1">
       <c r="B30" s="5">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>146</v>
-      </c>
+      <c r="C30" s="5"/>
       <c r="D30" s="6">
-        <v>39904</v>
+        <v>39448</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="G30" s="6">
-        <v>40253</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>179</v>
-      </c>
+        <v>39477</v>
+      </c>
+      <c r="H30" s="5"/>
       <c r="I30" s="6"/>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B31" s="5">
-        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>172</v>
-      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="6">
-        <v>40247</v>
+        <v>39448</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>173</v>
+        <v>57</v>
       </c>
       <c r="G31" s="6">
-        <v>40248</v>
-      </c>
-      <c r="H31" s="5"/>
+        <v>39477</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="I31" s="6"/>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B32" s="5">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>215</v>
+        <v>53</v>
       </c>
       <c r="D32" s="6">
-        <v>40625</v>
+        <v>39448</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="G32" s="6"/>
+        <v>52</v>
+      </c>
+      <c r="G32" s="6">
+        <v>39475</v>
+      </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="6">
-        <v>40704</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>224</v>
-      </c>
+      <c r="I32" s="6"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B33" s="5">
-        <v>100</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>216</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="6">
-        <v>40625</v>
+        <v>39448</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="G33" s="6"/>
+        <v>63</v>
+      </c>
+      <c r="G33" s="6">
+        <v>39475</v>
+      </c>
       <c r="H33" s="5"/>
-      <c r="I33" s="6">
-        <v>40704</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>223</v>
-      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B34" s="5">
-        <v>101</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>217</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C34" s="5"/>
       <c r="D34" s="6">
-        <v>40625</v>
+        <v>39448</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="6"/>
+      <c r="F34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G34" s="6">
+        <v>39466</v>
+      </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="6">
-        <v>40704</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>222</v>
-      </c>
+      <c r="I34" s="6"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B35" s="5">
-        <v>102</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>219</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="6">
-        <v>40625</v>
+        <v>39448</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="G35" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="G35" s="6">
+        <v>39465</v>
+      </c>
       <c r="H35" s="5"/>
-      <c r="I35" s="6">
-        <v>40704</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>222</v>
-      </c>
+      <c r="I35" s="6"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B36" s="5">
-        <f t="shared" ref="B36:B73" si="1">ROW()-3</f>
         <v>33</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>174</v>
+        <v>16</v>
       </c>
       <c r="D36" s="6">
-        <v>40247</v>
+        <v>39448</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>175</v>
+        <v>54</v>
       </c>
       <c r="G36" s="6">
-        <v>40248</v>
+        <v>39465</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="6"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="2:10" ht="56.25" hidden="1">
+    <row r="37" spans="2:10" hidden="1">
       <c r="B37" s="5">
-        <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="C37" s="5"/>
       <c r="D37" s="6">
-        <v>40213</v>
+        <v>39448</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>166</v>
+        <v>56</v>
       </c>
       <c r="G37" s="6">
-        <v>40248</v>
+        <v>39465</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="6"/>
@@ -2325,23 +2314,22 @@
     </row>
     <row r="38" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B38" s="5">
-        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D38" s="6">
-        <v>39904</v>
+        <v>39479</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="G38" s="6">
-        <v>40248</v>
+        <v>39518</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="6"/>
@@ -2349,45 +2337,45 @@
     </row>
     <row r="39" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B39" s="5">
-        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>168</v>
+        <v>76</v>
       </c>
       <c r="D39" s="6">
-        <v>40228</v>
+        <v>39479</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>169</v>
+        <v>77</v>
       </c>
       <c r="G39" s="6">
-        <v>40238</v>
+        <v>39518</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="6"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="2:10" ht="22.5" hidden="1">
+    <row r="40" spans="2:10" ht="67.5" hidden="1">
       <c r="B40" s="5">
-        <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>161</v>
+        <v>69</v>
       </c>
       <c r="D40" s="6">
-        <v>40197</v>
+        <v>39479</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>74</v>
+      </c>
       <c r="G40" s="6">
-        <v>40210</v>
+        <v>39507</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="6"/>
@@ -2395,95 +2383,93 @@
     </row>
     <row r="41" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B41" s="5">
-        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>156</v>
+        <v>65</v>
       </c>
       <c r="D41" s="6">
-        <v>40196</v>
+        <v>39479</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>157</v>
+        <v>66</v>
       </c>
       <c r="G41" s="6">
-        <v>40206</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>164</v>
-      </c>
+        <v>39503</v>
+      </c>
+      <c r="H41" s="5"/>
       <c r="I41" s="6"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B42" s="5">
-        <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="D42" s="6">
-        <v>40197</v>
+        <v>39479</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="G42" s="6">
-        <v>40198</v>
-      </c>
-      <c r="H42" s="5"/>
+        <v>39503</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="I42" s="6"/>
       <c r="J42" s="5"/>
     </row>
     <row r="43" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B43" s="5">
-        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="D43" s="6">
-        <v>39904</v>
+        <v>39508</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="G43" s="6">
-        <v>40179</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>160</v>
-      </c>
+        <v>39532</v>
+      </c>
+      <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" s="5"/>
     </row>
     <row r="44" spans="2:10" ht="22.5" hidden="1">
       <c r="B44" s="5">
-        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="D44" s="6">
-        <v>39873</v>
+        <v>39508</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F44" s="5"/>
+      <c r="F44" s="5" t="s">
+        <v>84</v>
+      </c>
       <c r="G44" s="6">
-        <v>39899</v>
+        <v>39528</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
@@ -2491,177 +2477,168 @@
     </row>
     <row r="45" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B45" s="5">
-        <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="D45" s="6">
-        <v>39814</v>
+        <v>39508</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="G45" s="6">
-        <v>39820</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>143</v>
-      </c>
+        <v>39520</v>
+      </c>
+      <c r="H45" s="5"/>
       <c r="I45" s="6"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B46" s="5">
-        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="D46" s="6">
-        <v>39692</v>
+        <v>39508</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="G46" s="6">
-        <v>39695</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="6">
+        <v>39528</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="47" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B47" s="5">
-        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="D47" s="6">
-        <v>39661</v>
+        <v>39508</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G47" s="6">
-        <v>39693</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="6">
+        <v>39538</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="48" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B48" s="5">
-        <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="D48" s="6">
-        <v>40248</v>
+        <v>39569</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="6">
+        <v>200</v>
+      </c>
+      <c r="G48" s="6">
         <v>40578</v>
       </c>
-      <c r="J48" s="5" t="s">
-        <v>205</v>
-      </c>
+      <c r="H48" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="5"/>
     </row>
     <row r="49" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B49" s="5">
-        <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="D49" s="6">
-        <v>39630</v>
+        <v>39569</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="G49" s="6">
-        <v>39660</v>
+        <v>39591</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="5"/>
     </row>
     <row r="50" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B50" s="5">
-        <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="D50" s="6">
-        <v>39630</v>
+        <v>39569</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>123</v>
+      <c r="F50" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="G50" s="6">
-        <v>39647</v>
-      </c>
-      <c r="H50" s="5"/>
+        <v>39586</v>
+      </c>
+      <c r="H50" s="6"/>
       <c r="I50" s="6"/>
       <c r="J50" s="5"/>
     </row>
     <row r="51" spans="2:10" ht="168.75" hidden="1" customHeight="1">
       <c r="B51" s="5">
-        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="D51" s="6">
-        <v>39630</v>
+        <v>39569</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="G51" s="6">
-        <v>39647</v>
+        <v>39586</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="6"/>
@@ -2669,61 +2646,58 @@
     </row>
     <row r="52" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B52" s="5">
-        <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="D52" s="6">
         <v>39569</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G52" s="6">
-        <v>39591</v>
+        <v>39586</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="5"/>
     </row>
     <row r="53" spans="2:10" ht="112.5" hidden="1" customHeight="1">
       <c r="B53" s="5">
-        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="D53" s="6">
         <v>39569</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>112</v>
+        <v>60</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="G53" s="6">
-        <v>39586</v>
-      </c>
-      <c r="H53" s="6"/>
+        <v>39575</v>
+      </c>
+      <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" s="5"/>
     </row>
     <row r="54" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B54" s="5">
-        <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D54" s="6">
         <v>39569</v>
@@ -2732,124 +2706,123 @@
         <v>59</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G54" s="6">
-        <v>39586</v>
-      </c>
-      <c r="H54" s="5"/>
+        <v>39574</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>118</v>
+      </c>
       <c r="I54" s="6"/>
       <c r="J54" s="5"/>
     </row>
     <row r="55" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B55" s="5">
-        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D55" s="6">
         <v>39569</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="G55" s="6">
-        <v>39586</v>
+        <v>39574</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="5"/>
     </row>
     <row r="56" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B56" s="5">
-        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>162</v>
+        <v>95</v>
       </c>
       <c r="D56" s="6">
-        <v>40199</v>
+        <v>39569</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>163</v>
+        <v>96</v>
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="5"/>
       <c r="I56" s="6">
-        <v>40253</v>
+        <v>39591</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>178</v>
+        <v>120</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B57" s="5">
-        <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D57" s="6">
         <v>39569</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="G57" s="6">
-        <v>39575</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G57" s="6"/>
       <c r="H57" s="5"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="5"/>
+      <c r="I57" s="6">
+        <v>39591</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="58" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B58" s="5">
-        <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D58" s="6">
         <v>39569</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G58" s="6">
-        <v>39574</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I58" s="6"/>
-      <c r="J58" s="5"/>
+        <v>103</v>
+      </c>
+      <c r="G58" s="6"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="6">
+        <v>39583</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="59" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B59" s="5">
-        <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D59" s="6">
         <v>39569</v>
@@ -2858,60 +2831,60 @@
         <v>59</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G59" s="6">
-        <v>39574</v>
-      </c>
-      <c r="H59" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I59" s="6"/>
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="2:10" ht="22.5" hidden="1">
+        <v>115</v>
+      </c>
+      <c r="G59" s="6"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="6">
+        <v>39586</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" ht="45" hidden="1">
       <c r="B60" s="5">
-        <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="D60" s="6">
-        <v>39508</v>
+        <v>39630</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="G60" s="6">
-        <v>39532</v>
-      </c>
-      <c r="H60" s="5"/>
+        <v>39660</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>131</v>
+      </c>
       <c r="I60" s="6"/>
       <c r="J60" s="5"/>
     </row>
     <row r="61" spans="2:10" ht="281.25" hidden="1" customHeight="1">
       <c r="B61" s="5">
-        <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="D61" s="6">
-        <v>39508</v>
+        <v>39630</v>
       </c>
       <c r="E61" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="G61" s="6">
-        <v>39528</v>
+        <v>39647</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="6"/>
@@ -2919,23 +2892,22 @@
     </row>
     <row r="62" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B62" s="5">
-        <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>80</v>
+        <v>124</v>
       </c>
       <c r="D62" s="6">
-        <v>39508</v>
+        <v>39630</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>81</v>
+        <v>128</v>
       </c>
       <c r="G62" s="6">
-        <v>39520</v>
+        <v>39647</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="6"/>
@@ -2943,167 +2915,166 @@
     </row>
     <row r="63" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B63" s="5">
-        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="D63" s="6">
-        <v>39479</v>
+        <v>39630</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G63" s="6">
-        <v>39518</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G63" s="6"/>
       <c r="H63" s="5"/>
-      <c r="I63" s="6"/>
-      <c r="J63" s="5"/>
+      <c r="I63" s="6">
+        <v>39647</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="64" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B64" s="5">
-        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>76</v>
+        <v>134</v>
       </c>
       <c r="D64" s="6">
-        <v>39479</v>
+        <v>39661</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>77</v>
+        <v>135</v>
       </c>
       <c r="G64" s="6">
-        <v>39518</v>
-      </c>
-      <c r="H64" s="5"/>
+        <v>39693</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="I64" s="6"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="2:10" ht="67.5" hidden="1">
+    <row r="65" spans="2:10" ht="33.75" hidden="1">
       <c r="B65" s="5">
-        <f t="shared" si="1"/>
         <v>62</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="D65" s="6">
-        <v>39479</v>
+        <v>39692</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="G65" s="6">
-        <v>39507</v>
-      </c>
-      <c r="H65" s="5"/>
+        <v>39695</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>137</v>
+      </c>
       <c r="I65" s="6"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="2:10" ht="45" hidden="1">
+    <row r="66" spans="2:10" ht="90" hidden="1">
       <c r="B66" s="5">
-        <f t="shared" si="1"/>
         <v>63</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="D66" s="6">
-        <v>39479</v>
+        <v>39814</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="G66" s="6">
-        <v>39503</v>
-      </c>
-      <c r="H66" s="5"/>
+        <v>39820</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="I66" s="6"/>
       <c r="J66" s="5"/>
     </row>
     <row r="67" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B67" s="5">
-        <f t="shared" si="1"/>
         <v>64</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="D67" s="6">
-        <v>39479</v>
+        <v>39814</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G67" s="6">
-        <v>39503</v>
-      </c>
-      <c r="H67" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I67" s="6"/>
-      <c r="J67" s="5"/>
+        <v>144</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="6">
+        <v>39832</v>
+      </c>
+      <c r="J67" s="5" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="68" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B68" s="5">
-        <f t="shared" si="1"/>
         <v>65</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>28</v>
+        <v>147</v>
       </c>
       <c r="D68" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5" t="s">
-        <v>40</v>
-      </c>
+        <v>39873</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F68" s="5"/>
       <c r="G68" s="6">
-        <v>39480</v>
-      </c>
-      <c r="H68" s="10"/>
+        <v>39899</v>
+      </c>
+      <c r="H68" s="5"/>
       <c r="I68" s="6"/>
       <c r="J68" s="5"/>
     </row>
     <row r="69" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B69" s="5">
-        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="D69" s="6">
-        <v>39417</v>
+        <v>39904</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F69" s="5"/>
       <c r="G69" s="6">
-        <v>39480</v>
+        <v>40587</v>
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="6"/>
@@ -3111,95 +3082,89 @@
     </row>
     <row r="70" spans="2:10" hidden="1">
       <c r="B70" s="5">
-        <f t="shared" si="1"/>
         <v>67</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>49</v>
+        <v>149</v>
       </c>
       <c r="D70" s="6">
-        <v>39448</v>
+        <v>39904</v>
       </c>
       <c r="E70" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F70" s="5" t="s">
-        <v>50</v>
-      </c>
+      <c r="F70" s="5"/>
       <c r="G70" s="6">
-        <v>39477</v>
-      </c>
-      <c r="H70" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>40587</v>
+      </c>
+      <c r="H70" s="5"/>
       <c r="I70" s="6"/>
       <c r="J70" s="5"/>
     </row>
     <row r="71" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B71" s="5">
-        <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="C71" s="5"/>
+      <c r="C71" s="5" t="s">
+        <v>150</v>
+      </c>
       <c r="D71" s="6">
-        <v>39448</v>
+        <v>39904</v>
       </c>
       <c r="E71" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F71" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="F71" s="5"/>
       <c r="G71" s="6">
-        <v>39477</v>
-      </c>
-      <c r="H71" s="5"/>
+        <v>40497</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>192</v>
+      </c>
       <c r="I71" s="6"/>
       <c r="J71" s="5"/>
     </row>
     <row r="72" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B72" s="5">
-        <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="C72" s="5"/>
+      <c r="C72" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="D72" s="6">
-        <v>39448</v>
+        <v>39904</v>
       </c>
       <c r="E72" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F72" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="F72" s="5"/>
       <c r="G72" s="6">
-        <v>39477</v>
+        <v>40253</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>64</v>
+        <v>179</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="5"/>
     </row>
     <row r="73" spans="2:10" ht="90" hidden="1" customHeight="1">
       <c r="B73" s="5">
-        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="D73" s="6">
-        <v>39448</v>
+        <v>39904</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G73" s="6">
-        <v>39475</v>
+        <v>40248</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="6"/>
@@ -3207,115 +3172,110 @@
     </row>
     <row r="74" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B74" s="5">
-        <f>ROW(B72)-1</f>
         <v>71</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D74" s="6">
-        <v>39814</v>
+        <v>39904</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="G74" s="6"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="6">
-        <v>39832</v>
-      </c>
-      <c r="J74" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+        <v>158</v>
+      </c>
+      <c r="G74" s="6">
+        <v>40179</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I74" s="6"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="2:10" ht="33.75" customHeight="1">
       <c r="B75" s="5">
-        <f>ROW()-3</f>
-        <v>72</v>
-      </c>
-      <c r="C75" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>304</v>
+      </c>
       <c r="D75" s="6">
-        <v>39448</v>
+        <v>41028</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G75" s="6">
-        <v>39475</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="G75" s="6"/>
       <c r="H75" s="5"/>
       <c r="I75" s="6"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="2:10" ht="101.25" hidden="1" customHeight="1">
+    <row r="76" spans="2:10" ht="101.25" customHeight="1">
       <c r="B76" s="5">
-        <f>ROW()-3</f>
-        <v>73</v>
-      </c>
-      <c r="C76" s="5"/>
+        <v>141</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>300</v>
+      </c>
       <c r="D76" s="6">
-        <v>39448</v>
+        <v>41012</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G76" s="6">
-        <v>39466</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="G76" s="6"/>
       <c r="H76" s="5"/>
       <c r="I76" s="6"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="2:10" ht="12.75" hidden="1" customHeight="1">
+    <row r="77" spans="2:10" ht="12.75" customHeight="1">
       <c r="B77" s="5">
-        <f>ROW()-3</f>
-        <v>74</v>
-      </c>
-      <c r="C77" s="5"/>
+        <v>142</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>302</v>
+      </c>
       <c r="D77" s="6">
-        <v>39448</v>
+        <v>41012</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G77" s="6">
-        <v>39465</v>
-      </c>
+        <v>307</v>
+      </c>
+      <c r="G77" s="6"/>
       <c r="H77" s="5"/>
       <c r="I77" s="6"/>
       <c r="J77" s="5"/>
     </row>
     <row r="78" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B78" s="5">
-        <f>ROW()-3</f>
         <v>75</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>16</v>
+        <v>154</v>
       </c>
       <c r="D78" s="6">
-        <v>39448</v>
+        <v>40098</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>54</v>
+        <v>155</v>
       </c>
       <c r="G78" s="6">
-        <v>39465</v>
+        <v>40497</v>
       </c>
       <c r="H78" s="5"/>
       <c r="I78" s="6"/>
@@ -3323,93 +3283,91 @@
     </row>
     <row r="79" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B79" s="5">
-        <f>ROW(B77)-1</f>
         <v>76</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="D79" s="6">
-        <v>39630</v>
+        <v>40098</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="G79" s="6"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="6">
-        <v>39647</v>
-      </c>
-      <c r="J79" s="5" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" ht="27" hidden="1" customHeight="1">
+        <v>189</v>
+      </c>
+      <c r="G79" s="6">
+        <v>40456</v>
+      </c>
+      <c r="H79" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="I79" s="6"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="2:10" ht="27" customHeight="1">
       <c r="B80" s="5">
-        <f>ROW()-3</f>
-        <v>77</v>
-      </c>
-      <c r="C80" s="5"/>
+        <v>139</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="D80" s="6">
-        <v>39448</v>
+        <v>41011</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G80" s="6">
-        <v>39465</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="G80" s="6"/>
       <c r="H80" s="5"/>
       <c r="I80" s="6"/>
       <c r="J80" s="5"/>
     </row>
     <row r="81" spans="2:10" ht="36" hidden="1" customHeight="1">
       <c r="B81" s="5">
-        <f>ROW()-3</f>
         <v>78</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="D81" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E81" s="5"/>
+        <v>40196</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="F81" s="5" t="s">
-        <v>39</v>
+        <v>157</v>
       </c>
       <c r="G81" s="6">
-        <v>39463</v>
-      </c>
-      <c r="H81" s="5"/>
+        <v>40206</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="I81" s="6"/>
       <c r="J81" s="5"/>
     </row>
     <row r="82" spans="2:10" ht="157.5" hidden="1" customHeight="1">
       <c r="B82" s="5">
-        <f>ROW()-3</f>
         <v>79</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>10</v>
+        <v>161</v>
       </c>
       <c r="D82" s="6">
-        <v>39417</v>
+        <v>40197</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>14</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F82" s="5"/>
       <c r="G82" s="6">
-        <v>39463</v>
+        <v>40210</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="6"/>
@@ -3417,21 +3375,20 @@
     </row>
     <row r="83" spans="2:10" ht="112.5" hidden="1" customHeight="1">
       <c r="B83" s="5">
-        <f>ROW()-3</f>
         <v>80</v>
       </c>
-      <c r="C83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>159</v>
+      </c>
       <c r="D83" s="6">
-        <v>39417</v>
+        <v>40197</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F83" s="5"/>
       <c r="G83" s="6">
-        <v>39463</v>
+        <v>40198</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="6"/>
@@ -3439,137 +3396,139 @@
     </row>
     <row r="84" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B84" s="5">
-        <f>ROW()-3</f>
         <v>81</v>
       </c>
-      <c r="C84" s="5"/>
+      <c r="C84" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="D84" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E84" s="5"/>
+        <v>40199</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F84" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G84" s="6">
-        <v>39462</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="G84" s="6"/>
       <c r="H84" s="5"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="5"/>
+      <c r="I84" s="6">
+        <v>40253</v>
+      </c>
+      <c r="J84" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="85" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B85" s="5">
-        <f>ROW(B83)-1</f>
         <v>82</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>95</v>
+        <v>165</v>
       </c>
       <c r="D85" s="6">
-        <v>39569</v>
+        <v>40213</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G85" s="6"/>
+        <v>166</v>
+      </c>
+      <c r="G85" s="6">
+        <v>40248</v>
+      </c>
       <c r="H85" s="5"/>
-      <c r="I85" s="6">
-        <v>39591</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>120</v>
-      </c>
+      <c r="I85" s="6"/>
+      <c r="J85" s="5"/>
     </row>
     <row r="86" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B86" s="5">
-        <f>ROW()-3</f>
         <v>83</v>
       </c>
-      <c r="C86" s="5"/>
+      <c r="C86" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="D86" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E86" s="5"/>
-      <c r="F86" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>40228</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F86" s="5"/>
       <c r="G86" s="6">
-        <v>39462</v>
-      </c>
-      <c r="H86" s="5"/>
+        <v>40429</v>
+      </c>
+      <c r="H86" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="I86" s="6"/>
       <c r="J86" s="5"/>
     </row>
     <row r="87" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B87" s="5">
-        <f>ROW(B85)-1</f>
         <v>84</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>101</v>
+        <v>168</v>
       </c>
       <c r="D87" s="6">
-        <v>39569</v>
+        <v>40228</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G87" s="6"/>
+        <v>169</v>
+      </c>
+      <c r="G87" s="6">
+        <v>40238</v>
+      </c>
       <c r="H87" s="5"/>
-      <c r="I87" s="6">
-        <v>39591</v>
-      </c>
-      <c r="J87" s="5" t="s">
-        <v>121</v>
-      </c>
+      <c r="I87" s="6"/>
+      <c r="J87" s="5"/>
     </row>
     <row r="88" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B88" s="5">
-        <f>ROW(B86)-1</f>
         <v>85</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
       <c r="D88" s="6">
-        <v>39569</v>
+        <v>40239</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G88" s="6"/>
+        <v>204</v>
+      </c>
+      <c r="G88" s="6">
+        <v>40587</v>
+      </c>
       <c r="H88" s="5"/>
-      <c r="I88" s="6">
-        <v>39583</v>
-      </c>
-      <c r="J88" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="I88" s="6"/>
+      <c r="J88" s="5"/>
     </row>
     <row r="89" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B89" s="5">
-        <f>ROW()-3</f>
         <v>86</v>
       </c>
-      <c r="C89" s="5"/>
+      <c r="C89" s="5" t="s">
+        <v>170</v>
+      </c>
       <c r="D89" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E89" s="5"/>
+        <v>40239</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F89" s="5" t="s">
-        <v>42</v>
+        <v>196</v>
       </c>
       <c r="G89" s="6">
-        <v>39462</v>
+        <v>40517</v>
       </c>
       <c r="H89" s="5"/>
       <c r="I89" s="6"/>
@@ -3577,19 +3536,22 @@
     </row>
     <row r="90" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B90" s="5">
-        <f>ROW()-3</f>
         <v>87</v>
       </c>
-      <c r="C90" s="5"/>
+      <c r="C90" s="5" t="s">
+        <v>172</v>
+      </c>
       <c r="D90" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E90" s="5"/>
+        <v>40247</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F90" s="5" t="s">
-        <v>31</v>
+        <v>173</v>
       </c>
       <c r="G90" s="6">
-        <v>39462</v>
+        <v>40248</v>
       </c>
       <c r="H90" s="5"/>
       <c r="I90" s="6"/>
@@ -3597,21 +3559,22 @@
     </row>
     <row r="91" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B91" s="5">
-        <f>ROW()-3</f>
         <v>88</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>29</v>
+        <v>174</v>
       </c>
       <c r="D91" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E91" s="5"/>
+        <v>40247</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F91" s="5" t="s">
-        <v>30</v>
+        <v>175</v>
       </c>
       <c r="G91" s="6">
-        <v>39462</v>
+        <v>40248</v>
       </c>
       <c r="H91" s="5"/>
       <c r="I91" s="6"/>
@@ -3619,245 +3582,227 @@
     </row>
     <row r="92" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B92" s="5">
-        <f>ROW(B90)-1</f>
         <v>89</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>114</v>
+        <v>176</v>
       </c>
       <c r="D92" s="6">
-        <v>39569</v>
+        <v>40248</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="5"/>
       <c r="I92" s="6">
-        <v>39586</v>
+        <v>40578</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>116</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B93" s="5">
-        <f>ROW(B91)-1</f>
         <v>90</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="D93" s="6">
-        <v>39508</v>
+        <v>40253</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="G93" s="6"/>
-      <c r="H93" s="5"/>
-      <c r="I93" s="6">
-        <v>39528</v>
-      </c>
-      <c r="J93" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="G93" s="6">
+        <v>40255</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="I93" s="6"/>
+      <c r="J93" s="5"/>
     </row>
     <row r="94" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B94" s="5">
-        <f>ROW()-3</f>
         <v>91</v>
       </c>
-      <c r="C94" s="5"/>
+      <c r="C94" s="5" t="s">
+        <v>181</v>
+      </c>
       <c r="D94" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E94" s="5"/>
+        <v>40253</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F94" s="5" t="s">
-        <v>43</v>
+        <v>182</v>
       </c>
       <c r="G94" s="6">
-        <v>39462</v>
-      </c>
-      <c r="H94" s="5"/>
+        <v>40254</v>
+      </c>
+      <c r="H94" s="5" t="s">
+        <v>183</v>
+      </c>
       <c r="I94" s="6"/>
       <c r="J94" s="5"/>
     </row>
     <row r="95" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B95" s="5">
-        <f>ROW()-3</f>
         <v>92</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>12</v>
+        <v>194</v>
       </c>
       <c r="D95" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E95" s="5"/>
+        <v>40461</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F95" s="5" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G95" s="6">
-        <v>39462</v>
+        <v>40523</v>
       </c>
       <c r="H95" s="5"/>
       <c r="I95" s="6"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="96" spans="2:10" ht="22.5" customHeight="1">
       <c r="B96" s="5">
-        <f>ROW(B94)-1</f>
-        <v>93</v>
+        <v>140</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>89</v>
+        <v>298</v>
       </c>
       <c r="D96" s="6">
-        <v>39508</v>
+        <v>41011</v>
       </c>
       <c r="E96" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>85</v>
+        <v>299</v>
       </c>
       <c r="G96" s="6"/>
       <c r="H96" s="5"/>
-      <c r="I96" s="6">
-        <v>39538</v>
-      </c>
-      <c r="J96" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="I96" s="6"/>
+      <c r="J96" s="5"/>
     </row>
     <row r="97" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B97" s="5">
-        <f t="shared" ref="B97:B106" si="2">ROW()-3</f>
         <v>94</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>19</v>
+        <v>195</v>
       </c>
       <c r="D97" s="6">
-        <v>39417</v>
+        <v>40517</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>20</v>
+        <v>199</v>
       </c>
       <c r="G97" s="6">
-        <v>39456</v>
-      </c>
-      <c r="H97" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>40526</v>
+      </c>
+      <c r="H97" s="5"/>
       <c r="I97" s="6"/>
       <c r="J97" s="5"/>
     </row>
     <row r="98" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B98" s="5">
-        <f t="shared" si="2"/>
         <v>95</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>38</v>
+        <v>208</v>
       </c>
       <c r="D98" s="6">
-        <v>39417</v>
+        <v>40519</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F98" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="F98" s="5"/>
       <c r="G98" s="6">
-        <v>39456</v>
-      </c>
-      <c r="H98" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>40742</v>
+      </c>
+      <c r="H98" s="5"/>
       <c r="I98" s="6"/>
       <c r="J98" s="5"/>
     </row>
     <row r="99" spans="2:10" ht="78.75" hidden="1" customHeight="1">
       <c r="B99" s="5">
-        <f t="shared" si="2"/>
         <v>96</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>23</v>
+        <v>197</v>
       </c>
       <c r="D99" s="6">
-        <v>39417</v>
+        <v>40519</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>24</v>
+        <v>198</v>
       </c>
       <c r="G99" s="6">
-        <v>39456</v>
-      </c>
-      <c r="H99" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>40607</v>
+      </c>
+      <c r="H99" s="5"/>
       <c r="I99" s="6"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+    <row r="100" spans="2:10" ht="67.5" customHeight="1">
       <c r="B100" s="5">
-        <f t="shared" si="2"/>
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>18</v>
+        <v>290</v>
       </c>
       <c r="D100" s="6">
-        <v>39417</v>
+        <v>40998</v>
       </c>
       <c r="E100" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F100" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G100" s="6">
-        <v>39456</v>
-      </c>
+      <c r="F100" s="5"/>
+      <c r="G100" s="6"/>
       <c r="H100" s="5"/>
       <c r="I100" s="6"/>
       <c r="J100" s="5"/>
     </row>
     <row r="101" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B101" s="5">
-        <f t="shared" si="2"/>
         <v>98</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>35</v>
+        <v>206</v>
       </c>
       <c r="D101" s="6">
-        <v>39417</v>
+        <v>40588</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>34</v>
+        <v>207</v>
       </c>
       <c r="G101" s="6">
-        <v>39456</v>
+        <v>40599</v>
       </c>
       <c r="H101" s="5"/>
       <c r="I101" s="6"/>
@@ -3865,65 +3810,64 @@
     </row>
     <row r="102" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B102" s="5">
-        <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="C102" s="5"/>
+      <c r="C102" s="5" t="s">
+        <v>211</v>
+      </c>
       <c r="D102" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E102" s="5"/>
+        <v>40589</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="F102" s="5" t="s">
-        <v>44</v>
+        <v>212</v>
       </c>
       <c r="G102" s="6">
-        <v>39452</v>
+        <v>40600</v>
       </c>
       <c r="H102" s="5"/>
       <c r="I102" s="6"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="2:10" ht="12.75" hidden="1" customHeight="1">
+    <row r="103" spans="2:10" ht="12.75" customHeight="1">
       <c r="B103" s="5">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>33</v>
+        <v>292</v>
       </c>
       <c r="D103" s="6">
-        <v>39417</v>
-      </c>
-      <c r="E103" s="5"/>
+        <v>40998</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F103" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G103" s="6">
-        <v>39448</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="G103" s="6"/>
       <c r="H103" s="5"/>
       <c r="I103" s="6"/>
       <c r="J103" s="5"/>
     </row>
     <row r="104" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B104" s="5">
-        <f t="shared" si="2"/>
         <v>101</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>26</v>
+        <v>214</v>
       </c>
       <c r="D104" s="6">
-        <v>39417</v>
+        <v>40625</v>
       </c>
       <c r="E104" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F104" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="F104" s="5"/>
       <c r="G104" s="6">
-        <v>39445</v>
+        <v>40786</v>
       </c>
       <c r="H104" s="5"/>
       <c r="I104" s="6"/>
@@ -3931,122 +3875,134 @@
     </row>
     <row r="105" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B105" s="5">
-        <f t="shared" si="2"/>
         <v>102</v>
       </c>
-      <c r="C105" s="5"/>
+      <c r="C105" s="5" t="s">
+        <v>215</v>
+      </c>
       <c r="D105" s="6">
-        <v>39417</v>
+        <v>40625</v>
       </c>
       <c r="E105" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G105" s="6">
-        <v>39437</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="G105" s="6"/>
       <c r="H105" s="5"/>
-      <c r="I105" s="6"/>
-      <c r="J105" s="5"/>
+      <c r="I105" s="6">
+        <v>40704</v>
+      </c>
+      <c r="J105" s="5" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="106" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B106" s="5">
-        <f t="shared" si="2"/>
         <v>103</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>36</v>
+        <v>216</v>
       </c>
       <c r="D106" s="6">
-        <v>39417</v>
+        <v>40625</v>
       </c>
       <c r="E106" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G106" s="6">
-        <v>39437</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="G106" s="6"/>
       <c r="H106" s="5"/>
-      <c r="I106" s="6"/>
-      <c r="J106" s="5"/>
-    </row>
-    <row r="107" spans="2:10" ht="22.5" customHeight="1">
+      <c r="I106" s="6">
+        <v>40704</v>
+      </c>
+      <c r="J106" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B107" s="5">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>286</v>
+        <v>217</v>
       </c>
       <c r="D107" s="6">
-        <v>40982</v>
+        <v>40625</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F107" s="5" t="s">
-        <v>287</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F107" s="5"/>
       <c r="G107" s="6"/>
       <c r="H107" s="5"/>
-      <c r="I107" s="6"/>
-      <c r="J107" s="5"/>
-    </row>
-    <row r="108" spans="2:10" ht="12.75" customHeight="1">
+      <c r="I107" s="6">
+        <v>40704</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="108" spans="2:10" ht="22.5" hidden="1">
       <c r="B108" s="5">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>283</v>
+        <v>219</v>
       </c>
       <c r="D108" s="6">
-        <v>40972</v>
+        <v>40625</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>284</v>
+        <v>220</v>
       </c>
       <c r="G108" s="6"/>
       <c r="H108" s="5"/>
-      <c r="I108" s="6"/>
-      <c r="J108" s="5"/>
-    </row>
-    <row r="109" spans="2:10" ht="22.5" customHeight="1">
+      <c r="I108" s="6">
+        <v>40704</v>
+      </c>
+      <c r="J108" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B109" s="5">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="D109" s="6">
-        <v>40959</v>
+        <v>40625</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="G109" s="6"/>
+        <v>242</v>
+      </c>
+      <c r="G109" s="6">
+        <v>40872</v>
+      </c>
       <c r="H109" s="5"/>
       <c r="I109" s="6"/>
       <c r="J109" s="5"/>
     </row>
     <row r="110" spans="2:10" ht="12.75" customHeight="1">
       <c r="B110" s="5">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="D110" s="6">
-        <v>40959</v>
+        <v>40998</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>59</v>
@@ -4057,188 +4013,194 @@
       <c r="I110" s="6"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="2:10">
+    <row r="111" spans="2:10" ht="33.75">
       <c r="B111" s="5">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>266</v>
+        <v>291</v>
       </c>
       <c r="D111" s="6">
-        <v>40959</v>
+        <v>40983</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>267</v>
+        <v>306</v>
       </c>
       <c r="G111" s="6"/>
       <c r="H111" s="5"/>
       <c r="I111" s="6"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="2:10">
+    <row r="112" spans="2:10" ht="22.5" hidden="1">
       <c r="B112" s="5">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
       <c r="D112" s="6">
-        <v>40956</v>
+        <v>40758</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F112" s="5"/>
-      <c r="G112" s="6"/>
+      <c r="G112" s="6">
+        <v>40763</v>
+      </c>
       <c r="H112" s="5"/>
       <c r="I112" s="6"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10" ht="45">
+    <row r="113" spans="2:10" ht="33.75" hidden="1">
       <c r="B113" s="5">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="D113" s="6">
-        <v>40956</v>
+        <v>40758</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="G113" s="6"/>
-      <c r="H113" s="5"/>
+        <v>230</v>
+      </c>
+      <c r="G113" s="6">
+        <v>40790</v>
+      </c>
+      <c r="H113" s="5" t="s">
+        <v>235</v>
+      </c>
       <c r="I113" s="6"/>
       <c r="J113" s="5"/>
     </row>
     <row r="114" spans="2:10">
       <c r="B114" s="5">
-        <v>119</v>
+        <v>133</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="D114" s="6">
-        <v>40947</v>
+        <v>40972</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F114" s="5"/>
+      <c r="F114" s="5" t="s">
+        <v>283</v>
+      </c>
       <c r="G114" s="6"/>
-      <c r="H114" s="5" t="s">
-        <v>279</v>
-      </c>
+      <c r="H114" s="5"/>
       <c r="I114" s="6"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="2:10" ht="45">
+    <row r="115" spans="2:10" ht="22.5">
       <c r="B115" s="5">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="D115" s="6">
-        <v>40947</v>
+        <v>40959</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G115" s="6"/>
       <c r="H115" s="5"/>
       <c r="I115" s="6"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="2:10" ht="33.75" customHeight="1">
+    <row r="116" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B116" s="5">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="D116" s="6">
-        <v>40941</v>
+        <v>40794</v>
       </c>
       <c r="E116" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="G116" s="6"/>
-      <c r="H116" s="5"/>
+        <v>238</v>
+      </c>
+      <c r="G116" s="6">
+        <v>40987</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>288</v>
+      </c>
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>
     <row r="117" spans="2:10" ht="33.75" customHeight="1">
       <c r="B117" s="5">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>249</v>
+        <v>284</v>
       </c>
       <c r="D117" s="6">
-        <v>40869</v>
+        <v>40959</v>
       </c>
       <c r="E117" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F117" s="5" t="s">
-        <v>250</v>
-      </c>
+      <c r="F117" s="5"/>
       <c r="G117" s="6"/>
       <c r="H117" s="5"/>
       <c r="I117" s="6"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="2:10" ht="22.5">
+    <row r="118" spans="2:10">
       <c r="B118" s="5">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="D118" s="6">
-        <v>40866</v>
+        <v>40959</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="G118" s="6"/>
       <c r="H118" s="5"/>
       <c r="I118" s="6"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="2:10" ht="33.75">
+    <row r="119" spans="2:10">
       <c r="B119" s="5">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>245</v>
+        <v>259</v>
       </c>
       <c r="D119" s="6">
-        <v>40829</v>
+        <v>40956</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F119" s="5" t="s">
-        <v>246</v>
-      </c>
+      <c r="F119" s="5"/>
       <c r="G119" s="6"/>
       <c r="H119" s="5"/>
       <c r="I119" s="6"/>
@@ -4246,19 +4208,19 @@
     </row>
     <row r="120" spans="2:10" ht="33.75" customHeight="1">
       <c r="B120" s="5">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="D120" s="6">
-        <v>40829</v>
+        <v>40956</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>248</v>
+        <v>261</v>
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="5"/>
@@ -4267,86 +4229,84 @@
     </row>
     <row r="121" spans="2:10">
       <c r="B121" s="5">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="D121" s="6">
-        <v>40822</v>
+        <v>40947</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>271</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F121" s="5"/>
       <c r="G121" s="6"/>
-      <c r="H121" s="5"/>
+      <c r="H121" s="5" t="s">
+        <v>278</v>
+      </c>
       <c r="I121" s="6"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="2:10" ht="22.5" customHeight="1">
+    <row r="122" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B122" s="5">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="D122" s="6">
-        <v>40816</v>
+        <v>40866</v>
       </c>
       <c r="E122" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F122" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="G122" s="6"/>
-      <c r="H122" s="5"/>
+      <c r="F122" s="5"/>
+      <c r="G122" s="6">
+        <v>40965</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="I122" s="6"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+    <row r="123" spans="2:10" ht="67.5" customHeight="1">
       <c r="B123" s="5">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>236</v>
+        <v>256</v>
       </c>
       <c r="D123" s="6">
-        <v>40794</v>
+        <v>40947</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="G123" s="6">
-        <v>40987</v>
-      </c>
-      <c r="H123" s="5" t="s">
-        <v>289</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="G123" s="6"/>
+      <c r="H123" s="5"/>
       <c r="I123" s="6"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="2:10" ht="22.5">
+    <row r="124" spans="2:10" ht="33.75">
       <c r="B124" s="5">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="D124" s="6">
-        <v>40794</v>
+        <v>40941</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="5"/>
@@ -4355,19 +4315,19 @@
     </row>
     <row r="125" spans="2:10" ht="12.75" customHeight="1">
       <c r="B125" s="5">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="D125" s="6">
-        <v>40763</v>
+        <v>40869</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="G125" s="6"/>
       <c r="H125" s="5"/>
@@ -4376,40 +4336,40 @@
     </row>
     <row r="126" spans="2:10" ht="22.5" customHeight="1">
       <c r="B126" s="5">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
       <c r="D126" s="6">
-        <v>40762</v>
+        <v>40866</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="5"/>
       <c r="I126" s="6"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="2:10" ht="22.5">
+    <row r="127" spans="2:10" ht="33.75">
       <c r="B127" s="5">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>226</v>
+        <v>244</v>
       </c>
       <c r="D127" s="6">
-        <v>40750</v>
+        <v>40829</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>227</v>
+        <v>245</v>
       </c>
       <c r="G127" s="6"/>
       <c r="H127" s="5"/>
@@ -4418,19 +4378,19 @@
     </row>
     <row r="128" spans="2:10" ht="12.75" customHeight="1">
       <c r="B128" s="5">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="D128" s="6">
-        <v>40742</v>
+        <v>40829</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="5"/>
@@ -4439,20 +4399,19 @@
     </row>
     <row r="129" spans="2:10" ht="22.5" customHeight="1">
       <c r="B129" s="5">
-        <f>ROW()-3</f>
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="D129" s="6">
-        <v>40589</v>
+        <v>40822</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>210</v>
+        <v>270</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="5"/>
@@ -4461,188 +4420,227 @@
     </row>
     <row r="130" spans="2:10" ht="12.75" customHeight="1">
       <c r="B130" s="5">
-        <f>ROW()-3</f>
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="D130" s="6">
-        <v>40566</v>
+        <v>40816</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>203</v>
+        <v>289</v>
       </c>
       <c r="G130" s="6"/>
-      <c r="H130" s="5"/>
+      <c r="H130" s="5" t="s">
+        <v>296</v>
+      </c>
       <c r="I130" s="6"/>
       <c r="J130" s="5"/>
     </row>
     <row r="131" spans="2:10" ht="22.5" customHeight="1">
       <c r="B131" s="5">
-        <f>ROW()-3</f>
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="D131" s="6">
-        <v>40506</v>
+        <v>40794</v>
       </c>
       <c r="E131" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="G131" s="6"/>
       <c r="H131" s="5"/>
       <c r="I131" s="6"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="2:10">
+    <row r="132" spans="2:10" ht="22.5">
       <c r="B132" s="5">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="D132" s="6">
-        <v>40188</v>
+        <v>40763</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F132" s="5"/>
+      <c r="F132" s="5" t="s">
+        <v>234</v>
+      </c>
       <c r="G132" s="6"/>
       <c r="H132" s="5"/>
       <c r="I132" s="6"/>
       <c r="J132" s="5"/>
     </row>
-    <row r="133" spans="2:10">
+    <row r="133" spans="2:10" ht="67.5" hidden="1">
       <c r="B133" s="5">
-        <f>ROW()-3</f>
         <v>130</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>138</v>
+        <v>264</v>
       </c>
       <c r="D133" s="6">
-        <v>39904</v>
+        <v>40959</v>
       </c>
       <c r="E133" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F133" s="5"/>
+      <c r="F133" s="5" t="s">
+        <v>275</v>
+      </c>
       <c r="G133" s="6"/>
       <c r="H133" s="5"/>
-      <c r="I133" s="6"/>
-      <c r="J133" s="5"/>
-    </row>
-    <row r="134" spans="2:10">
+      <c r="I133" s="6">
+        <v>40960</v>
+      </c>
+      <c r="J133" s="5" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="134" spans="2:10" ht="33.75" hidden="1">
       <c r="B134" s="5">
-        <f>ROW()-3</f>
         <v>131</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>139</v>
+        <v>267</v>
       </c>
       <c r="D134" s="6">
-        <v>39904</v>
+        <v>40959</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F134" s="5"/>
-      <c r="G134" s="6"/>
-      <c r="H134" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="G134" s="6">
+        <v>40960</v>
+      </c>
+      <c r="H134" s="5" t="s">
+        <v>287</v>
+      </c>
       <c r="I134" s="6"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="2:10" ht="22.5">
+    <row r="135" spans="2:10" ht="56.25" hidden="1">
       <c r="B135" s="5">
-        <f>ROW()-3</f>
         <v>132</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>153</v>
+        <v>268</v>
       </c>
       <c r="D135" s="6">
-        <v>39904</v>
+        <v>40959</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F135" s="5"/>
-      <c r="G135" s="6"/>
-      <c r="H135" s="5"/>
+      <c r="F135" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G135" s="6">
+        <v>40972</v>
+      </c>
+      <c r="H135" s="5" t="s">
+        <v>281</v>
+      </c>
       <c r="I135" s="6"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="2:10" ht="22.5">
+    <row r="136" spans="2:10">
       <c r="B136" s="5">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="D136" s="6">
-        <v>39122</v>
+        <v>40762</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F136" s="5"/>
+      <c r="F136" s="5" t="s">
+        <v>232</v>
+      </c>
       <c r="G136" s="6"/>
       <c r="H136" s="5"/>
       <c r="I136" s="6"/>
       <c r="J136" s="5"/>
     </row>
-    <row r="137" spans="2:10" ht="22.5">
+    <row r="137" spans="2:10" hidden="1">
       <c r="B137" s="5">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="D137" s="6">
-        <v>39122</v>
+        <v>40982</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="5"/>
-      <c r="I137" s="6"/>
-      <c r="J137" s="5"/>
-    </row>
-    <row r="138" spans="2:10">
+      <c r="I137" s="6">
+        <v>41011</v>
+      </c>
+      <c r="J137" s="5" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="138" spans="2:10" ht="22.5">
       <c r="B138" s="5">
-        <v>135</v>
-      </c>
-      <c r="C138" s="5"/>
-      <c r="D138" s="6"/>
-      <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
+        <v>108</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D138" s="6">
+        <v>40750</v>
+      </c>
+      <c r="E138" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>227</v>
+      </c>
       <c r="G138" s="6"/>
       <c r="H138" s="5"/>
       <c r="I138" s="6"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="2:10">
+    <row r="139" spans="2:10" ht="33.75">
       <c r="B139" s="5">
-        <v>136</v>
-      </c>
-      <c r="C139" s="5"/>
-      <c r="D139" s="6"/>
-      <c r="E139" s="5"/>
-      <c r="F139" s="5"/>
+        <v>107</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D139" s="6">
+        <v>40742</v>
+      </c>
+      <c r="E139" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F139" s="5" t="s">
+        <v>243</v>
+      </c>
       <c r="G139" s="6"/>
       <c r="H139" s="5"/>
       <c r="I139" s="6"/>
@@ -4650,38 +4648,62 @@
     </row>
     <row r="140" spans="2:10">
       <c r="B140" s="5">
-        <v>137</v>
-      </c>
-      <c r="C140" s="5"/>
-      <c r="D140" s="6"/>
-      <c r="E140" s="5"/>
-      <c r="F140" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D140" s="6">
+        <v>40589</v>
+      </c>
+      <c r="E140" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>210</v>
+      </c>
       <c r="G140" s="6"/>
       <c r="H140" s="5"/>
       <c r="I140" s="6"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="2:10">
+    <row r="141" spans="2:10" ht="67.5">
       <c r="B141" s="5">
-        <v>138</v>
-      </c>
-      <c r="C141" s="5"/>
-      <c r="D141" s="6"/>
-      <c r="E141" s="5"/>
-      <c r="F141" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D141" s="6">
+        <v>40566</v>
+      </c>
+      <c r="E141" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F141" s="5" t="s">
+        <v>203</v>
+      </c>
       <c r="G141" s="6"/>
       <c r="H141" s="5"/>
       <c r="I141" s="6"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10">
+    <row r="142" spans="2:10" ht="33.75">
       <c r="B142" s="5">
-        <v>139</v>
-      </c>
-      <c r="C142" s="5"/>
-      <c r="D142" s="6"/>
-      <c r="E142" s="5"/>
-      <c r="F142" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D142" s="6">
+        <v>40506</v>
+      </c>
+      <c r="E142" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F142" s="5" t="s">
+        <v>252</v>
+      </c>
       <c r="G142" s="6"/>
       <c r="H142" s="5"/>
       <c r="I142" s="6"/>
@@ -4689,11 +4711,17 @@
     </row>
     <row r="143" spans="2:10">
       <c r="B143" s="5">
-        <v>140</v>
-      </c>
-      <c r="C143" s="5"/>
-      <c r="D143" s="6"/>
-      <c r="E143" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D143" s="6">
+        <v>40188</v>
+      </c>
+      <c r="E143" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F143" s="5"/>
       <c r="G143" s="6"/>
       <c r="H143" s="5"/>
@@ -4702,11 +4730,17 @@
     </row>
     <row r="144" spans="2:10">
       <c r="B144" s="5">
-        <v>141</v>
-      </c>
-      <c r="C144" s="5"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D144" s="6">
+        <v>39904</v>
+      </c>
+      <c r="E144" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F144" s="5"/>
       <c r="G144" s="6"/>
       <c r="H144" s="5"/>
@@ -4715,56 +4749,86 @@
     </row>
     <row r="145" spans="2:10">
       <c r="B145" s="5">
-        <v>142</v>
-      </c>
-      <c r="C145" s="5"/>
-      <c r="D145" s="6"/>
-      <c r="E145" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D145" s="6">
+        <v>39904</v>
+      </c>
+      <c r="E145" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F145" s="5"/>
       <c r="G145" s="6"/>
       <c r="H145" s="5"/>
       <c r="I145" s="6"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="2:10">
+    <row r="146" spans="2:10" ht="22.5">
       <c r="B146" s="5">
-        <v>143</v>
-      </c>
-      <c r="C146" s="5"/>
-      <c r="D146" s="6"/>
-      <c r="E146" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D146" s="6">
+        <v>39904</v>
+      </c>
+      <c r="E146" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F146" s="5"/>
       <c r="G146" s="6"/>
       <c r="H146" s="5"/>
       <c r="I146" s="6"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="2:10">
+    <row r="147" spans="2:10" ht="22.5">
       <c r="B147" s="5">
-        <v>144</v>
-      </c>
-      <c r="C147" s="5"/>
-      <c r="D147" s="6"/>
-      <c r="E147" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D147" s="6">
+        <v>39122</v>
+      </c>
+      <c r="E147" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F147" s="5"/>
       <c r="G147" s="6"/>
       <c r="H147" s="5"/>
       <c r="I147" s="6"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10">
-      <c r="B148" s="5"/>
-      <c r="C148" s="5"/>
-      <c r="D148" s="6"/>
-      <c r="E148" s="5"/>
-      <c r="F148" s="5"/>
+    <row r="148" spans="2:10" ht="22.5">
+      <c r="B148" s="5">
+        <v>2</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D148" s="6">
+        <v>39122</v>
+      </c>
+      <c r="E148" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F148" s="5" t="s">
+        <v>274</v>
+      </c>
       <c r="G148" s="6"/>
       <c r="H148" s="5"/>
-      <c r="I148" s="5"/>
+      <c r="I148" s="6"/>
       <c r="J148" s="5"/>
     </row>
     <row r="149" spans="2:10">
-      <c r="B149" s="5"/>
+      <c r="B149" s="5">
+        <v>146</v>
+      </c>
       <c r="C149" s="5"/>
       <c r="D149" s="6"/>
       <c r="E149" s="5"/>
@@ -4775,7 +4839,9 @@
       <c r="J149" s="5"/>
     </row>
     <row r="150" spans="2:10">
-      <c r="B150" s="5"/>
+      <c r="B150" s="5">
+        <v>147</v>
+      </c>
       <c r="C150" s="5"/>
       <c r="D150" s="6"/>
       <c r="E150" s="5"/>
@@ -4786,7 +4852,9 @@
       <c r="J150" s="5"/>
     </row>
     <row r="151" spans="2:10">
-      <c r="B151" s="5"/>
+      <c r="B151" s="5">
+        <v>148</v>
+      </c>
       <c r="C151" s="5"/>
       <c r="D151" s="6"/>
       <c r="E151" s="5"/>
@@ -4797,7 +4865,9 @@
       <c r="J151" s="5"/>
     </row>
     <row r="152" spans="2:10">
-      <c r="B152" s="5"/>
+      <c r="B152" s="5">
+        <v>149</v>
+      </c>
       <c r="C152" s="5"/>
       <c r="D152" s="6"/>
       <c r="E152" s="5"/>
@@ -4808,7 +4878,9 @@
       <c r="J152" s="5"/>
     </row>
     <row r="153" spans="2:10">
-      <c r="B153" s="5"/>
+      <c r="B153" s="5">
+        <v>150</v>
+      </c>
       <c r="C153" s="5"/>
       <c r="D153" s="6"/>
       <c r="E153" s="5"/>
@@ -4819,7 +4891,9 @@
       <c r="J153" s="5"/>
     </row>
     <row r="154" spans="2:10">
-      <c r="B154" s="5"/>
+      <c r="B154" s="5">
+        <v>151</v>
+      </c>
       <c r="C154" s="5"/>
       <c r="D154" s="6"/>
       <c r="E154" s="5"/>
@@ -4830,7 +4904,9 @@
       <c r="J154" s="5"/>
     </row>
     <row r="155" spans="2:10">
-      <c r="B155" s="5"/>
+      <c r="B155" s="5">
+        <v>152</v>
+      </c>
       <c r="C155" s="5"/>
       <c r="D155" s="6"/>
       <c r="E155" s="5"/>
@@ -4841,7 +4917,9 @@
       <c r="J155" s="5"/>
     </row>
     <row r="156" spans="2:10">
-      <c r="B156" s="5"/>
+      <c r="B156" s="5">
+        <v>153</v>
+      </c>
       <c r="C156" s="5"/>
       <c r="D156" s="6"/>
       <c r="E156" s="5"/>
@@ -4852,7 +4930,9 @@
       <c r="J156" s="5"/>
     </row>
     <row r="157" spans="2:10">
-      <c r="B157" s="5"/>
+      <c r="B157" s="5">
+        <v>154</v>
+      </c>
       <c r="C157" s="5"/>
       <c r="D157" s="6"/>
       <c r="E157" s="5"/>
@@ -4863,7 +4943,9 @@
       <c r="J157" s="5"/>
     </row>
     <row r="158" spans="2:10">
-      <c r="B158" s="5"/>
+      <c r="B158" s="5">
+        <v>155</v>
+      </c>
       <c r="C158" s="5"/>
       <c r="D158" s="6"/>
       <c r="E158" s="5"/>
@@ -4874,7 +4956,9 @@
       <c r="J158" s="5"/>
     </row>
     <row r="159" spans="2:10">
-      <c r="B159" s="5"/>
+      <c r="B159" s="5">
+        <v>156</v>
+      </c>
       <c r="C159" s="5"/>
       <c r="D159" s="6"/>
       <c r="E159" s="5"/>
@@ -4885,7 +4969,9 @@
       <c r="J159" s="5"/>
     </row>
     <row r="160" spans="2:10">
-      <c r="B160" s="5"/>
+      <c r="B160" s="5">
+        <v>157</v>
+      </c>
       <c r="C160" s="5"/>
       <c r="D160" s="6"/>
       <c r="E160" s="5"/>
@@ -4896,7 +4982,9 @@
       <c r="J160" s="5"/>
     </row>
     <row r="161" spans="2:10">
-      <c r="B161" s="5"/>
+      <c r="B161" s="5">
+        <v>158</v>
+      </c>
       <c r="C161" s="5"/>
       <c r="D161" s="6"/>
       <c r="E161" s="5"/>
@@ -4907,7 +4995,9 @@
       <c r="J161" s="5"/>
     </row>
     <row r="162" spans="2:10">
-      <c r="B162" s="5"/>
+      <c r="B162" s="5">
+        <v>159</v>
+      </c>
       <c r="C162" s="5"/>
       <c r="D162" s="6"/>
       <c r="E162" s="5"/>
@@ -5985,15 +6075,15 @@
       <c r="J259" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J147">
+  <autoFilter ref="A3:J162">
     <filterColumn colId="6">
       <filters blank="1"/>
     </filterColumn>
     <filterColumn colId="8">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="B107:J147">
-      <sortCondition descending="1" ref="D3:D147"/>
+    <sortState ref="B4:J162">
+      <sortCondition descending="1" ref="D3:D162"/>
     </sortState>
   </autoFilter>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Issue no. 54 @1339531427
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Template" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$A$3:$J$162</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$B$3:$J$162</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="317">
   <si>
     <t>Konzept</t>
   </si>
@@ -257,9 +257,6 @@
   </si>
   <si>
     <t>Nur getName() entfernt.</t>
-  </si>
-  <si>
-    <t>Circle-Attribut fov bezeichnet Circle-Gruppe, die Sichtfenster festlegt. Catalog-Attribut fov verweist auf Circle-Gruppe. Eine Circle-Gruppe definiert ein Outline eines fov. Bei Catalog mehrere fov durch Komma getrennt: 1. ist Outline des fov, folgende sind Löcher im fov.</t>
   </si>
   <si>
     <t>.properties speichert substitutes und locales. Index für locales ist ident aus ADC. Substitutes sind Katalogname, Konstallationsname, Abkürzung, Nominativ, Genitiv, Locale-Name.
@@ -1027,6 +1024,25 @@
   </si>
   <si>
     <t>Konzept für Postscript GraphicState einführen</t>
+  </si>
+  <si>
+    <t>Globale Parameter über Registry</t>
+  </si>
+  <si>
+    <t>Projector, Epoch</t>
+  </si>
+  <si>
+    <t>In Atlas.map für Klassen Atlas*, DMS und Rational in &lt;class&gt; Element verify-constructable="false" einfügen (s. Kap. 7.4 in Castor XML Mapping).</t>
+  </si>
+  <si>
+    <t>Castor-Default-Konstruktor-Check umgehen</t>
+  </si>
+  <si>
+    <t>11.06.2012: Erste Umsetzung am 29.02.2008.</t>
+  </si>
+  <si>
+    <t>Circle-Attribut fov bezeichnet Circle-Gruppe, die Sichtfenster festlegt. Catalog-Attribut fov verweist auf Circle-Gruppe. Eine Circle-Gruppe definiert ein Outline eines fov. fov immer geschlossen (Polygon). Geschlossener fov ersetzt ggf. vorhandenen, offener schneidet ggf. vorhandenen falls genau 2 Schnittpunkte, !!!Konzept für Auswahl der resultierenden!!!
+Bei Catalog mehrere fov durch Komma getrennt: 1. ist Outline des fov, folgende sind Löcher im fov.</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1519,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B159" sqref="B159"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1570,21 +1586,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:10" ht="33.75">
       <c r="B4" s="5">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D4" s="6">
-        <v>41039</v>
+        <v>41059</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="5"/>
@@ -1593,23 +1609,23 @@
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="5">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D5" s="6">
-        <v>41030</v>
+        <v>41057</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="8"/>
-      <c r="I5" s="6"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="67.5" hidden="1" customHeight="1">
@@ -1626,17 +1642,17 @@
         <v>59</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G6" s="6">
         <v>40607</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="33.75" hidden="1">
@@ -2326,7 +2342,7 @@
         <v>59</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G38" s="6">
         <v>39518</v>
@@ -2340,7 +2356,7 @@
         <v>36</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D39" s="6">
         <v>39479</v>
@@ -2349,7 +2365,7 @@
         <v>60</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G39" s="6">
         <v>39518</v>
@@ -2358,27 +2374,25 @@
       <c r="I39" s="6"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="2:10" ht="67.5" hidden="1">
+    <row r="40" spans="2:10">
       <c r="B40" s="5">
-        <v>37</v>
+        <v>145</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>69</v>
+        <v>310</v>
       </c>
       <c r="D40" s="6">
-        <v>39479</v>
+        <v>41039</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G40" s="6">
-        <v>39507</v>
-      </c>
+        <v>309</v>
+      </c>
+      <c r="G40" s="6"/>
       <c r="H40" s="5"/>
-      <c r="I40" s="6"/>
+      <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="2:10" ht="33.75" hidden="1" customHeight="1">
@@ -2434,7 +2448,7 @@
         <v>40</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" s="6">
         <v>39508</v>
@@ -2443,7 +2457,7 @@
         <v>60</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G43" s="6">
         <v>39532</v>
@@ -2457,7 +2471,7 @@
         <v>41</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D44" s="6">
         <v>39508</v>
@@ -2466,7 +2480,7 @@
         <v>59</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G44" s="6">
         <v>39528</v>
@@ -2480,7 +2494,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="6">
         <v>39508</v>
@@ -2489,7 +2503,7 @@
         <v>60</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G45" s="6">
         <v>39520</v>
@@ -2503,7 +2517,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D46" s="6">
         <v>39508</v>
@@ -2512,7 +2526,7 @@
         <v>60</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="5"/>
@@ -2520,7 +2534,7 @@
         <v>39528</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="33.75" hidden="1" customHeight="1">
@@ -2528,7 +2542,7 @@
         <v>44</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" s="6">
         <v>39508</v>
@@ -2537,7 +2551,7 @@
         <v>59</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="5"/>
@@ -2545,7 +2559,7 @@
         <v>39538</v>
       </c>
       <c r="J47" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="56.25" hidden="1" customHeight="1">
@@ -2562,13 +2576,13 @@
         <v>60</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G48" s="6">
         <v>40578</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="5"/>
@@ -2578,7 +2592,7 @@
         <v>46</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" s="6">
         <v>39569</v>
@@ -2587,13 +2601,13 @@
         <v>59</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G49" s="6">
         <v>39591</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="5"/>
@@ -2603,7 +2617,7 @@
         <v>47</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D50" s="6">
         <v>39569</v>
@@ -2612,7 +2626,7 @@
         <v>59</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G50" s="6">
         <v>39586</v>
@@ -2626,7 +2640,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D51" s="6">
         <v>39569</v>
@@ -2635,7 +2649,7 @@
         <v>59</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G51" s="6">
         <v>39586</v>
@@ -2649,7 +2663,7 @@
         <v>49</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D52" s="6">
         <v>39569</v>
@@ -2658,13 +2672,13 @@
         <v>60</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G52" s="6">
         <v>39586</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="5"/>
@@ -2674,7 +2688,7 @@
         <v>50</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D53" s="6">
         <v>39569</v>
@@ -2683,7 +2697,7 @@
         <v>60</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G53" s="6">
         <v>39575</v>
@@ -2697,7 +2711,7 @@
         <v>51</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D54" s="6">
         <v>39569</v>
@@ -2706,13 +2720,13 @@
         <v>59</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G54" s="6">
         <v>39574</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="5"/>
@@ -2722,7 +2736,7 @@
         <v>52</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D55" s="6">
         <v>39569</v>
@@ -2731,13 +2745,13 @@
         <v>59</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G55" s="6">
         <v>39574</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="5"/>
@@ -2747,7 +2761,7 @@
         <v>53</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D56" s="6">
         <v>39569</v>
@@ -2756,7 +2770,7 @@
         <v>59</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="5"/>
@@ -2764,7 +2778,7 @@
         <v>39591</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="2:10" ht="45" hidden="1" customHeight="1">
@@ -2772,7 +2786,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D57" s="6">
         <v>39569</v>
@@ -2781,7 +2795,7 @@
         <v>59</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="5"/>
@@ -2789,7 +2803,7 @@
         <v>39591</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="2:10" ht="22.5" hidden="1" customHeight="1">
@@ -2797,7 +2811,7 @@
         <v>55</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D58" s="6">
         <v>39569</v>
@@ -2806,7 +2820,7 @@
         <v>60</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="5"/>
@@ -2814,7 +2828,7 @@
         <v>39583</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="2:10" ht="45" hidden="1" customHeight="1">
@@ -2822,7 +2836,7 @@
         <v>56</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D59" s="6">
         <v>39569</v>
@@ -2831,7 +2845,7 @@
         <v>59</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="5"/>
@@ -2839,7 +2853,7 @@
         <v>39586</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="60" spans="2:10" ht="45" hidden="1">
@@ -2847,7 +2861,7 @@
         <v>57</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D60" s="6">
         <v>39630</v>
@@ -2856,13 +2870,13 @@
         <v>59</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G60" s="6">
         <v>39660</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="5"/>
@@ -2872,7 +2886,7 @@
         <v>58</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D61" s="6">
         <v>39630</v>
@@ -2881,7 +2895,7 @@
         <v>59</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G61" s="6">
         <v>39647</v>
@@ -2895,7 +2909,7 @@
         <v>59</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D62" s="6">
         <v>39630</v>
@@ -2904,7 +2918,7 @@
         <v>59</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G62" s="6">
         <v>39647</v>
@@ -2918,7 +2932,7 @@
         <v>60</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D63" s="6">
         <v>39630</v>
@@ -2927,7 +2941,7 @@
         <v>59</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="5"/>
@@ -2935,7 +2949,7 @@
         <v>39647</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="2:10" ht="56.25" hidden="1" customHeight="1">
@@ -2943,7 +2957,7 @@
         <v>61</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D64" s="6">
         <v>39661</v>
@@ -2952,13 +2966,13 @@
         <v>59</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G64" s="6">
         <v>39693</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I64" s="6"/>
       <c r="J64" s="5"/>
@@ -2968,7 +2982,7 @@
         <v>62</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D65" s="6">
         <v>39692</v>
@@ -2977,13 +2991,13 @@
         <v>59</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G65" s="6">
         <v>39695</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="5"/>
@@ -2993,7 +3007,7 @@
         <v>63</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D66" s="6">
         <v>39814</v>
@@ -3002,13 +3016,13 @@
         <v>59</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G66" s="6">
         <v>39820</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I66" s="6"/>
       <c r="J66" s="5"/>
@@ -3018,7 +3032,7 @@
         <v>64</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D67" s="6">
         <v>39814</v>
@@ -3027,7 +3041,7 @@
         <v>59</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="5"/>
@@ -3035,7 +3049,7 @@
         <v>39832</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="2:10" ht="33.75" hidden="1" customHeight="1">
@@ -3043,7 +3057,7 @@
         <v>65</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D68" s="6">
         <v>39873</v>
@@ -3064,7 +3078,7 @@
         <v>66</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D69" s="6">
         <v>39904</v>
@@ -3085,7 +3099,7 @@
         <v>67</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D70" s="6">
         <v>39904</v>
@@ -3106,7 +3120,7 @@
         <v>68</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D71" s="6">
         <v>39904</v>
@@ -3119,7 +3133,7 @@
         <v>40497</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I71" s="6"/>
       <c r="J71" s="5"/>
@@ -3129,7 +3143,7 @@
         <v>69</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D72" s="6">
         <v>39904</v>
@@ -3142,7 +3156,7 @@
         <v>40253</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="5"/>
@@ -3152,7 +3166,7 @@
         <v>70</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D73" s="6">
         <v>39904</v>
@@ -3161,7 +3175,7 @@
         <v>59</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G73" s="6">
         <v>40248</v>
@@ -3175,7 +3189,7 @@
         <v>71</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D74" s="6">
         <v>39904</v>
@@ -3184,32 +3198,32 @@
         <v>60</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G74" s="6">
         <v>40179</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="5"/>
     </row>
     <row r="75" spans="2:10" ht="33.75" customHeight="1">
       <c r="B75" s="5">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="D75" s="6">
-        <v>41028</v>
+        <v>41030</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="5"/>
@@ -3218,19 +3232,19 @@
     </row>
     <row r="76" spans="2:10" ht="101.25" customHeight="1">
       <c r="B76" s="5">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D76" s="6">
-        <v>41012</v>
+        <v>41028</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="5"/>
@@ -3239,10 +3253,10 @@
     </row>
     <row r="77" spans="2:10" ht="12.75" customHeight="1">
       <c r="B77" s="5">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D77" s="6">
         <v>41012</v>
@@ -3251,7 +3265,7 @@
         <v>59</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="5"/>
@@ -3263,7 +3277,7 @@
         <v>75</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D78" s="6">
         <v>40098</v>
@@ -3272,7 +3286,7 @@
         <v>59</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G78" s="6">
         <v>40497</v>
@@ -3286,7 +3300,7 @@
         <v>76</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D79" s="6">
         <v>40098</v>
@@ -3295,32 +3309,32 @@
         <v>59</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G79" s="6">
         <v>40456</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I79" s="6"/>
       <c r="J79" s="5"/>
     </row>
     <row r="80" spans="2:10" ht="27" customHeight="1">
       <c r="B80" s="5">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D80" s="6">
-        <v>41011</v>
+        <v>41012</v>
       </c>
       <c r="E80" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="G80" s="6"/>
       <c r="H80" s="5"/>
@@ -3332,7 +3346,7 @@
         <v>78</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D81" s="6">
         <v>40196</v>
@@ -3341,13 +3355,13 @@
         <v>60</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G81" s="6">
         <v>40206</v>
       </c>
       <c r="H81" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I81" s="6"/>
       <c r="J81" s="5"/>
@@ -3357,7 +3371,7 @@
         <v>79</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D82" s="6">
         <v>40197</v>
@@ -3378,7 +3392,7 @@
         <v>80</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D83" s="6">
         <v>40197</v>
@@ -3399,7 +3413,7 @@
         <v>81</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D84" s="6">
         <v>40199</v>
@@ -3408,7 +3422,7 @@
         <v>59</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G84" s="6"/>
       <c r="H84" s="5"/>
@@ -3416,7 +3430,7 @@
         <v>40253</v>
       </c>
       <c r="J84" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="85" spans="2:10" ht="12.75" hidden="1" customHeight="1">
@@ -3424,7 +3438,7 @@
         <v>82</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D85" s="6">
         <v>40213</v>
@@ -3433,7 +3447,7 @@
         <v>59</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G85" s="6">
         <v>40248</v>
@@ -3447,7 +3461,7 @@
         <v>83</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D86" s="6">
         <v>40228</v>
@@ -3460,7 +3474,7 @@
         <v>40429</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I86" s="6"/>
       <c r="J86" s="5"/>
@@ -3470,7 +3484,7 @@
         <v>84</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D87" s="6">
         <v>40228</v>
@@ -3479,7 +3493,7 @@
         <v>60</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G87" s="6">
         <v>40238</v>
@@ -3493,7 +3507,7 @@
         <v>85</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D88" s="6">
         <v>40239</v>
@@ -3502,7 +3516,7 @@
         <v>59</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G88" s="6">
         <v>40587</v>
@@ -3516,7 +3530,7 @@
         <v>86</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D89" s="6">
         <v>40239</v>
@@ -3525,7 +3539,7 @@
         <v>59</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G89" s="6">
         <v>40517</v>
@@ -3539,7 +3553,7 @@
         <v>87</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D90" s="6">
         <v>40247</v>
@@ -3548,7 +3562,7 @@
         <v>59</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G90" s="6">
         <v>40248</v>
@@ -3562,7 +3576,7 @@
         <v>88</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D91" s="6">
         <v>40247</v>
@@ -3571,7 +3585,7 @@
         <v>59</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G91" s="6">
         <v>40248</v>
@@ -3585,7 +3599,7 @@
         <v>89</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D92" s="6">
         <v>40248</v>
@@ -3594,7 +3608,7 @@
         <v>60</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="5"/>
@@ -3602,7 +3616,7 @@
         <v>40578</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="2:10" ht="12.75" hidden="1" customHeight="1">
@@ -3610,7 +3624,7 @@
         <v>90</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D93" s="6">
         <v>40253</v>
@@ -3619,13 +3633,13 @@
         <v>60</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G93" s="6">
         <v>40255</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="5"/>
@@ -3635,7 +3649,7 @@
         <v>91</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D94" s="6">
         <v>40253</v>
@@ -3644,13 +3658,13 @@
         <v>59</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G94" s="6">
         <v>40254</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I94" s="6"/>
       <c r="J94" s="5"/>
@@ -3660,7 +3674,7 @@
         <v>92</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D95" s="6">
         <v>40461</v>
@@ -3669,7 +3683,7 @@
         <v>59</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G95" s="6">
         <v>40523</v>
@@ -3680,10 +3694,10 @@
     </row>
     <row r="96" spans="2:10" ht="22.5" customHeight="1">
       <c r="B96" s="5">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D96" s="6">
         <v>41011</v>
@@ -3692,7 +3706,7 @@
         <v>59</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="G96" s="6"/>
       <c r="H96" s="5"/>
@@ -3704,7 +3718,7 @@
         <v>94</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D97" s="6">
         <v>40517</v>
@@ -3713,7 +3727,7 @@
         <v>60</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G97" s="6">
         <v>40526</v>
@@ -3727,7 +3741,7 @@
         <v>95</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D98" s="6">
         <v>40519</v>
@@ -3748,7 +3762,7 @@
         <v>96</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D99" s="6">
         <v>40519</v>
@@ -3757,7 +3771,7 @@
         <v>59</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G99" s="6">
         <v>40607</v>
@@ -3766,12 +3780,12 @@
       <c r="I99" s="6"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="2:10" ht="67.5" customHeight="1">
+    <row r="100" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B100" s="5">
         <v>136</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D100" s="6">
         <v>40998</v>
@@ -3780,7 +3794,9 @@
         <v>59</v>
       </c>
       <c r="F100" s="5"/>
-      <c r="G100" s="6"/>
+      <c r="G100" s="6">
+        <v>41046</v>
+      </c>
       <c r="H100" s="5"/>
       <c r="I100" s="6"/>
       <c r="J100" s="5"/>
@@ -3790,7 +3806,7 @@
         <v>98</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D101" s="6">
         <v>40588</v>
@@ -3799,7 +3815,7 @@
         <v>60</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G101" s="6">
         <v>40599</v>
@@ -3813,7 +3829,7 @@
         <v>99</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D102" s="6">
         <v>40589</v>
@@ -3822,7 +3838,7 @@
         <v>60</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G102" s="6">
         <v>40600</v>
@@ -3833,19 +3849,19 @@
     </row>
     <row r="103" spans="2:10" ht="12.75" customHeight="1">
       <c r="B103" s="5">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="D103" s="6">
-        <v>40998</v>
+        <v>41011</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="5"/>
@@ -3857,7 +3873,7 @@
         <v>101</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D104" s="6">
         <v>40625</v>
@@ -3878,7 +3894,7 @@
         <v>102</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D105" s="6">
         <v>40625</v>
@@ -3887,7 +3903,7 @@
         <v>59</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="5"/>
@@ -3895,7 +3911,7 @@
         <v>40704</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="106" spans="2:10" ht="12.75" hidden="1" customHeight="1">
@@ -3903,7 +3919,7 @@
         <v>103</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D106" s="6">
         <v>40625</v>
@@ -3912,7 +3928,7 @@
         <v>59</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G106" s="6"/>
       <c r="H106" s="5"/>
@@ -3920,7 +3936,7 @@
         <v>40704</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="107" spans="2:10" ht="22.5" hidden="1" customHeight="1">
@@ -3928,7 +3944,7 @@
         <v>104</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D107" s="6">
         <v>40625</v>
@@ -3943,7 +3959,7 @@
         <v>40704</v>
       </c>
       <c r="J107" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="108" spans="2:10" ht="22.5" hidden="1">
@@ -3951,7 +3967,7 @@
         <v>105</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D108" s="6">
         <v>40625</v>
@@ -3960,7 +3976,7 @@
         <v>59</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G108" s="6"/>
       <c r="H108" s="5"/>
@@ -3968,7 +3984,7 @@
         <v>40704</v>
       </c>
       <c r="J108" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="109" spans="2:10" ht="22.5" hidden="1" customHeight="1">
@@ -3976,7 +3992,7 @@
         <v>106</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D109" s="6">
         <v>40625</v>
@@ -3985,7 +4001,7 @@
         <v>59</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G109" s="6">
         <v>40872</v>
@@ -3996,10 +4012,10 @@
     </row>
     <row r="110" spans="2:10" ht="12.75" customHeight="1">
       <c r="B110" s="5">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D110" s="6">
         <v>40998</v>
@@ -4007,28 +4023,28 @@
       <c r="E110" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F110" s="5"/>
+      <c r="F110" s="5" t="s">
+        <v>292</v>
+      </c>
       <c r="G110" s="6"/>
       <c r="H110" s="5"/>
       <c r="I110" s="6"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="2:10" ht="33.75">
+    <row r="111" spans="2:10">
       <c r="B111" s="5">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D111" s="6">
-        <v>40983</v>
+        <v>40998</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F111" s="5" t="s">
-        <v>306</v>
-      </c>
+      <c r="F111" s="5"/>
       <c r="G111" s="6"/>
       <c r="H111" s="5"/>
       <c r="I111" s="6"/>
@@ -4039,7 +4055,7 @@
         <v>109</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D112" s="6">
         <v>40758</v>
@@ -4060,7 +4076,7 @@
         <v>110</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D113" s="6">
         <v>40758</v>
@@ -4069,53 +4085,53 @@
         <v>59</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G113" s="6">
         <v>40790</v>
       </c>
       <c r="H113" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I113" s="6"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="2:10">
+    <row r="114" spans="2:10" ht="33.75">
       <c r="B114" s="5">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="D114" s="6">
-        <v>40972</v>
+        <v>40983</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="G114" s="6"/>
       <c r="H114" s="5"/>
       <c r="I114" s="6"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="2:10" ht="22.5">
+    <row r="115" spans="2:10">
       <c r="B115" s="5">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>262</v>
+        <v>281</v>
       </c>
       <c r="D115" s="6">
-        <v>40959</v>
+        <v>40972</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="G115" s="6"/>
       <c r="H115" s="5"/>
@@ -4127,7 +4143,7 @@
         <v>113</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D116" s="6">
         <v>40794</v>
@@ -4136,23 +4152,23 @@
         <v>59</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G116" s="6">
         <v>40987</v>
       </c>
       <c r="H116" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>
     <row r="117" spans="2:10" ht="33.75" customHeight="1">
       <c r="B117" s="5">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="D117" s="6">
         <v>40959</v>
@@ -4160,7 +4176,9 @@
       <c r="E117" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F117" s="5"/>
+      <c r="F117" s="5" t="s">
+        <v>262</v>
+      </c>
       <c r="G117" s="6"/>
       <c r="H117" s="5"/>
       <c r="I117" s="6"/>
@@ -4168,10 +4186,10 @@
     </row>
     <row r="118" spans="2:10">
       <c r="B118" s="5">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>265</v>
+        <v>283</v>
       </c>
       <c r="D118" s="6">
         <v>40959</v>
@@ -4179,9 +4197,7 @@
       <c r="E118" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F118" s="5" t="s">
-        <v>266</v>
-      </c>
+      <c r="F118" s="5"/>
       <c r="G118" s="6"/>
       <c r="H118" s="5"/>
       <c r="I118" s="6"/>
@@ -4189,18 +4205,20 @@
     </row>
     <row r="119" spans="2:10">
       <c r="B119" s="5">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="D119" s="6">
-        <v>40956</v>
+        <v>40959</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F119" s="5"/>
+      <c r="F119" s="5" t="s">
+        <v>265</v>
+      </c>
       <c r="G119" s="6"/>
       <c r="H119" s="5"/>
       <c r="I119" s="6"/>
@@ -4208,10 +4226,10 @@
     </row>
     <row r="120" spans="2:10" ht="33.75" customHeight="1">
       <c r="B120" s="5">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D120" s="6">
         <v>40956</v>
@@ -4219,32 +4237,30 @@
       <c r="E120" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F120" s="5" t="s">
-        <v>261</v>
-      </c>
+      <c r="F120" s="5"/>
       <c r="G120" s="6"/>
       <c r="H120" s="5"/>
       <c r="I120" s="6"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="2:10">
+    <row r="121" spans="2:10" ht="45">
       <c r="B121" s="5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="D121" s="6">
-        <v>40947</v>
+        <v>40956</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F121" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F121" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="G121" s="6"/>
-      <c r="H121" s="5" t="s">
-        <v>278</v>
-      </c>
+      <c r="H121" s="5"/>
       <c r="I121" s="6"/>
       <c r="J121" s="5"/>
     </row>
@@ -4253,7 +4269,7 @@
         <v>119</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D122" s="6">
         <v>40866</v>
@@ -4266,47 +4282,47 @@
         <v>40965</v>
       </c>
       <c r="H122" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I122" s="6"/>
       <c r="J122" s="5"/>
     </row>
     <row r="123" spans="2:10" ht="67.5" customHeight="1">
       <c r="B123" s="5">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D123" s="6">
         <v>40947</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F123" s="5" t="s">
-        <v>257</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F123" s="5"/>
       <c r="G123" s="6"/>
-      <c r="H123" s="5"/>
+      <c r="H123" s="5" t="s">
+        <v>277</v>
+      </c>
       <c r="I123" s="6"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="2:10" ht="33.75">
+    <row r="124" spans="2:10" ht="45">
       <c r="B124" s="5">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D124" s="6">
-        <v>40941</v>
+        <v>40947</v>
       </c>
       <c r="E124" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="5"/>
@@ -4315,19 +4331,19 @@
     </row>
     <row r="125" spans="2:10" ht="12.75" customHeight="1">
       <c r="B125" s="5">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="D125" s="6">
-        <v>40869</v>
+        <v>40941</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="G125" s="6"/>
       <c r="H125" s="5"/>
@@ -4336,40 +4352,40 @@
     </row>
     <row r="126" spans="2:10" ht="22.5" customHeight="1">
       <c r="B126" s="5">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D126" s="6">
-        <v>40866</v>
+        <v>40869</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="5"/>
       <c r="I126" s="6"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="2:10" ht="33.75">
+    <row r="127" spans="2:10" ht="22.5">
       <c r="B127" s="5">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D127" s="6">
-        <v>40829</v>
+        <v>40866</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="G127" s="6"/>
       <c r="H127" s="5"/>
@@ -4378,10 +4394,10 @@
     </row>
     <row r="128" spans="2:10" ht="12.75" customHeight="1">
       <c r="B128" s="5">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D128" s="6">
         <v>40829</v>
@@ -4390,7 +4406,7 @@
         <v>59</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="5"/>
@@ -4399,19 +4415,19 @@
     </row>
     <row r="129" spans="2:10" ht="22.5" customHeight="1">
       <c r="B129" s="5">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="D129" s="6">
-        <v>40822</v>
+        <v>40829</v>
       </c>
       <c r="E129" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="5"/>
@@ -4420,63 +4436,63 @@
     </row>
     <row r="130" spans="2:10" ht="12.75" customHeight="1">
       <c r="B130" s="5">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
       <c r="D130" s="6">
-        <v>40816</v>
+        <v>40822</v>
       </c>
       <c r="E130" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>289</v>
+        <v>269</v>
       </c>
       <c r="G130" s="6"/>
-      <c r="H130" s="5" t="s">
-        <v>296</v>
-      </c>
+      <c r="H130" s="5"/>
       <c r="I130" s="6"/>
       <c r="J130" s="5"/>
     </row>
     <row r="131" spans="2:10" ht="22.5" customHeight="1">
       <c r="B131" s="5">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="D131" s="6">
-        <v>40794</v>
+        <v>40816</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>240</v>
+        <v>288</v>
       </c>
       <c r="G131" s="6"/>
-      <c r="H131" s="5"/>
+      <c r="H131" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="I131" s="6"/>
       <c r="J131" s="5"/>
     </row>
     <row r="132" spans="2:10" ht="22.5">
       <c r="B132" s="5">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="D132" s="6">
-        <v>40763</v>
+        <v>40794</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="5"/>
@@ -4488,7 +4504,7 @@
         <v>130</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D133" s="6">
         <v>40959</v>
@@ -4497,7 +4513,7 @@
         <v>59</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G133" s="6"/>
       <c r="H133" s="5"/>
@@ -4505,7 +4521,7 @@
         <v>40960</v>
       </c>
       <c r="J133" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="134" spans="2:10" ht="33.75" hidden="1">
@@ -4513,7 +4529,7 @@
         <v>131</v>
       </c>
       <c r="C134" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D134" s="6">
         <v>40959</v>
@@ -4522,13 +4538,13 @@
         <v>60</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G134" s="6">
         <v>40960</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I134" s="6"/>
       <c r="J134" s="5"/>
@@ -4538,7 +4554,7 @@
         <v>132</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D135" s="6">
         <v>40959</v>
@@ -4547,32 +4563,32 @@
         <v>59</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G135" s="6">
         <v>40972</v>
       </c>
       <c r="H135" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I135" s="6"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="2:10">
+    <row r="136" spans="2:10" ht="22.5">
       <c r="B136" s="5">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D136" s="6">
-        <v>40762</v>
+        <v>40763</v>
       </c>
       <c r="E136" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="5"/>
@@ -4584,7 +4600,7 @@
         <v>134</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D137" s="6">
         <v>40982</v>
@@ -4593,7 +4609,7 @@
         <v>60</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="5"/>
@@ -4601,128 +4617,130 @@
         <v>41011</v>
       </c>
       <c r="J137" s="5" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="138" spans="2:10" ht="22.5">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="138" spans="2:10">
       <c r="B138" s="5">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D138" s="6">
-        <v>40750</v>
+        <v>40762</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="5"/>
       <c r="I138" s="6"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="2:10" ht="33.75">
+    <row r="139" spans="2:10" ht="22.5">
       <c r="B139" s="5">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>225</v>
       </c>
       <c r="D139" s="6">
-        <v>40742</v>
+        <v>40750</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="G139" s="6"/>
       <c r="H139" s="5"/>
       <c r="I139" s="6"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="2:10">
+    <row r="140" spans="2:10" ht="33.75">
       <c r="B140" s="5">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="D140" s="6">
-        <v>40589</v>
+        <v>40742</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>210</v>
+        <v>242</v>
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="5"/>
       <c r="I140" s="6"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="2:10" ht="67.5">
+    <row r="141" spans="2:10">
       <c r="B141" s="5">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="D141" s="6">
-        <v>40566</v>
+        <v>40589</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="G141" s="6"/>
       <c r="H141" s="5"/>
       <c r="I141" s="6"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10" ht="33.75">
+    <row r="142" spans="2:10" ht="67.5">
       <c r="B142" s="5">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="D142" s="6">
-        <v>40506</v>
+        <v>40566</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="G142" s="6"/>
       <c r="H142" s="5"/>
       <c r="I142" s="6"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="2:10">
+    <row r="143" spans="2:10" ht="33.75">
       <c r="B143" s="5">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>271</v>
+        <v>192</v>
       </c>
       <c r="D143" s="6">
-        <v>40188</v>
+        <v>40506</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F143" s="5"/>
+      <c r="F143" s="5" t="s">
+        <v>251</v>
+      </c>
       <c r="G143" s="6"/>
       <c r="H143" s="5"/>
       <c r="I143" s="6"/>
@@ -4730,13 +4748,13 @@
     </row>
     <row r="144" spans="2:10">
       <c r="B144" s="5">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>138</v>
+        <v>270</v>
       </c>
       <c r="D144" s="6">
-        <v>39904</v>
+        <v>40188</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>59</v>
@@ -4749,10 +4767,10 @@
     </row>
     <row r="145" spans="2:10">
       <c r="B145" s="5">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D145" s="6">
         <v>39904</v>
@@ -4766,12 +4784,12 @@
       <c r="I145" s="6"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="2:10" ht="22.5">
+    <row r="146" spans="2:10">
       <c r="B146" s="5">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D146" s="6">
         <v>39904</v>
@@ -4787,13 +4805,13 @@
     </row>
     <row r="147" spans="2:10" ht="22.5">
       <c r="B147" s="5">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>272</v>
+        <v>152</v>
       </c>
       <c r="D147" s="6">
-        <v>39122</v>
+        <v>39904</v>
       </c>
       <c r="E147" s="5" t="s">
         <v>59</v>
@@ -4804,51 +4822,67 @@
       <c r="I147" s="6"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10" ht="22.5">
+    <row r="148" spans="2:10" ht="112.5">
       <c r="B148" s="5">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>273</v>
+        <v>69</v>
       </c>
       <c r="D148" s="6">
-        <v>39122</v>
+        <v>39479</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F148" s="5" t="s">
-        <v>274</v>
+        <v>316</v>
       </c>
       <c r="G148" s="6"/>
-      <c r="H148" s="5"/>
+      <c r="H148" s="5" t="s">
+        <v>315</v>
+      </c>
       <c r="I148" s="6"/>
       <c r="J148" s="5"/>
     </row>
-    <row r="149" spans="2:10">
+    <row r="149" spans="2:10" ht="22.5">
       <c r="B149" s="5">
-        <v>146</v>
-      </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="6"/>
-      <c r="E149" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D149" s="6">
+        <v>39122</v>
+      </c>
+      <c r="E149" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F149" s="5"/>
       <c r="G149" s="6"/>
       <c r="H149" s="5"/>
-      <c r="I149" s="5"/>
+      <c r="I149" s="6"/>
       <c r="J149" s="5"/>
     </row>
-    <row r="150" spans="2:10">
+    <row r="150" spans="2:10" ht="22.5">
       <c r="B150" s="5">
-        <v>147</v>
-      </c>
-      <c r="C150" s="5"/>
-      <c r="D150" s="6"/>
-      <c r="E150" s="5"/>
-      <c r="F150" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D150" s="6">
+        <v>39122</v>
+      </c>
+      <c r="E150" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>273</v>
+      </c>
       <c r="G150" s="6"/>
       <c r="H150" s="5"/>
-      <c r="I150" s="5"/>
+      <c r="I150" s="6"/>
       <c r="J150" s="5"/>
     </row>
     <row r="151" spans="2:10">
@@ -6075,11 +6109,11 @@
       <c r="J259" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J162">
-    <filterColumn colId="6">
+  <autoFilter ref="B3:J162">
+    <filterColumn colId="5">
       <filters blank="1"/>
     </filterColumn>
-    <filterColumn colId="8">
+    <filterColumn colId="7">
       <filters blank="1"/>
     </filterColumn>
     <sortState ref="B4:J162">

</xml_diff>

<commit_message>
Issue no. 55 @1340710520
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Template" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$B$3:$J$162</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$B$3:$J$161</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>Quadratgrad</t>
-  </si>
-  <si>
-    <t>Field of view</t>
   </si>
   <si>
     <t>Notwendigkeit der peer-Methoden in companion-Interfaces prüfen. Entfernen falls betreffender Code emitPS() der betreffenden Klasse aufrufen kann.</t>
@@ -1041,8 +1038,10 @@
     <t>11.06.2012: Erste Umsetzung am 29.02.2008.</t>
   </si>
   <si>
-    <t>Circle-Attribut fov bezeichnet Circle-Gruppe, die Sichtfenster festlegt. Catalog-Attribut fov verweist auf Circle-Gruppe. Eine Circle-Gruppe definiert ein Outline eines fov. fov immer geschlossen (Polygon). Geschlossener fov ersetzt ggf. vorhandenen, offener schneidet ggf. vorhandenen falls genau 2 Schnittpunkte, !!!Konzept für Auswahl der resultierenden!!!
-Bei Catalog mehrere fov durch Komma getrennt: 1. ist Outline des fov, folgende sind Löcher im fov.</t>
+    <t>Konzept für FOV aus Circle-Kombinationen</t>
+  </si>
+  <si>
+    <t>LAB: Geometry erweitern? Falls möglich FOV retrieve, FOV change; anderenfalls FOV degister/ retrieve, FOV change, FOV register.</t>
   </si>
 </sst>
 </file>
@@ -1513,13 +1512,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="B1:J259"/>
+  <dimension ref="B1:J258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1591,7 +1590,7 @@
         <v>147</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D4" s="6">
         <v>41059</v>
@@ -1600,118 +1599,120 @@
         <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B5" s="5">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>311</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6">
-        <v>41057</v>
+        <v>39417</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+        <v>185</v>
+      </c>
+      <c r="G5" s="6">
+        <v>40607</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="33.75" hidden="1">
       <c r="B6" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="D6" s="6">
         <v>39417</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
-        <v>186</v>
+        <v>40</v>
       </c>
       <c r="G6" s="6">
-        <v>40607</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>212</v>
-      </c>
+        <v>39480</v>
+      </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="33.75" hidden="1">
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:10" ht="22.5" hidden="1">
       <c r="B7" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6">
         <v>39417</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F7" s="5" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G7" s="6">
         <v>39480</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="6"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="2:10" ht="22.5" hidden="1">
+    <row r="8" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B8" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D8" s="6">
         <v>39417</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="E8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="G8" s="6">
-        <v>39480</v>
+        <v>39463</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="9" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B9" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="6">
         <v>39417</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F9" s="5" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="G9" s="6">
         <v>39463</v>
@@ -1720,13 +1721,11 @@
       <c r="I9" s="6"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:10" ht="56.25" hidden="1" customHeight="1">
+    <row r="10" spans="2:10" hidden="1">
       <c r="B10" s="5">
-        <v>7</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C10" s="5"/>
       <c r="D10" s="6">
         <v>39417</v>
       </c>
@@ -1734,7 +1733,7 @@
         <v>59</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G10" s="6">
         <v>39463</v>
@@ -1743,30 +1742,28 @@
       <c r="I10" s="6"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:10" hidden="1">
+    <row r="11" spans="2:10" ht="67.5" hidden="1">
       <c r="B11" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6">
         <v>39417</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="E11" s="5"/>
       <c r="F11" s="5" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G11" s="6">
-        <v>39463</v>
+        <v>39462</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="6"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:10" ht="67.5" hidden="1">
+    <row r="12" spans="2:10" ht="78.75" hidden="1">
       <c r="B12" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="6">
@@ -1774,7 +1771,7 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G12" s="6">
         <v>39462</v>
@@ -1783,9 +1780,9 @@
       <c r="I12" s="6"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="2:10" ht="78.75" hidden="1">
+    <row r="13" spans="2:10" ht="33.75" hidden="1">
       <c r="B13" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="6">
@@ -1793,7 +1790,7 @@
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G13" s="6">
         <v>39462</v>
@@ -1804,7 +1801,7 @@
     </row>
     <row r="14" spans="2:10" ht="33.75" hidden="1">
       <c r="B14" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6">
@@ -1812,7 +1809,7 @@
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="G14" s="6">
         <v>39462</v>
@@ -1821,17 +1818,19 @@
       <c r="I14" s="6"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="2:10" ht="33.75" hidden="1">
+    <row r="15" spans="2:10" ht="45" hidden="1">
       <c r="B15" s="5">
-        <v>12</v>
-      </c>
-      <c r="C15" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D15" s="6">
         <v>39417</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="6">
         <v>39462</v>
@@ -1840,19 +1839,17 @@
       <c r="I15" s="6"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="2:10" ht="45" hidden="1">
+    <row r="16" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B16" s="5">
-        <v>13</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>29</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="6">
         <v>39417</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G16" s="6">
         <v>39462</v>
@@ -1861,17 +1858,19 @@
       <c r="I16" s="6"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="17" spans="2:10" ht="45" hidden="1">
       <c r="B17" s="5">
-        <v>14</v>
-      </c>
-      <c r="C17" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D17" s="6">
         <v>39417</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G17" s="6">
         <v>39462</v>
@@ -1880,33 +1879,37 @@
       <c r="I17" s="6"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10" ht="45" hidden="1">
+    <row r="18" spans="2:10" ht="56.25" hidden="1">
       <c r="B18" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D18" s="6">
         <v>39417</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F18" s="5" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G18" s="6">
-        <v>39462</v>
-      </c>
-      <c r="H18" s="5"/>
+        <v>39456</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="I18" s="6"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10" ht="56.25" hidden="1">
+    <row r="19" spans="2:10" hidden="1">
       <c r="B19" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D19" s="6">
         <v>39417</v>
@@ -1915,23 +1918,23 @@
         <v>59</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G19" s="6">
         <v>39456</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10" hidden="1">
+    <row r="20" spans="2:10" ht="22.5" hidden="1">
       <c r="B20" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D20" s="6">
         <v>39417</v>
@@ -1946,17 +1949,17 @@
         <v>39456</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10" ht="22.5" hidden="1">
+    <row r="21" spans="2:10" hidden="1">
       <c r="B21" s="5">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="D21" s="6">
         <v>39417</v>
@@ -1965,23 +1968,21 @@
         <v>59</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G21" s="6">
         <v>39456</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="H21" s="5"/>
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10" hidden="1">
+    <row r="22" spans="2:10" ht="22.5" hidden="1">
       <c r="B22" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D22" s="6">
         <v>39417</v>
@@ -1990,7 +1991,7 @@
         <v>59</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="G22" s="6">
         <v>39456</v>
@@ -2001,74 +2002,72 @@
     </row>
     <row r="23" spans="2:10" ht="22.5" hidden="1">
       <c r="B23" s="5">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="6">
         <v>39417</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>59</v>
-      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="G23" s="6">
-        <v>39456</v>
+        <v>39452</v>
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="6"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10" ht="22.5" hidden="1">
+    <row r="24" spans="2:10" ht="90" hidden="1">
       <c r="B24" s="5">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D24" s="6">
         <v>39417</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G24" s="6">
-        <v>39452</v>
+        <v>39448</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="2:10" ht="90" hidden="1">
+    <row r="25" spans="2:10" ht="33.75" hidden="1">
       <c r="B25" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D25" s="6">
         <v>39417</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>59</v>
+      </c>
       <c r="F25" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G25" s="6">
-        <v>39448</v>
+        <v>39445</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="6"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="2:10" ht="33.75" hidden="1">
+    <row r="26" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B26" s="5">
-        <v>23</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C26" s="5"/>
       <c r="D26" s="6">
         <v>39417</v>
       </c>
@@ -2076,10 +2075,10 @@
         <v>59</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G26" s="6">
-        <v>39445</v>
+        <v>39437</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="6"/>
@@ -2087,9 +2086,11 @@
     </row>
     <row r="27" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B27" s="5">
-        <v>24</v>
-      </c>
-      <c r="C27" s="5"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D27" s="6">
         <v>39417</v>
       </c>
@@ -2097,7 +2098,7 @@
         <v>59</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="G27" s="6">
         <v>39437</v>
@@ -2106,36 +2107,36 @@
       <c r="I27" s="6"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="28" spans="2:10" hidden="1">
       <c r="B28" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="D28" s="6">
-        <v>39417</v>
+        <v>39448</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G28" s="6">
-        <v>39437</v>
-      </c>
-      <c r="H28" s="5"/>
+        <v>39477</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>62</v>
+      </c>
       <c r="I28" s="6"/>
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="2:10" hidden="1">
       <c r="B29" s="5">
-        <v>26</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C29" s="5"/>
       <c r="D29" s="6">
         <v>39448</v>
       </c>
@@ -2143,20 +2144,18 @@
         <v>59</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G29" s="6">
         <v>39477</v>
       </c>
-      <c r="H29" s="5" t="s">
-        <v>62</v>
-      </c>
+      <c r="H29" s="5"/>
       <c r="I29" s="6"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="2:10" hidden="1">
+    <row r="30" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B30" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="6">
@@ -2166,45 +2165,45 @@
         <v>59</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="G30" s="6">
         <v>39477</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="I30" s="6"/>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B31" s="5">
-        <v>28</v>
-      </c>
-      <c r="C31" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D31" s="6">
         <v>39448</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G31" s="6">
-        <v>39477</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>64</v>
-      </c>
+        <v>39475</v>
+      </c>
+      <c r="H31" s="5"/>
       <c r="I31" s="6"/>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B32" s="5">
-        <v>29</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>53</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="6">
         <v>39448</v>
       </c>
@@ -2212,7 +2211,7 @@
         <v>60</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G32" s="6">
         <v>39475</v>
@@ -2223,20 +2222,20 @@
     </row>
     <row r="33" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B33" s="5">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="6">
         <v>39448</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G33" s="6">
-        <v>39475</v>
+        <v>39466</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="6"/>
@@ -2244,7 +2243,7 @@
     </row>
     <row r="34" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B34" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="6">
@@ -2254,20 +2253,22 @@
         <v>59</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G34" s="6">
-        <v>39466</v>
+        <v>39465</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="6"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="35" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B35" s="5">
-        <v>32</v>
-      </c>
-      <c r="C35" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="D35" s="6">
         <v>39448</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>59</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G35" s="6">
         <v>39465</v>
@@ -2284,13 +2285,11 @@
       <c r="I35" s="6"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="36" spans="2:10" hidden="1">
       <c r="B36" s="5">
-        <v>33</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C36" s="5"/>
       <c r="D36" s="6">
         <v>39448</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>59</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G36" s="6">
         <v>39465</v>
@@ -2307,22 +2306,24 @@
       <c r="I36" s="6"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="2:10" hidden="1">
+    <row r="37" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B37" s="5">
-        <v>34</v>
-      </c>
-      <c r="C37" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="D37" s="6">
-        <v>39448</v>
+        <v>39479</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="G37" s="6">
-        <v>39465</v>
+        <v>39518</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="6"/>
@@ -2330,19 +2331,19 @@
     </row>
     <row r="38" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B38" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D38" s="6">
         <v>39479</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G38" s="6">
         <v>39518</v>
@@ -2351,150 +2352,150 @@
       <c r="I38" s="6"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="39" spans="2:10">
       <c r="B39" s="5">
-        <v>36</v>
+        <v>146</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>75</v>
+        <v>310</v>
       </c>
       <c r="D39" s="6">
+        <v>41057</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+      <c r="B40" s="5">
+        <v>38</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="6">
         <v>39479</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E40" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G39" s="6">
-        <v>39518</v>
-      </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="B40" s="5">
-        <v>145</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="D40" s="6">
-        <v>41039</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="F40" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="G40" s="6"/>
+        <v>66</v>
+      </c>
+      <c r="G40" s="6">
+        <v>39503</v>
+      </c>
       <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
+      <c r="I40" s="6"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="41" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B41" s="5">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="D41" s="6">
         <v>39479</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G41" s="6">
         <v>39503</v>
       </c>
-      <c r="H41" s="5"/>
+      <c r="H41" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="I41" s="6"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B42" s="5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="D42" s="6">
-        <v>39479</v>
+        <v>39508</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="G42" s="6">
-        <v>39503</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>73</v>
-      </c>
+        <v>39532</v>
+      </c>
+      <c r="H42" s="5"/>
       <c r="I42" s="6"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="43" spans="2:10" ht="22.5" hidden="1">
       <c r="B43" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D43" s="6">
         <v>39508</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G43" s="6">
-        <v>39532</v>
+        <v>39528</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="2:10" ht="22.5" hidden="1">
+    <row r="44" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B44" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D44" s="6">
         <v>39508</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G44" s="6">
-        <v>39528</v>
+        <v>39520</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="45" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B45" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D45" s="6">
         <v>39508</v>
@@ -2505,94 +2506,96 @@
       <c r="F45" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="G45" s="6">
-        <v>39520</v>
-      </c>
+      <c r="G45" s="6"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="5"/>
+      <c r="I45" s="6">
+        <v>39528</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="46" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B46" s="5">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="D46" s="6">
         <v>39508</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>81</v>
+        <v>59</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="5"/>
       <c r="I46" s="6">
-        <v>39528</v>
+        <v>39538</v>
       </c>
       <c r="J46" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B47" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D47" s="6">
-        <v>39508</v>
+        <v>39569</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F47" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G47" s="6">
+        <v>40578</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I47" s="6"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+      <c r="B48" s="5">
+        <v>46</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="6">
-        <v>39538</v>
-      </c>
-      <c r="J47" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="48" spans="2:10" ht="56.25" hidden="1" customHeight="1">
-      <c r="B48" s="5">
-        <v>45</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="D48" s="6">
         <v>39569</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>199</v>
+        <v>102</v>
       </c>
       <c r="G48" s="6">
-        <v>40578</v>
+        <v>39591</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>200</v>
+        <v>117</v>
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="5"/>
     </row>
     <row r="49" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B49" s="5">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D49" s="6">
         <v>39569</v>
@@ -2600,24 +2603,22 @@
       <c r="E49" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>103</v>
+      <c r="F49" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="G49" s="6">
-        <v>39591</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>118</v>
-      </c>
+        <v>39586</v>
+      </c>
+      <c r="H49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="50" spans="2:10" ht="168.75" hidden="1" customHeight="1">
       <c r="B50" s="5">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D50" s="6">
         <v>39569</v>
@@ -2625,45 +2626,47 @@
       <c r="E50" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="9" t="s">
-        <v>111</v>
+      <c r="F50" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="G50" s="6">
         <v>39586</v>
       </c>
-      <c r="H50" s="6"/>
+      <c r="H50" s="5"/>
       <c r="I50" s="6"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="2:10" ht="168.75" hidden="1" customHeight="1">
+    <row r="51" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B51" s="5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D51" s="6">
         <v>39569</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G51" s="6">
         <v>39586</v>
       </c>
-      <c r="H51" s="5"/>
+      <c r="H51" s="5" t="s">
+        <v>115</v>
+      </c>
       <c r="I51" s="6"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="2:10" ht="56.25" hidden="1" customHeight="1">
+    <row r="52" spans="2:10" ht="112.5" hidden="1" customHeight="1">
       <c r="B52" s="5">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D52" s="6">
         <v>39569</v>
@@ -2672,46 +2675,46 @@
         <v>60</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G52" s="6">
-        <v>39586</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>116</v>
-      </c>
+        <v>39575</v>
+      </c>
+      <c r="H52" s="5"/>
       <c r="I52" s="6"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="2:10" ht="112.5" hidden="1" customHeight="1">
+    <row r="53" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B53" s="5">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D53" s="6">
         <v>39569</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="G53" s="6">
-        <v>39575</v>
-      </c>
-      <c r="H53" s="5"/>
+        <v>39574</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="I53" s="6"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="54" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B54" s="5">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D54" s="6">
         <v>39569</v>
@@ -2720,23 +2723,23 @@
         <v>59</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="G54" s="6">
         <v>39574</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="2:10" ht="56.25" hidden="1" customHeight="1">
+    <row r="55" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B55" s="5">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="D55" s="6">
         <v>39569</v>
@@ -2745,23 +2748,23 @@
         <v>59</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G55" s="6">
-        <v>39574</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I55" s="6"/>
-      <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+        <v>94</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="6">
+        <v>39591</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B56" s="5">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D56" s="6">
         <v>39569</v>
@@ -2770,7 +2773,7 @@
         <v>59</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G56" s="6"/>
       <c r="H56" s="5"/>
@@ -2781,9 +2784,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="57" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="57" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B57" s="5">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>100</v>
@@ -2792,76 +2795,76 @@
         <v>39569</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G57" s="6"/>
       <c r="H57" s="5"/>
       <c r="I57" s="6">
-        <v>39591</v>
+        <v>39583</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="58" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B58" s="5">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="D58" s="6">
         <v>39569</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="5"/>
       <c r="I58" s="6">
-        <v>39583</v>
+        <v>39586</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59" spans="2:10" ht="45" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="45" hidden="1">
       <c r="B59" s="5">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D59" s="6">
-        <v>39569</v>
+        <v>39630</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G59" s="6"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="6">
-        <v>39586</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="2:10" ht="45" hidden="1">
+        <v>128</v>
+      </c>
+      <c r="G59" s="6">
+        <v>39660</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I59" s="6"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="2:10" ht="281.25" hidden="1" customHeight="1">
       <c r="B60" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D60" s="6">
         <v>39630</v>
@@ -2870,23 +2873,21 @@
         <v>59</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="G60" s="6">
-        <v>39660</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>130</v>
-      </c>
+        <v>39647</v>
+      </c>
+      <c r="H60" s="5"/>
       <c r="I60" s="6"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="2:10" ht="281.25" hidden="1" customHeight="1">
+    <row r="61" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B61" s="5">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D61" s="6">
         <v>39630</v>
@@ -2895,7 +2896,7 @@
         <v>59</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="G61" s="6">
         <v>39647</v>
@@ -2904,12 +2905,12 @@
       <c r="I61" s="6"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="62" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B62" s="5">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D62" s="6">
         <v>39630</v>
@@ -2918,58 +2919,60 @@
         <v>59</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G62" s="6">
+        <v>123</v>
+      </c>
+      <c r="G62" s="6"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="6">
         <v>39647</v>
       </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+      <c r="J62" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B63" s="5">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D63" s="6">
-        <v>39630</v>
+        <v>39661</v>
       </c>
       <c r="E63" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G63" s="6"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="6">
-        <v>39647</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="64" spans="2:10" ht="56.25" hidden="1" customHeight="1">
+        <v>133</v>
+      </c>
+      <c r="G63" s="6">
+        <v>39693</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="I63" s="6"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="2:10" ht="33.75" hidden="1">
       <c r="B64" s="5">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D64" s="6">
-        <v>39661</v>
+        <v>39692</v>
       </c>
       <c r="E64" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G64" s="6">
-        <v>39693</v>
+        <v>39695</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>135</v>
@@ -2977,34 +2980,34 @@
       <c r="I64" s="6"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="2:10" ht="33.75" hidden="1">
+    <row r="65" spans="2:10" ht="90" hidden="1">
       <c r="B65" s="5">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D65" s="6">
-        <v>39692</v>
+        <v>39814</v>
       </c>
       <c r="E65" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="G65" s="6">
-        <v>39695</v>
+        <v>39820</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="2:10" ht="90" hidden="1">
+    <row r="66" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B66" s="5">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>139</v>
@@ -3016,66 +3019,62 @@
         <v>59</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="G66" s="6">
-        <v>39820</v>
-      </c>
-      <c r="H66" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="I66" s="6"/>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+      <c r="G66" s="6"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="6">
+        <v>39832</v>
+      </c>
+      <c r="J66" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B67" s="5">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D67" s="6">
-        <v>39814</v>
+        <v>39873</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F67" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="G67" s="6"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="6">
+        <v>39899</v>
+      </c>
       <c r="H67" s="5"/>
-      <c r="I67" s="6">
-        <v>39832</v>
-      </c>
-      <c r="J67" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+      <c r="I67" s="6"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B68" s="5">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>146</v>
       </c>
       <c r="D68" s="6">
-        <v>39873</v>
+        <v>39904</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F68" s="5"/>
       <c r="G68" s="6">
-        <v>39899</v>
+        <v>40587</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="6"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+    <row r="69" spans="2:10" hidden="1">
       <c r="B69" s="5">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>147</v>
@@ -3084,7 +3083,7 @@
         <v>39904</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F69" s="5"/>
       <c r="G69" s="6">
@@ -3094,9 +3093,9 @@
       <c r="I69" s="6"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="2:10" hidden="1">
+    <row r="70" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B70" s="5">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>148</v>
@@ -3109,18 +3108,20 @@
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="6">
-        <v>40587</v>
-      </c>
-      <c r="H70" s="5"/>
+        <v>40497</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="I70" s="6"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="71" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B71" s="5">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D71" s="6">
         <v>39904</v>
@@ -3130,20 +3131,20 @@
       </c>
       <c r="F71" s="5"/>
       <c r="G71" s="6">
-        <v>40497</v>
+        <v>40253</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="I71" s="6"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="72" spans="2:10" ht="90" hidden="1" customHeight="1">
       <c r="B72" s="5">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>145</v>
+        <v>88</v>
       </c>
       <c r="D72" s="6">
         <v>39904</v>
@@ -3151,70 +3152,68 @@
       <c r="E72" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F72" s="5"/>
+      <c r="F72" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="G72" s="6">
-        <v>40253</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>178</v>
-      </c>
+        <v>40248</v>
+      </c>
+      <c r="H72" s="5"/>
       <c r="I72" s="6"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="2:10" ht="90" hidden="1" customHeight="1">
+    <row r="73" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B73" s="5">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D73" s="6">
         <v>39904</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="G73" s="6">
-        <v>40248</v>
-      </c>
-      <c r="H73" s="5"/>
+        <v>40179</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>158</v>
+      </c>
       <c r="I73" s="6"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+    <row r="74" spans="2:10" ht="33.75" customHeight="1">
       <c r="B74" s="5">
-        <v>71</v>
+        <v>145</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>150</v>
+        <v>309</v>
       </c>
       <c r="D74" s="6">
-        <v>39904</v>
+        <v>41039</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="G74" s="6">
-        <v>40179</v>
-      </c>
-      <c r="H74" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="I74" s="6"/>
+        <v>308</v>
+      </c>
+      <c r="G74" s="6"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="2:10" ht="33.75" customHeight="1">
+    <row r="75" spans="2:10" ht="101.25" customHeight="1">
       <c r="B75" s="5">
         <v>144</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D75" s="6">
         <v>41030</v>
@@ -3223,19 +3222,19 @@
         <v>59</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="5"/>
       <c r="I75" s="6"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="2:10" ht="101.25" customHeight="1">
+    <row r="76" spans="2:10" ht="12.75" customHeight="1">
       <c r="B76" s="5">
         <v>143</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D76" s="6">
         <v>41028</v>
@@ -3244,40 +3243,42 @@
         <v>60</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="5"/>
       <c r="I76" s="6"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="2:10" ht="12.75" customHeight="1">
+    <row r="77" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B77" s="5">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>299</v>
+        <v>152</v>
       </c>
       <c r="D77" s="6">
-        <v>41012</v>
+        <v>40098</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="G77" s="6"/>
+        <v>153</v>
+      </c>
+      <c r="G77" s="6">
+        <v>40497</v>
+      </c>
       <c r="H77" s="5"/>
       <c r="I77" s="6"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="2:10" ht="56.25" hidden="1" customHeight="1">
+    <row r="78" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B78" s="5">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D78" s="6">
         <v>40098</v>
@@ -3286,92 +3287,92 @@
         <v>59</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="G78" s="6">
-        <v>40497</v>
-      </c>
-      <c r="H78" s="5"/>
+        <v>40456</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="I78" s="6"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="79" spans="2:10" ht="27" hidden="1" customHeight="1">
       <c r="B79" s="5">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>151</v>
+        <v>298</v>
       </c>
       <c r="D79" s="6">
-        <v>40098</v>
+        <v>41012</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>188</v>
+        <v>299</v>
       </c>
       <c r="G79" s="6">
-        <v>40456</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>189</v>
-      </c>
+        <v>41077</v>
+      </c>
+      <c r="H79" s="5"/>
       <c r="I79" s="6"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="2:10" ht="27" customHeight="1">
+    <row r="80" spans="2:10" ht="36" hidden="1" customHeight="1">
       <c r="B80" s="5">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>301</v>
+        <v>154</v>
       </c>
       <c r="D80" s="6">
-        <v>41012</v>
+        <v>40196</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="G80" s="6"/>
-      <c r="H80" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="G80" s="6">
+        <v>40206</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="I80" s="6"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="2:10" ht="36" hidden="1" customHeight="1">
+    <row r="81" spans="2:10" ht="157.5" hidden="1" customHeight="1">
       <c r="B81" s="5">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D81" s="6">
-        <v>40196</v>
+        <v>40197</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F81" s="5" t="s">
-        <v>156</v>
-      </c>
+      <c r="F81" s="5"/>
       <c r="G81" s="6">
-        <v>40206</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>163</v>
-      </c>
+        <v>40210</v>
+      </c>
+      <c r="H81" s="5"/>
       <c r="I81" s="6"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="2:10" ht="157.5" hidden="1" customHeight="1">
+    <row r="82" spans="2:10" ht="112.5" hidden="1" customHeight="1">
       <c r="B82" s="5">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D82" s="6">
         <v>40197</v>
@@ -3381,84 +3382,86 @@
       </c>
       <c r="F82" s="5"/>
       <c r="G82" s="6">
-        <v>40210</v>
+        <v>40198</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="6"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="2:10" ht="112.5" hidden="1" customHeight="1">
+    <row r="83" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B83" s="5">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D83" s="6">
-        <v>40197</v>
+        <v>40199</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F83" s="5"/>
-      <c r="G83" s="6">
-        <v>40198</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G83" s="6"/>
       <c r="H83" s="5"/>
-      <c r="I83" s="6"/>
-      <c r="J83" s="5"/>
-    </row>
-    <row r="84" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+      <c r="I83" s="6">
+        <v>40253</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B84" s="5">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D84" s="6">
-        <v>40199</v>
+        <v>40213</v>
       </c>
       <c r="E84" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="G84" s="6"/>
+        <v>164</v>
+      </c>
+      <c r="G84" s="6">
+        <v>40248</v>
+      </c>
       <c r="H84" s="5"/>
-      <c r="I84" s="6">
-        <v>40253</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="85" spans="2:10" ht="12.75" hidden="1" customHeight="1">
+      <c r="I84" s="6"/>
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B85" s="5">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D85" s="6">
-        <v>40213</v>
+        <v>40228</v>
       </c>
       <c r="E85" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F85" s="5" t="s">
-        <v>165</v>
-      </c>
+      <c r="F85" s="5"/>
       <c r="G85" s="6">
-        <v>40248</v>
-      </c>
-      <c r="H85" s="5"/>
+        <v>40429</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>186</v>
+      </c>
       <c r="I85" s="6"/>
       <c r="J85" s="5"/>
     </row>
     <row r="86" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B86" s="5">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>166</v>
@@ -3467,47 +3470,47 @@
         <v>40228</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F86" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>167</v>
+      </c>
       <c r="G86" s="6">
-        <v>40429</v>
-      </c>
-      <c r="H86" s="5" t="s">
-        <v>187</v>
-      </c>
+        <v>40238</v>
+      </c>
+      <c r="H86" s="5"/>
       <c r="I86" s="6"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="87" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B87" s="5">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D87" s="6">
-        <v>40228</v>
+        <v>40239</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="G87" s="6">
-        <v>40238</v>
+        <v>40587</v>
       </c>
       <c r="H87" s="5"/>
       <c r="I87" s="6"/>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="88" spans="2:10" ht="56.25" hidden="1" customHeight="1">
       <c r="B88" s="5">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D88" s="6">
         <v>40239</v>
@@ -3516,44 +3519,44 @@
         <v>59</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="G88" s="6">
-        <v>40587</v>
+        <v>40517</v>
       </c>
       <c r="H88" s="5"/>
       <c r="I88" s="6"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="2:10" ht="56.25" hidden="1" customHeight="1">
+    <row r="89" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B89" s="5">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D89" s="6">
-        <v>40239</v>
+        <v>40247</v>
       </c>
       <c r="E89" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="G89" s="6">
-        <v>40517</v>
+        <v>40248</v>
       </c>
       <c r="H89" s="5"/>
       <c r="I89" s="6"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="90" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B90" s="5">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D90" s="6">
         <v>40247</v>
@@ -3562,7 +3565,7 @@
         <v>59</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G90" s="6">
         <v>40248</v>
@@ -3573,55 +3576,57 @@
     </row>
     <row r="91" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B91" s="5">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D91" s="6">
-        <v>40247</v>
+        <v>40248</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G91" s="6">
-        <v>40248</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="G91" s="6"/>
       <c r="H91" s="5"/>
-      <c r="I91" s="6"/>
-      <c r="J91" s="5"/>
-    </row>
-    <row r="92" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+      <c r="I91" s="6">
+        <v>40578</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B92" s="5">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D92" s="6">
-        <v>40248</v>
+        <v>40253</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="G92" s="6"/>
-      <c r="H92" s="5"/>
-      <c r="I92" s="6">
-        <v>40578</v>
-      </c>
-      <c r="J92" s="5" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="93" spans="2:10" ht="12.75" hidden="1" customHeight="1">
+        <v>182</v>
+      </c>
+      <c r="G92" s="6">
+        <v>40255</v>
+      </c>
+      <c r="H92" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I92" s="6"/>
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B93" s="5">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>179</v>
@@ -3630,118 +3635,114 @@
         <v>40253</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G93" s="6">
-        <v>40255</v>
+        <v>40254</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="5"/>
     </row>
     <row r="94" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B94" s="5">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="D94" s="6">
-        <v>40253</v>
+        <v>40461</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="G94" s="6">
-        <v>40254</v>
-      </c>
-      <c r="H94" s="5" t="s">
-        <v>182</v>
-      </c>
+        <v>40523</v>
+      </c>
+      <c r="H94" s="5"/>
       <c r="I94" s="6"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="95" spans="2:10" ht="22.5" customHeight="1">
       <c r="B95" s="5">
-        <v>92</v>
+        <v>142</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>193</v>
+        <v>300</v>
       </c>
       <c r="D95" s="6">
-        <v>40461</v>
+        <v>41012</v>
       </c>
       <c r="E95" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="G95" s="6">
-        <v>40523</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="G95" s="6"/>
       <c r="H95" s="5"/>
       <c r="I95" s="6"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="2:10" ht="22.5" customHeight="1">
+    <row r="96" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B96" s="5">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>296</v>
+        <v>193</v>
       </c>
       <c r="D96" s="6">
-        <v>41011</v>
+        <v>40517</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="G96" s="6"/>
+        <v>197</v>
+      </c>
+      <c r="G96" s="6">
+        <v>40526</v>
+      </c>
       <c r="H96" s="5"/>
       <c r="I96" s="6"/>
       <c r="J96" s="5"/>
     </row>
-    <row r="97" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="97" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B97" s="5">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="D97" s="6">
-        <v>40517</v>
+        <v>40519</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F97" s="5" t="s">
-        <v>198</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F97" s="5"/>
       <c r="G97" s="6">
-        <v>40526</v>
+        <v>40742</v>
       </c>
       <c r="H97" s="5"/>
       <c r="I97" s="6"/>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="98" spans="2:10" ht="78.75" hidden="1" customHeight="1">
       <c r="B98" s="5">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D98" s="6">
         <v>40519</v>
@@ -3749,128 +3750,128 @@
       <c r="E98" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F98" s="5"/>
+      <c r="F98" s="5" t="s">
+        <v>196</v>
+      </c>
       <c r="G98" s="6">
-        <v>40742</v>
+        <v>40607</v>
       </c>
       <c r="H98" s="5"/>
       <c r="I98" s="6"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="2:10" ht="78.75" hidden="1" customHeight="1">
+    <row r="99" spans="2:10" ht="67.5" hidden="1" customHeight="1">
       <c r="B99" s="5">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>196</v>
+        <v>288</v>
       </c>
       <c r="D99" s="6">
-        <v>40519</v>
+        <v>40998</v>
       </c>
       <c r="E99" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F99" s="5" t="s">
-        <v>197</v>
-      </c>
+      <c r="F99" s="5"/>
       <c r="G99" s="6">
-        <v>40607</v>
+        <v>41046</v>
       </c>
       <c r="H99" s="5"/>
       <c r="I99" s="6"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="2:10" ht="67.5" hidden="1" customHeight="1">
+    <row r="100" spans="2:10" ht="45" hidden="1" customHeight="1">
       <c r="B100" s="5">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>289</v>
+        <v>204</v>
       </c>
       <c r="D100" s="6">
-        <v>40998</v>
+        <v>40588</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F100" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>205</v>
+      </c>
       <c r="G100" s="6">
-        <v>41046</v>
+        <v>40599</v>
       </c>
       <c r="H100" s="5"/>
       <c r="I100" s="6"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="2:10" ht="45" hidden="1" customHeight="1">
+    <row r="101" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B101" s="5">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="D101" s="6">
-        <v>40588</v>
+        <v>40589</v>
       </c>
       <c r="E101" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="G101" s="6">
-        <v>40599</v>
+        <v>40600</v>
       </c>
       <c r="H101" s="5"/>
       <c r="I101" s="6"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="102" spans="2:10" ht="22.5">
       <c r="B102" s="5">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>210</v>
+        <v>295</v>
       </c>
       <c r="D102" s="6">
-        <v>40589</v>
+        <v>41011</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="G102" s="6">
-        <v>40600</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="G102" s="6"/>
       <c r="H102" s="5"/>
       <c r="I102" s="6"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="2:10" ht="12.75" customHeight="1">
+    <row r="103" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B103" s="5">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>297</v>
+        <v>212</v>
       </c>
       <c r="D103" s="6">
-        <v>41011</v>
+        <v>40625</v>
       </c>
       <c r="E103" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F103" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="G103" s="6"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="6">
+        <v>40786</v>
+      </c>
       <c r="H103" s="5"/>
       <c r="I103" s="6"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="2:10" ht="12.75" hidden="1" customHeight="1">
+    <row r="104" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B104" s="5">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C104" s="5" t="s">
         <v>213</v>
@@ -3881,17 +3882,21 @@
       <c r="E104" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F104" s="5"/>
-      <c r="G104" s="6">
-        <v>40786</v>
-      </c>
+      <c r="F104" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G104" s="6"/>
       <c r="H104" s="5"/>
-      <c r="I104" s="6"/>
-      <c r="J104" s="5"/>
-    </row>
-    <row r="105" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+      <c r="I104" s="6">
+        <v>40704</v>
+      </c>
+      <c r="J104" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B105" s="5">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>214</v>
@@ -3903,7 +3908,7 @@
         <v>59</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="5"/>
@@ -3911,12 +3916,12 @@
         <v>40704</v>
       </c>
       <c r="J105" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="106" spans="2:10" ht="12.75" hidden="1" customHeight="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="106" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B106" s="5">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>215</v>
@@ -3927,24 +3932,22 @@
       <c r="E106" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F106" s="5" t="s">
-        <v>217</v>
-      </c>
+      <c r="F106" s="5"/>
       <c r="G106" s="6"/>
       <c r="H106" s="5"/>
       <c r="I106" s="6">
         <v>40704</v>
       </c>
       <c r="J106" s="5" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" ht="22.5" hidden="1">
       <c r="B107" s="5">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D107" s="6">
         <v>40625</v>
@@ -3952,22 +3955,24 @@
       <c r="E107" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F107" s="5"/>
+      <c r="F107" s="5" t="s">
+        <v>218</v>
+      </c>
       <c r="G107" s="6"/>
       <c r="H107" s="5"/>
       <c r="I107" s="6">
         <v>40704</v>
       </c>
       <c r="J107" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" ht="22.5" hidden="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="108" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B108" s="5">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>218</v>
+        <v>237</v>
       </c>
       <c r="D108" s="6">
         <v>40625</v>
@@ -3976,46 +3981,42 @@
         <v>59</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="G108" s="6"/>
+        <v>240</v>
+      </c>
+      <c r="G108" s="6">
+        <v>40872</v>
+      </c>
       <c r="H108" s="5"/>
-      <c r="I108" s="6">
-        <v>40704</v>
-      </c>
-      <c r="J108" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="109" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+      <c r="I108" s="6"/>
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="2:10" ht="12.75" customHeight="1">
       <c r="B109" s="5">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>238</v>
+        <v>296</v>
       </c>
       <c r="D109" s="6">
-        <v>40625</v>
+        <v>41011</v>
       </c>
       <c r="E109" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="G109" s="6">
-        <v>40872</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="G109" s="6"/>
       <c r="H109" s="5"/>
       <c r="I109" s="6"/>
       <c r="J109" s="5"/>
     </row>
-    <row r="110" spans="2:10" ht="12.75" customHeight="1">
+    <row r="110" spans="2:10" ht="22.5">
       <c r="B110" s="5">
         <v>137</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D110" s="6">
         <v>40998</v>
@@ -4024,35 +4025,37 @@
         <v>59</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G110" s="6"/>
       <c r="H110" s="5"/>
       <c r="I110" s="6"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="2:10">
+    <row r="111" spans="2:10" ht="22.5" hidden="1">
       <c r="B111" s="5">
-        <v>138</v>
+        <v>109</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>293</v>
+        <v>226</v>
       </c>
       <c r="D111" s="6">
-        <v>40998</v>
+        <v>40758</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F111" s="5"/>
-      <c r="G111" s="6"/>
+      <c r="G111" s="6">
+        <v>40763</v>
+      </c>
       <c r="H111" s="5"/>
       <c r="I111" s="6"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="2:10" ht="22.5" hidden="1">
+    <row r="112" spans="2:10" ht="33.75" hidden="1">
       <c r="B112" s="5">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>227</v>
@@ -4061,38 +4064,36 @@
         <v>40758</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F112" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F112" s="5" t="s">
+        <v>228</v>
+      </c>
       <c r="G112" s="6">
-        <v>40763</v>
-      </c>
-      <c r="H112" s="5"/>
+        <v>40790</v>
+      </c>
+      <c r="H112" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="I112" s="6"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10" ht="33.75" hidden="1">
+    <row r="113" spans="2:10">
       <c r="B113" s="5">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>228</v>
+        <v>292</v>
       </c>
       <c r="D113" s="6">
-        <v>40758</v>
+        <v>40998</v>
       </c>
       <c r="E113" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F113" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="G113" s="6">
-        <v>40790</v>
-      </c>
-      <c r="H113" s="5" t="s">
-        <v>234</v>
-      </c>
+      <c r="F113" s="5"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="5"/>
       <c r="I113" s="6"/>
       <c r="J113" s="5"/>
     </row>
@@ -4101,7 +4102,7 @@
         <v>135</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D114" s="6">
         <v>40983</v>
@@ -4110,65 +4111,65 @@
         <v>59</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G114" s="6"/>
       <c r="H114" s="5"/>
       <c r="I114" s="6"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="2:10">
+    <row r="115" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B115" s="5">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>281</v>
+        <v>234</v>
       </c>
       <c r="D115" s="6">
-        <v>40972</v>
+        <v>40794</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="G115" s="6"/>
-      <c r="H115" s="5"/>
+        <v>236</v>
+      </c>
+      <c r="G115" s="6">
+        <v>40987</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>286</v>
+      </c>
       <c r="I115" s="6"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="2:10" ht="33.75" hidden="1" customHeight="1">
+    <row r="116" spans="2:10" ht="33.75" customHeight="1">
       <c r="B116" s="5">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>235</v>
+        <v>280</v>
       </c>
       <c r="D116" s="6">
-        <v>40794</v>
+        <v>40972</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="G116" s="6">
-        <v>40987</v>
-      </c>
-      <c r="H116" s="5" t="s">
-        <v>287</v>
-      </c>
+        <v>281</v>
+      </c>
+      <c r="G116" s="6"/>
+      <c r="H116" s="5"/>
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10" ht="33.75" customHeight="1">
+    <row r="117" spans="2:10" ht="22.5">
       <c r="B117" s="5">
         <v>127</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D117" s="6">
         <v>40959</v>
@@ -4177,7 +4178,7 @@
         <v>59</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G117" s="6"/>
       <c r="H117" s="5"/>
@@ -4189,7 +4190,7 @@
         <v>128</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D118" s="6">
         <v>40959</v>
@@ -4203,12 +4204,12 @@
       <c r="I118" s="6"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="2:10">
+    <row r="119" spans="2:10" ht="33.75" customHeight="1">
       <c r="B119" s="5">
         <v>129</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D119" s="6">
         <v>40959</v>
@@ -4217,19 +4218,19 @@
         <v>59</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G119" s="6"/>
       <c r="H119" s="5"/>
       <c r="I119" s="6"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="2:10" ht="33.75" customHeight="1">
+    <row r="120" spans="2:10">
       <c r="B120" s="5">
         <v>125</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D120" s="6">
         <v>40956</v>
@@ -4243,56 +4244,56 @@
       <c r="I120" s="6"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="2:10" ht="45">
+    <row r="121" spans="2:10" ht="22.5" hidden="1" customHeight="1">
       <c r="B121" s="5">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D121" s="6">
-        <v>40956</v>
+        <v>40866</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F121" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="G121" s="6"/>
-      <c r="H121" s="5"/>
+        <v>60</v>
+      </c>
+      <c r="F121" s="5"/>
+      <c r="G121" s="6">
+        <v>40965</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>277</v>
+      </c>
       <c r="I121" s="6"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="2:10" ht="22.5" hidden="1" customHeight="1">
+    <row r="122" spans="2:10" ht="45">
       <c r="B122" s="5">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D122" s="6">
-        <v>40866</v>
+        <v>40956</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F122" s="5"/>
-      <c r="G122" s="6">
-        <v>40965</v>
-      </c>
-      <c r="H122" s="5" t="s">
-        <v>278</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F122" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="G122" s="6"/>
+      <c r="H122" s="5"/>
       <c r="I122" s="6"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10" ht="67.5" customHeight="1">
+    <row r="123" spans="2:10">
       <c r="B123" s="5">
         <v>123</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D123" s="6">
         <v>40947</v>
@@ -4303,7 +4304,7 @@
       <c r="F123" s="5"/>
       <c r="G123" s="6"/>
       <c r="H123" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I123" s="6"/>
       <c r="J123" s="5"/>
@@ -4313,7 +4314,7 @@
         <v>124</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D124" s="6">
         <v>40947</v>
@@ -4322,19 +4323,19 @@
         <v>59</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="5"/>
       <c r="I124" s="6"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="2:10" ht="12.75" customHeight="1">
+    <row r="125" spans="2:10" ht="33.75">
       <c r="B125" s="5">
         <v>122</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D125" s="6">
         <v>40941</v>
@@ -4343,19 +4344,19 @@
         <v>59</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G125" s="6"/>
       <c r="H125" s="5"/>
       <c r="I125" s="6"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="2:10" ht="22.5" customHeight="1">
+    <row r="126" spans="2:10" ht="22.5">
       <c r="B126" s="5">
         <v>121</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D126" s="6">
         <v>40869</v>
@@ -4364,7 +4365,7 @@
         <v>59</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="5"/>
@@ -4376,7 +4377,7 @@
         <v>120</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D127" s="6">
         <v>40866</v>
@@ -4385,19 +4386,19 @@
         <v>59</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G127" s="6"/>
       <c r="H127" s="5"/>
       <c r="I127" s="6"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="2:10" ht="12.75" customHeight="1">
+    <row r="128" spans="2:10" ht="33.75">
       <c r="B128" s="5">
         <v>117</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D128" s="6">
         <v>40829</v>
@@ -4406,19 +4407,19 @@
         <v>59</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="5"/>
       <c r="I128" s="6"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="2:10" ht="22.5" customHeight="1">
+    <row r="129" spans="2:10" ht="45">
       <c r="B129" s="5">
         <v>118</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D129" s="6">
         <v>40829</v>
@@ -4427,19 +4428,19 @@
         <v>59</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="5"/>
       <c r="I129" s="6"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="2:10" ht="12.75" customHeight="1">
+    <row r="130" spans="2:10" ht="22.5" customHeight="1">
       <c r="B130" s="5">
         <v>116</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D130" s="6">
         <v>40822</v>
@@ -4448,19 +4449,19 @@
         <v>59</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G130" s="6"/>
       <c r="H130" s="5"/>
       <c r="I130" s="6"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="2:10" ht="22.5" customHeight="1">
+    <row r="131" spans="2:10" ht="22.5">
       <c r="B131" s="5">
         <v>115</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D131" s="6">
         <v>40816</v>
@@ -4469,64 +4470,68 @@
         <v>60</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G131" s="6"/>
       <c r="H131" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I131" s="6"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="2:10" ht="22.5">
+    <row r="132" spans="2:10" ht="67.5" hidden="1">
       <c r="B132" s="5">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="C132" s="5" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="D132" s="6">
-        <v>40794</v>
+        <v>40959</v>
       </c>
       <c r="E132" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="G132" s="6"/>
       <c r="H132" s="5"/>
-      <c r="I132" s="6"/>
-      <c r="J132" s="5"/>
-    </row>
-    <row r="133" spans="2:10" ht="67.5" hidden="1">
+      <c r="I132" s="6">
+        <v>40960</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="133" spans="2:10" ht="33.75" hidden="1">
       <c r="B133" s="5">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D133" s="6">
         <v>40959</v>
       </c>
       <c r="E133" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="G133" s="6"/>
-      <c r="H133" s="5"/>
-      <c r="I133" s="6">
+        <v>275</v>
+      </c>
+      <c r="G133" s="6">
         <v>40960</v>
       </c>
-      <c r="J133" s="5" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="134" spans="2:10" ht="33.75" hidden="1">
+      <c r="H133" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="I133" s="6"/>
+      <c r="J133" s="5"/>
+    </row>
+    <row r="134" spans="2:10" ht="56.25" hidden="1">
       <c r="B134" s="5">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>266</v>
@@ -4535,97 +4540,93 @@
         <v>40959</v>
       </c>
       <c r="E134" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G134" s="6">
-        <v>40960</v>
+        <v>40972</v>
       </c>
       <c r="H134" s="5" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I134" s="6"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="2:10" ht="56.25" hidden="1">
+    <row r="135" spans="2:10" ht="22.5">
       <c r="B135" s="5">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
       <c r="D135" s="6">
-        <v>40959</v>
+        <v>40794</v>
       </c>
       <c r="E135" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="G135" s="6">
-        <v>40972</v>
-      </c>
-      <c r="H135" s="5" t="s">
-        <v>280</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="G135" s="6"/>
+      <c r="H135" s="5"/>
       <c r="I135" s="6"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="2:10" ht="22.5">
+    <row r="136" spans="2:10" hidden="1">
       <c r="B136" s="5">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="C136" s="5" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
       <c r="D136" s="6">
-        <v>40763</v>
+        <v>40982</v>
       </c>
       <c r="E136" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="5"/>
-      <c r="I136" s="6"/>
-      <c r="J136" s="5"/>
-    </row>
-    <row r="137" spans="2:10" hidden="1">
+      <c r="I136" s="6">
+        <v>41011</v>
+      </c>
+      <c r="J136" s="5" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="137" spans="2:10" ht="22.5">
       <c r="B137" s="5">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>284</v>
+        <v>231</v>
       </c>
       <c r="D137" s="6">
-        <v>40982</v>
+        <v>40763</v>
       </c>
       <c r="E137" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>285</v>
+        <v>232</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="5"/>
-      <c r="I137" s="6">
-        <v>41011</v>
-      </c>
-      <c r="J137" s="5" t="s">
-        <v>294</v>
-      </c>
+      <c r="I137" s="6"/>
+      <c r="J137" s="5"/>
     </row>
     <row r="138" spans="2:10">
       <c r="B138" s="5">
         <v>111</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D138" s="6">
         <v>40762</v>
@@ -4634,7 +4635,7 @@
         <v>59</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="5"/>
@@ -4646,7 +4647,7 @@
         <v>108</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D139" s="6">
         <v>40750</v>
@@ -4655,7 +4656,7 @@
         <v>59</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G139" s="6"/>
       <c r="H139" s="5"/>
@@ -4667,7 +4668,7 @@
         <v>107</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D140" s="6">
         <v>40742</v>
@@ -4676,7 +4677,7 @@
         <v>59</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="5"/>
@@ -4688,7 +4689,7 @@
         <v>100</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D141" s="6">
         <v>40589</v>
@@ -4697,7 +4698,7 @@
         <v>59</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G141" s="6"/>
       <c r="H141" s="5"/>
@@ -4709,7 +4710,7 @@
         <v>97</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D142" s="6">
         <v>40566</v>
@@ -4718,7 +4719,7 @@
         <v>59</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G142" s="6"/>
       <c r="H142" s="5"/>
@@ -4730,7 +4731,7 @@
         <v>93</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D143" s="6">
         <v>40506</v>
@@ -4739,7 +4740,7 @@
         <v>59</v>
       </c>
       <c r="F143" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G143" s="6"/>
       <c r="H143" s="5"/>
@@ -4751,7 +4752,7 @@
         <v>77</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D144" s="6">
         <v>40188</v>
@@ -4770,7 +4771,7 @@
         <v>72</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D145" s="6">
         <v>39904</v>
@@ -4789,7 +4790,7 @@
         <v>73</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D146" s="6">
         <v>39904</v>
@@ -4808,7 +4809,7 @@
         <v>74</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D147" s="6">
         <v>39904</v>
@@ -4822,12 +4823,12 @@
       <c r="I147" s="6"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10" ht="112.5">
+    <row r="148" spans="2:10" ht="33.75">
       <c r="B148" s="5">
         <v>37</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>69</v>
+        <v>315</v>
       </c>
       <c r="D148" s="6">
         <v>39479</v>
@@ -4840,7 +4841,7 @@
       </c>
       <c r="G148" s="6"/>
       <c r="H148" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I148" s="6"/>
       <c r="J148" s="5"/>
@@ -4850,7 +4851,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D149" s="6">
         <v>39122</v>
@@ -4869,7 +4870,7 @@
         <v>2</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D150" s="6">
         <v>39122</v>
@@ -4878,7 +4879,7 @@
         <v>59</v>
       </c>
       <c r="F150" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G150" s="6"/>
       <c r="H150" s="5"/>
@@ -4887,7 +4888,7 @@
     </row>
     <row r="151" spans="2:10">
       <c r="B151" s="5">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C151" s="5"/>
       <c r="D151" s="6"/>
@@ -4900,7 +4901,7 @@
     </row>
     <row r="152" spans="2:10">
       <c r="B152" s="5">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C152" s="5"/>
       <c r="D152" s="6"/>
@@ -4913,7 +4914,7 @@
     </row>
     <row r="153" spans="2:10">
       <c r="B153" s="5">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C153" s="5"/>
       <c r="D153" s="6"/>
@@ -4926,7 +4927,7 @@
     </row>
     <row r="154" spans="2:10">
       <c r="B154" s="5">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C154" s="5"/>
       <c r="D154" s="6"/>
@@ -4939,7 +4940,7 @@
     </row>
     <row r="155" spans="2:10">
       <c r="B155" s="5">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C155" s="5"/>
       <c r="D155" s="6"/>
@@ -4952,7 +4953,7 @@
     </row>
     <row r="156" spans="2:10">
       <c r="B156" s="5">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="6"/>
@@ -4965,7 +4966,7 @@
     </row>
     <row r="157" spans="2:10">
       <c r="B157" s="5">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C157" s="5"/>
       <c r="D157" s="6"/>
@@ -4978,7 +4979,7 @@
     </row>
     <row r="158" spans="2:10">
       <c r="B158" s="5">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C158" s="5"/>
       <c r="D158" s="6"/>
@@ -4991,7 +4992,7 @@
     </row>
     <row r="159" spans="2:10">
       <c r="B159" s="5">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C159" s="5"/>
       <c r="D159" s="6"/>
@@ -5004,7 +5005,7 @@
     </row>
     <row r="160" spans="2:10">
       <c r="B160" s="5">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C160" s="5"/>
       <c r="D160" s="6"/>
@@ -5017,7 +5018,7 @@
     </row>
     <row r="161" spans="2:10">
       <c r="B161" s="5">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C161" s="5"/>
       <c r="D161" s="6"/>
@@ -5029,9 +5030,7 @@
       <c r="J161" s="5"/>
     </row>
     <row r="162" spans="2:10">
-      <c r="B162" s="5">
-        <v>159</v>
-      </c>
+      <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="6"/>
       <c r="E162" s="5"/>
@@ -6097,19 +6096,8 @@
       <c r="I258" s="5"/>
       <c r="J258" s="5"/>
     </row>
-    <row r="259" spans="2:10">
-      <c r="B259" s="5"/>
-      <c r="C259" s="5"/>
-      <c r="D259" s="6"/>
-      <c r="E259" s="5"/>
-      <c r="F259" s="5"/>
-      <c r="G259" s="6"/>
-      <c r="H259" s="5"/>
-      <c r="I259" s="5"/>
-      <c r="J259" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="B3:J162">
+  <autoFilter ref="B3:J161">
     <filterColumn colId="5">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue no. 56 @1341495452
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="320">
   <si>
     <t>Konzept</t>
   </si>
@@ -1042,6 +1042,15 @@
   </si>
   <si>
     <t>LAB: Geometry erweitern? Falls möglich FOV retrieve, FOV change; anderenfalls FOV degister/ retrieve, FOV change, FOV register.</t>
+  </si>
+  <si>
+    <t>Oblique einführen für ChartAzimuthalType</t>
+  </si>
+  <si>
+    <t>Synomym von Center für Oblique auflösen; Center ist eigentlich eine Art translate für Kugelkoordinaten.</t>
+  </si>
+  <si>
+    <t>http://www.ngdc.noaa.gov/mgg/shorelines/shorelines.html</t>
   </si>
 </sst>
 </file>
@@ -1518,7 +1527,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F141" sqref="F141"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1587,19 +1596,19 @@
     </row>
     <row r="4" spans="2:10" ht="33.75">
       <c r="B4" s="5">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="D4" s="6">
-        <v>41059</v>
+        <v>41092</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>312</v>
+        <v>318</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="8"/>
@@ -2352,21 +2361,21 @@
       <c r="I38" s="6"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10">
+    <row r="39" spans="2:10" ht="33.75">
       <c r="B39" s="5">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="D39" s="6">
-        <v>41057</v>
+        <v>41059</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
@@ -3189,19 +3198,19 @@
     </row>
     <row r="74" spans="2:10" ht="33.75" customHeight="1">
       <c r="B74" s="5">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D74" s="6">
-        <v>41039</v>
+        <v>41057</v>
       </c>
       <c r="E74" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="G74" s="6"/>
       <c r="H74" s="5"/>
@@ -3210,40 +3219,40 @@
     </row>
     <row r="75" spans="2:10" ht="101.25" customHeight="1">
       <c r="B75" s="5">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="D75" s="6">
-        <v>41030</v>
+        <v>41039</v>
       </c>
       <c r="E75" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G75" s="6"/>
       <c r="H75" s="5"/>
-      <c r="I75" s="6"/>
+      <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
     <row r="76" spans="2:10" ht="12.75" customHeight="1">
       <c r="B76" s="5">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="D76" s="6">
-        <v>41028</v>
+        <v>41030</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="5"/>
@@ -3674,19 +3683,19 @@
     </row>
     <row r="95" spans="2:10" ht="22.5" customHeight="1">
       <c r="B95" s="5">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D95" s="6">
-        <v>41012</v>
+        <v>41028</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G95" s="6"/>
       <c r="H95" s="5"/>
@@ -3827,21 +3836,21 @@
       <c r="I101" s="6"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="2:10" ht="22.5">
+    <row r="102" spans="2:10" ht="33.75">
       <c r="B102" s="5">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="D102" s="6">
-        <v>41011</v>
+        <v>41012</v>
       </c>
       <c r="E102" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="G102" s="6"/>
       <c r="H102" s="5"/>
@@ -3992,10 +4001,10 @@
     </row>
     <row r="109" spans="2:10" ht="12.75" customHeight="1">
       <c r="B109" s="5">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D109" s="6">
         <v>41011</v>
@@ -4004,7 +4013,7 @@
         <v>59</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="G109" s="6"/>
       <c r="H109" s="5"/>
@@ -4013,19 +4022,19 @@
     </row>
     <row r="110" spans="2:10" ht="22.5">
       <c r="B110" s="5">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="D110" s="6">
-        <v>40998</v>
+        <v>41011</v>
       </c>
       <c r="E110" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="G110" s="6"/>
       <c r="H110" s="5"/>
@@ -4078,12 +4087,12 @@
       <c r="I112" s="6"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10">
+    <row r="113" spans="2:10" ht="22.5">
       <c r="B113" s="5">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D113" s="6">
         <v>40998</v>
@@ -4091,28 +4100,28 @@
       <c r="E113" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F113" s="5"/>
+      <c r="F113" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="G113" s="6"/>
       <c r="H113" s="5"/>
       <c r="I113" s="6"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="2:10" ht="33.75">
+    <row r="114" spans="2:10">
       <c r="B114" s="5">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D114" s="6">
-        <v>40983</v>
+        <v>40998</v>
       </c>
       <c r="E114" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F114" s="5" t="s">
-        <v>304</v>
-      </c>
+      <c r="F114" s="5"/>
       <c r="G114" s="6"/>
       <c r="H114" s="5"/>
       <c r="I114" s="6"/>
@@ -4145,52 +4154,52 @@
     </row>
     <row r="116" spans="2:10" ht="33.75" customHeight="1">
       <c r="B116" s="5">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="D116" s="6">
-        <v>40972</v>
+        <v>40983</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="G116" s="6"/>
       <c r="H116" s="5"/>
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10" ht="22.5">
+    <row r="117" spans="2:10">
       <c r="B117" s="5">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="D117" s="6">
-        <v>40959</v>
+        <v>40972</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="G117" s="6"/>
       <c r="H117" s="5"/>
       <c r="I117" s="6"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="2:10">
+    <row r="118" spans="2:10" ht="22.5">
       <c r="B118" s="5">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="D118" s="6">
         <v>40959</v>
@@ -4198,7 +4207,9 @@
       <c r="E118" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F118" s="5"/>
+      <c r="F118" s="5" t="s">
+        <v>261</v>
+      </c>
       <c r="G118" s="6"/>
       <c r="H118" s="5"/>
       <c r="I118" s="6"/>
@@ -4206,10 +4217,10 @@
     </row>
     <row r="119" spans="2:10" ht="33.75" customHeight="1">
       <c r="B119" s="5">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>263</v>
+        <v>282</v>
       </c>
       <c r="D119" s="6">
         <v>40959</v>
@@ -4217,9 +4228,7 @@
       <c r="E119" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F119" s="5" t="s">
-        <v>264</v>
-      </c>
+      <c r="F119" s="5"/>
       <c r="G119" s="6"/>
       <c r="H119" s="5"/>
       <c r="I119" s="6"/>
@@ -4227,18 +4236,20 @@
     </row>
     <row r="120" spans="2:10">
       <c r="B120" s="5">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="D120" s="6">
-        <v>40956</v>
+        <v>40959</v>
       </c>
       <c r="E120" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F120" s="5"/>
+      <c r="F120" s="5" t="s">
+        <v>264</v>
+      </c>
       <c r="G120" s="6"/>
       <c r="H120" s="5"/>
       <c r="I120" s="6"/>
@@ -4267,12 +4278,12 @@
       <c r="I121" s="6"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="2:10" ht="45">
+    <row r="122" spans="2:10">
       <c r="B122" s="5">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D122" s="6">
         <v>40956</v>
@@ -4280,92 +4291,90 @@
       <c r="E122" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F122" s="5" t="s">
-        <v>259</v>
-      </c>
+      <c r="F122" s="5"/>
       <c r="G122" s="6"/>
       <c r="H122" s="5"/>
       <c r="I122" s="6"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10">
+    <row r="123" spans="2:10" ht="45">
       <c r="B123" s="5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="D123" s="6">
-        <v>40947</v>
+        <v>40956</v>
       </c>
       <c r="E123" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F123" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>259</v>
+      </c>
       <c r="G123" s="6"/>
-      <c r="H123" s="5" t="s">
-        <v>276</v>
-      </c>
+      <c r="H123" s="5"/>
       <c r="I123" s="6"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="2:10" ht="45">
+    <row r="124" spans="2:10">
       <c r="B124" s="5">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C124" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D124" s="6">
         <v>40947</v>
       </c>
       <c r="E124" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F124" s="5" t="s">
-        <v>255</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F124" s="5"/>
       <c r="G124" s="6"/>
-      <c r="H124" s="5"/>
+      <c r="H124" s="5" t="s">
+        <v>276</v>
+      </c>
       <c r="I124" s="6"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="2:10" ht="33.75">
+    <row r="125" spans="2:10" ht="45">
       <c r="B125" s="5">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C125" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D125" s="6">
-        <v>40941</v>
+        <v>40947</v>
       </c>
       <c r="E125" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G125" s="6"/>
       <c r="H125" s="5"/>
       <c r="I125" s="6"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="2:10" ht="22.5">
+    <row r="126" spans="2:10" ht="33.75">
       <c r="B126" s="5">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C126" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D126" s="6">
-        <v>40869</v>
+        <v>40941</v>
       </c>
       <c r="E126" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="5"/>
@@ -4374,52 +4383,52 @@
     </row>
     <row r="127" spans="2:10" ht="22.5">
       <c r="B127" s="5">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C127" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D127" s="6">
-        <v>40866</v>
+        <v>40869</v>
       </c>
       <c r="E127" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G127" s="6"/>
       <c r="H127" s="5"/>
       <c r="I127" s="6"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="2:10" ht="33.75">
+    <row r="128" spans="2:10" ht="22.5">
       <c r="B128" s="5">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C128" s="5" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D128" s="6">
-        <v>40829</v>
+        <v>40866</v>
       </c>
       <c r="E128" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="5"/>
       <c r="I128" s="6"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="2:10" ht="45">
+    <row r="129" spans="2:10" ht="33.75">
       <c r="B129" s="5">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C129" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D129" s="6">
         <v>40829</v>
@@ -4428,7 +4437,7 @@
         <v>59</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G129" s="6"/>
       <c r="H129" s="5"/>
@@ -4437,45 +4446,43 @@
     </row>
     <row r="130" spans="2:10" ht="22.5" customHeight="1">
       <c r="B130" s="5">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C130" s="5" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="D130" s="6">
-        <v>40822</v>
+        <v>40829</v>
       </c>
       <c r="E130" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="G130" s="6"/>
       <c r="H130" s="5"/>
       <c r="I130" s="6"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="2:10" ht="22.5">
+    <row r="131" spans="2:10">
       <c r="B131" s="5">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C131" s="5" t="s">
-        <v>239</v>
+        <v>267</v>
       </c>
       <c r="D131" s="6">
-        <v>40816</v>
+        <v>40822</v>
       </c>
       <c r="E131" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>287</v>
+        <v>268</v>
       </c>
       <c r="G131" s="6"/>
-      <c r="H131" s="5" t="s">
-        <v>294</v>
-      </c>
+      <c r="H131" s="5"/>
       <c r="I131" s="6"/>
       <c r="J131" s="5"/>
     </row>
@@ -4556,22 +4563,24 @@
     </row>
     <row r="135" spans="2:10" ht="22.5">
       <c r="B135" s="5">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C135" s="5" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="D135" s="6">
-        <v>40794</v>
+        <v>40816</v>
       </c>
       <c r="E135" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>238</v>
+        <v>287</v>
       </c>
       <c r="G135" s="6"/>
-      <c r="H135" s="5"/>
+      <c r="H135" s="5" t="s">
+        <v>294</v>
+      </c>
       <c r="I135" s="6"/>
       <c r="J135" s="5"/>
     </row>
@@ -4602,165 +4611,167 @@
     </row>
     <row r="137" spans="2:10" ht="22.5">
       <c r="B137" s="5">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D137" s="6">
-        <v>40763</v>
+        <v>40794</v>
       </c>
       <c r="E137" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="5"/>
       <c r="I137" s="6"/>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="2:10">
+    <row r="138" spans="2:10" ht="22.5">
       <c r="B138" s="5">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C138" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D138" s="6">
-        <v>40762</v>
+        <v>40763</v>
       </c>
       <c r="E138" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F138" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="5"/>
       <c r="I138" s="6"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="2:10" ht="22.5">
+    <row r="139" spans="2:10">
       <c r="B139" s="5">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C139" s="5" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D139" s="6">
-        <v>40750</v>
+        <v>40762</v>
       </c>
       <c r="E139" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="G139" s="6"/>
       <c r="H139" s="5"/>
       <c r="I139" s="6"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="2:10" ht="33.75">
+    <row r="140" spans="2:10" ht="22.5">
       <c r="B140" s="5">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C140" s="5" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D140" s="6">
-        <v>40742</v>
+        <v>40750</v>
       </c>
       <c r="E140" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="5"/>
       <c r="I140" s="6"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="2:10">
+    <row r="141" spans="2:10" ht="33.75">
       <c r="B141" s="5">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C141" s="5" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="D141" s="6">
-        <v>40589</v>
+        <v>40742</v>
       </c>
       <c r="E141" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>208</v>
+        <v>241</v>
       </c>
       <c r="G141" s="6"/>
       <c r="H141" s="5"/>
       <c r="I141" s="6"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10" ht="67.5">
+    <row r="142" spans="2:10">
       <c r="B142" s="5">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C142" s="5" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D142" s="6">
-        <v>40566</v>
+        <v>40589</v>
       </c>
       <c r="E142" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="G142" s="6"/>
       <c r="H142" s="5"/>
       <c r="I142" s="6"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="2:10" ht="33.75">
+    <row r="143" spans="2:10" ht="67.5">
       <c r="B143" s="5">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C143" s="5" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="D143" s="6">
-        <v>40506</v>
+        <v>40566</v>
       </c>
       <c r="E143" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F143" s="5" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="G143" s="6"/>
       <c r="H143" s="5"/>
       <c r="I143" s="6"/>
       <c r="J143" s="5"/>
     </row>
-    <row r="144" spans="2:10">
+    <row r="144" spans="2:10" ht="33.75">
       <c r="B144" s="5">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C144" s="5" t="s">
-        <v>269</v>
+        <v>191</v>
       </c>
       <c r="D144" s="6">
-        <v>40188</v>
+        <v>40506</v>
       </c>
       <c r="E144" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F144" s="5"/>
+      <c r="F144" s="5" t="s">
+        <v>250</v>
+      </c>
       <c r="G144" s="6"/>
       <c r="H144" s="5"/>
       <c r="I144" s="6"/>
@@ -4768,13 +4779,13 @@
     </row>
     <row r="145" spans="2:10">
       <c r="B145" s="5">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>136</v>
+        <v>269</v>
       </c>
       <c r="D145" s="6">
-        <v>39904</v>
+        <v>40188</v>
       </c>
       <c r="E145" s="5" t="s">
         <v>59</v>
@@ -4787,10 +4798,10 @@
     </row>
     <row r="146" spans="2:10">
       <c r="B146" s="5">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C146" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D146" s="6">
         <v>39904</v>
@@ -4798,18 +4809,20 @@
       <c r="E146" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F146" s="5"/>
+      <c r="F146" s="5" t="s">
+        <v>319</v>
+      </c>
       <c r="G146" s="6"/>
       <c r="H146" s="5"/>
       <c r="I146" s="6"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="2:10" ht="22.5">
+    <row r="147" spans="2:10">
       <c r="B147" s="5">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C147" s="5" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D147" s="6">
         <v>39904</v>
@@ -4823,54 +4836,54 @@
       <c r="I147" s="6"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10" ht="33.75">
+    <row r="148" spans="2:10" ht="22.5">
       <c r="B148" s="5">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C148" s="5" t="s">
-        <v>315</v>
+        <v>151</v>
       </c>
       <c r="D148" s="6">
-        <v>39479</v>
+        <v>39904</v>
       </c>
       <c r="E148" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F148" s="5" t="s">
-        <v>316</v>
-      </c>
+      <c r="F148" s="5"/>
       <c r="G148" s="6"/>
-      <c r="H148" s="5" t="s">
-        <v>314</v>
-      </c>
+      <c r="H148" s="5"/>
       <c r="I148" s="6"/>
       <c r="J148" s="5"/>
     </row>
-    <row r="149" spans="2:10" ht="22.5">
+    <row r="149" spans="2:10" ht="33.75">
       <c r="B149" s="5">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C149" s="5" t="s">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="D149" s="6">
-        <v>39122</v>
+        <v>39479</v>
       </c>
       <c r="E149" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F149" s="5"/>
+      <c r="F149" s="5" t="s">
+        <v>316</v>
+      </c>
       <c r="G149" s="6"/>
-      <c r="H149" s="5"/>
+      <c r="H149" s="5" t="s">
+        <v>314</v>
+      </c>
       <c r="I149" s="6"/>
       <c r="J149" s="5"/>
     </row>
     <row r="150" spans="2:10" ht="22.5">
       <c r="B150" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C150" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D150" s="6">
         <v>39122</v>
@@ -4878,25 +4891,31 @@
       <c r="E150" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F150" s="5" t="s">
-        <v>272</v>
-      </c>
+      <c r="F150" s="5"/>
       <c r="G150" s="6"/>
       <c r="H150" s="5"/>
       <c r="I150" s="6"/>
       <c r="J150" s="5"/>
     </row>
-    <row r="151" spans="2:10">
+    <row r="151" spans="2:10" ht="22.5">
       <c r="B151" s="5">
-        <v>149</v>
-      </c>
-      <c r="C151" s="5"/>
-      <c r="D151" s="6"/>
-      <c r="E151" s="5"/>
-      <c r="F151" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="C151" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D151" s="6">
+        <v>39122</v>
+      </c>
+      <c r="E151" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F151" s="5" t="s">
+        <v>272</v>
+      </c>
       <c r="G151" s="6"/>
       <c r="H151" s="5"/>
-      <c r="I151" s="5"/>
+      <c r="I151" s="6"/>
       <c r="J151" s="5"/>
     </row>
     <row r="152" spans="2:10">
@@ -6104,8 +6123,8 @@
     <filterColumn colId="7">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="B4:J162">
-      <sortCondition descending="1" ref="D3:D162"/>
+    <sortState ref="B4:J161">
+      <sortCondition descending="1" ref="D3:D161"/>
     </sortState>
   </autoFilter>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Issue no. 57 @1342099925
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="323">
   <si>
     <t>Konzept</t>
   </si>
@@ -1051,6 +1051,16 @@
   </si>
   <si>
     <t>http://www.ngdc.noaa.gov/mgg/shorelines/shorelines.html</t>
+  </si>
+  <si>
+    <t>Anforderung unverständlich.</t>
+  </si>
+  <si>
+    <t>Nicht notwendig.</t>
+  </si>
+  <si>
+    <t>http://www.ihsenergy.com/epsg/guid7.pdf
+PROJ 1.4</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1621,9 @@
         <v>318</v>
       </c>
       <c r="G4" s="6"/>
-      <c r="H4" s="8"/>
+      <c r="H4" s="5" t="s">
+        <v>322</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
@@ -2361,7 +2373,7 @@
       <c r="I38" s="6"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10" ht="33.75">
+    <row r="39" spans="2:10" ht="33.75" hidden="1">
       <c r="B39" s="5">
         <v>147</v>
       </c>
@@ -2377,7 +2389,9 @@
       <c r="F39" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="G39" s="6"/>
+      <c r="G39" s="6">
+        <v>41099</v>
+      </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -3217,7 +3231,7 @@
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="2:10" ht="101.25" customHeight="1">
+    <row r="75" spans="2:10" ht="101.25" hidden="1" customHeight="1">
       <c r="B75" s="5">
         <v>145</v>
       </c>
@@ -3233,12 +3247,14 @@
       <c r="F75" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="G75" s="6"/>
+      <c r="G75" s="6">
+        <v>41098</v>
+      </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="2:10" ht="12.75" customHeight="1">
+    <row r="76" spans="2:10" ht="12.75" hidden="1" customHeight="1">
       <c r="B76" s="5">
         <v>144</v>
       </c>
@@ -3254,7 +3270,9 @@
       <c r="F76" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="G76" s="6"/>
+      <c r="G76" s="6">
+        <v>41102</v>
+      </c>
       <c r="H76" s="5"/>
       <c r="I76" s="6"/>
       <c r="J76" s="5"/>
@@ -3836,7 +3854,7 @@
       <c r="I101" s="6"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="2:10" ht="33.75">
+    <row r="102" spans="2:10" ht="33.75" hidden="1">
       <c r="B102" s="5">
         <v>142</v>
       </c>
@@ -3852,7 +3870,9 @@
       <c r="F102" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="G102" s="6"/>
+      <c r="G102" s="6">
+        <v>41099</v>
+      </c>
       <c r="H102" s="5"/>
       <c r="I102" s="6"/>
       <c r="J102" s="5"/>
@@ -3999,7 +4019,7 @@
       <c r="I108" s="6"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="2:10" ht="12.75" customHeight="1">
+    <row r="109" spans="2:10" ht="22.5">
       <c r="B109" s="5">
         <v>139</v>
       </c>
@@ -4173,7 +4193,7 @@
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10">
+    <row r="117" spans="2:10" hidden="1">
       <c r="B117" s="5">
         <v>133</v>
       </c>
@@ -4189,7 +4209,9 @@
       <c r="F117" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G117" s="6"/>
+      <c r="G117" s="6">
+        <v>41099</v>
+      </c>
       <c r="H117" s="5"/>
       <c r="I117" s="6"/>
       <c r="J117" s="5"/>
@@ -4215,7 +4237,7 @@
       <c r="I118" s="6"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="2:10" ht="33.75" customHeight="1">
+    <row r="119" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B119" s="5">
         <v>128</v>
       </c>
@@ -4231,8 +4253,12 @@
       <c r="F119" s="5"/>
       <c r="G119" s="6"/>
       <c r="H119" s="5"/>
-      <c r="I119" s="6"/>
-      <c r="J119" s="5"/>
+      <c r="I119" s="6">
+        <v>41099</v>
+      </c>
+      <c r="J119" s="5" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="120" spans="2:10">
       <c r="B120" s="5">
@@ -4423,7 +4449,7 @@
       <c r="I128" s="6"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="2:10" ht="33.75">
+    <row r="129" spans="2:10" ht="33.75" hidden="1">
       <c r="B129" s="5">
         <v>117</v>
       </c>
@@ -4439,12 +4465,14 @@
       <c r="F129" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G129" s="6"/>
+      <c r="G129" s="6">
+        <v>41099</v>
+      </c>
       <c r="H129" s="5"/>
       <c r="I129" s="6"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="2:10" ht="22.5" customHeight="1">
+    <row r="130" spans="2:10" ht="45">
       <c r="B130" s="5">
         <v>118</v>
       </c>
@@ -4561,7 +4589,7 @@
       <c r="I134" s="6"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="2:10" ht="22.5">
+    <row r="135" spans="2:10" ht="22.5" hidden="1">
       <c r="B135" s="5">
         <v>115</v>
       </c>
@@ -4577,7 +4605,9 @@
       <c r="F135" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="G135" s="6"/>
+      <c r="G135" s="6">
+        <v>41099</v>
+      </c>
       <c r="H135" s="5" t="s">
         <v>294</v>
       </c>
@@ -4672,7 +4702,7 @@
       <c r="I139" s="6"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="2:10" ht="22.5">
+    <row r="140" spans="2:10" ht="22.5" hidden="1">
       <c r="B140" s="5">
         <v>108</v>
       </c>
@@ -4690,8 +4720,12 @@
       </c>
       <c r="G140" s="6"/>
       <c r="H140" s="5"/>
-      <c r="I140" s="6"/>
-      <c r="J140" s="5"/>
+      <c r="I140" s="6">
+        <v>41099</v>
+      </c>
+      <c r="J140" s="5" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="141" spans="2:10" ht="33.75">
       <c r="B141" s="5">
@@ -4714,7 +4748,7 @@
       <c r="I141" s="6"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10">
+    <row r="142" spans="2:10" hidden="1">
       <c r="B142" s="5">
         <v>100</v>
       </c>
@@ -4730,12 +4764,14 @@
       <c r="F142" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="G142" s="6"/>
+      <c r="G142" s="6">
+        <v>41099</v>
+      </c>
       <c r="H142" s="5"/>
       <c r="I142" s="6"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="2:10" ht="67.5">
+    <row r="143" spans="2:10" ht="67.5" hidden="1">
       <c r="B143" s="5">
         <v>97</v>
       </c>
@@ -4753,8 +4789,12 @@
       </c>
       <c r="G143" s="6"/>
       <c r="H143" s="5"/>
-      <c r="I143" s="6"/>
-      <c r="J143" s="5"/>
+      <c r="I143" s="6">
+        <v>41099</v>
+      </c>
+      <c r="J143" s="5" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="144" spans="2:10" ht="33.75">
       <c r="B144" s="5">
@@ -4796,7 +4836,7 @@
       <c r="I145" s="6"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="2:10">
+    <row r="146" spans="2:10" ht="22.5">
       <c r="B146" s="5">
         <v>72</v>
       </c>

</xml_diff>

<commit_message>
Issue no. 58 @1342808581
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="10410" windowHeight="7335"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="326">
   <si>
     <t>Konzept</t>
   </si>
@@ -1061,6 +1061,15 @@
   <si>
     <t>http://www.ihsenergy.com/epsg/guid7.pdf
 PROJ 1.4</t>
+  </si>
+  <si>
+    <t>Projector.</t>
+  </si>
+  <si>
+    <t>Epoch.</t>
+  </si>
+  <si>
+    <t>Interface Projector überarbeitet.</t>
   </si>
 </sst>
 </file>
@@ -1177,7 +1186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1235,6 +1244,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1537,7 +1549,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -3210,7 +3222,7 @@
       <c r="I73" s="6"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="2:10" ht="33.75" customHeight="1">
+    <row r="74" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B74" s="5">
         <v>146</v>
       </c>
@@ -3226,10 +3238,18 @@
       <c r="F74" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="G74" s="6"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
+      <c r="G74" s="6">
+        <v>41108</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="I74" s="20">
+        <v>41108</v>
+      </c>
+      <c r="J74" s="5" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="75" spans="2:10" ht="101.25" hidden="1" customHeight="1">
       <c r="B75" s="5">
@@ -4019,7 +4039,7 @@
       <c r="I108" s="6"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="2:10" ht="22.5">
+    <row r="109" spans="2:10" ht="22.5" hidden="1">
       <c r="B109" s="5">
         <v>139</v>
       </c>
@@ -4035,7 +4055,9 @@
       <c r="F109" s="5" t="s">
         <v>301</v>
       </c>
-      <c r="G109" s="6"/>
+      <c r="G109" s="6">
+        <v>41108</v>
+      </c>
       <c r="H109" s="5"/>
       <c r="I109" s="6"/>
       <c r="J109" s="5"/>
@@ -4107,7 +4129,7 @@
       <c r="I112" s="6"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10" ht="22.5">
+    <row r="113" spans="2:10" ht="22.5" hidden="1">
       <c r="B113" s="5">
         <v>137</v>
       </c>
@@ -4123,7 +4145,9 @@
       <c r="F113" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="G113" s="6"/>
+      <c r="G113" s="6">
+        <v>41108</v>
+      </c>
       <c r="H113" s="5"/>
       <c r="I113" s="6"/>
       <c r="J113" s="5"/>
@@ -4172,7 +4196,7 @@
       <c r="I115" s="6"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="2:10" ht="33.75" customHeight="1">
+    <row r="116" spans="2:10" ht="33.75" hidden="1" customHeight="1">
       <c r="B116" s="5">
         <v>135</v>
       </c>
@@ -4188,8 +4212,12 @@
       <c r="F116" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="G116" s="6"/>
-      <c r="H116" s="5"/>
+      <c r="G116" s="6">
+        <v>41108</v>
+      </c>
+      <c r="H116" s="5" t="s">
+        <v>325</v>
+      </c>
       <c r="I116" s="6"/>
       <c r="J116" s="5"/>
     </row>

</xml_diff>

<commit_message>
Issue no. 60 @1375284891
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="344">
   <si>
     <t>Konzept</t>
   </si>
@@ -1123,7 +1123,11 @@
     <t>jdToEcliptical umbenannt in jdToEquatorial, BodyPlanet, BodySun, BodyMoon angepasst.</t>
   </si>
   <si>
-    <t>07.06.2013: Artwork umgesetzt; schwache Performance.</t>
+    <t>Aus Viewer-Pipe lesen</t>
+  </si>
+  <si>
+    <t>07.06.2013: Artwork umgesetzt; schwache Performance.
+30.07.2013: Durch Verwendung on PS:image Performance verbessert.</t>
   </si>
 </sst>
 </file>
@@ -1607,10 +1611,10 @@
   <dimension ref="B1:J258"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H53" sqref="H53"/>
+      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1704,20 +1708,18 @@
     </row>
     <row r="5" spans="2:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="D5" s="6">
-        <v>41363</v>
+        <v>41484</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>338</v>
-      </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="6"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -1744,21 +1746,21 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D7" s="6">
-        <v>41362</v>
+        <v>41363</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
@@ -1767,19 +1769,19 @@
     </row>
     <row r="8" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="D8" s="6">
-        <v>41229</v>
+        <v>41362</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5"/>
@@ -1788,10 +1790,10 @@
     </row>
     <row r="9" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D9" s="6">
         <v>41229</v>
@@ -1800,73 +1802,71 @@
         <v>59</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="D10" s="6">
-        <v>41224</v>
+        <v>41229</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D11" s="6">
-        <v>41128</v>
+        <v>41224</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5" t="s">
+        <v>325</v>
+      </c>
       <c r="G11" s="6"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="D12" s="6">
-        <v>41092</v>
+        <v>41128</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>316</v>
-      </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="5" t="s">
-        <v>331</v>
-      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
@@ -1968,25 +1968,27 @@
       <c r="I16" s="6"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B17" s="5">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="D17" s="6">
-        <v>41028</v>
+        <v>41092</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
+      <c r="H17" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
@@ -2058,21 +2060,21 @@
       <c r="I20" s="6"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" s="5">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="D21" s="6">
-        <v>41011</v>
+        <v>41028</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="5"/>
@@ -2123,20 +2125,22 @@
       <c r="I23" s="6"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B24" s="5">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="D24" s="6">
-        <v>40998</v>
+        <v>41011</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5" t="s">
+        <v>330</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
@@ -2215,22 +2219,20 @@
       <c r="I27" s="6"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="5">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>259</v>
+        <v>291</v>
       </c>
       <c r="D28" s="6">
-        <v>40959</v>
+        <v>40998</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>260</v>
-      </c>
+      <c r="F28" s="5"/>
       <c r="G28" s="6"/>
       <c r="H28" s="5"/>
       <c r="I28" s="6"/>
@@ -2261,10 +2263,10 @@
     </row>
     <row r="30" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="5">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D30" s="6">
         <v>40959</v>
@@ -2273,7 +2275,7 @@
         <v>59</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="5"/>
@@ -2357,18 +2359,20 @@
     </row>
     <row r="34" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D34" s="6">
-        <v>40956</v>
+        <v>40959</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F34" s="5"/>
+      <c r="F34" s="5" t="s">
+        <v>263</v>
+      </c>
       <c r="G34" s="6"/>
       <c r="H34" s="5"/>
       <c r="I34" s="6"/>
@@ -2376,10 +2380,10 @@
     </row>
     <row r="35" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D35" s="6">
         <v>40956</v>
@@ -2387,92 +2391,90 @@
       <c r="E35" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>258</v>
-      </c>
+      <c r="F35" s="5"/>
       <c r="G35" s="6"/>
       <c r="H35" s="5"/>
       <c r="I35" s="6"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" ht="45" x14ac:dyDescent="0.2">
       <c r="B36" s="5">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="D36" s="6">
-        <v>40947</v>
+        <v>40956</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="5"/>
+        <v>59</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>258</v>
+      </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="5" t="s">
-        <v>275</v>
-      </c>
+      <c r="H36" s="5"/>
       <c r="I36" s="6"/>
       <c r="J36" s="5"/>
     </row>
     <row r="37" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D37" s="6">
         <v>40947</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>254</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F37" s="5"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="5"/>
+      <c r="H37" s="5" t="s">
+        <v>275</v>
+      </c>
       <c r="I37" s="6"/>
       <c r="J37" s="5"/>
     </row>
     <row r="38" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="D38" s="6">
-        <v>40941</v>
+        <v>40947</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="5"/>
       <c r="I38" s="6"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B39" s="5">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D39" s="6">
-        <v>40869</v>
+        <v>40941</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
@@ -2504,19 +2506,19 @@
     </row>
     <row r="41" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D41" s="6">
-        <v>40866</v>
+        <v>40869</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="5"/>
@@ -2546,21 +2548,21 @@
       <c r="I42" s="6"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="2:10" ht="45" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B43" s="5">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D43" s="6">
-        <v>40829</v>
+        <v>40866</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="5"/>
@@ -2569,19 +2571,19 @@
     </row>
     <row r="44" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="5">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="D44" s="6">
-        <v>40822</v>
+        <v>40829</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="G44" s="6"/>
       <c r="H44" s="5"/>
@@ -2640,19 +2642,19 @@
     </row>
     <row r="47" spans="2:10" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="5">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>235</v>
+        <v>266</v>
       </c>
       <c r="D47" s="6">
-        <v>40794</v>
+        <v>40822</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="5"/>
@@ -2661,19 +2663,19 @@
     </row>
     <row r="48" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="5">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D48" s="6">
-        <v>40763</v>
+        <v>40794</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="5"/>
@@ -2682,19 +2684,19 @@
     </row>
     <row r="49" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="5">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D49" s="6">
-        <v>40762</v>
+        <v>40763</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="5"/>
@@ -2774,24 +2776,22 @@
     </row>
     <row r="53" spans="2:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="5">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="D53" s="6">
-        <v>40742</v>
+        <v>40762</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>333</v>
+        <v>230</v>
       </c>
       <c r="G53" s="6"/>
-      <c r="H53" s="5" t="s">
-        <v>342</v>
-      </c>
+      <c r="H53" s="5"/>
       <c r="I53" s="6"/>
       <c r="J53" s="5"/>
     </row>
@@ -3098,24 +3098,28 @@
       <c r="I66" s="6"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="2:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:10" ht="33.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="5">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="D67" s="6">
-        <v>40506</v>
+        <v>40742</v>
       </c>
       <c r="E67" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="G67" s="6"/>
-      <c r="H67" s="5"/>
+        <v>333</v>
+      </c>
+      <c r="G67" s="6">
+        <v>41485</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>343</v>
+      </c>
       <c r="I67" s="6"/>
       <c r="J67" s="5"/>
     </row>
@@ -3472,18 +3476,20 @@
     </row>
     <row r="83" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="5">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>268</v>
+        <v>191</v>
       </c>
       <c r="D83" s="6">
-        <v>40188</v>
+        <v>40506</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F83" s="5"/>
+      <c r="F83" s="5" t="s">
+        <v>249</v>
+      </c>
       <c r="G83" s="6"/>
       <c r="H83" s="5"/>
       <c r="I83" s="6"/>
@@ -3675,20 +3681,18 @@
     </row>
     <row r="92" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B92" s="5">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>136</v>
+        <v>268</v>
       </c>
       <c r="D92" s="6">
-        <v>39904</v>
+        <v>40188</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F92" s="5" t="s">
-        <v>329</v>
-      </c>
+      <c r="F92" s="5"/>
       <c r="G92" s="6"/>
       <c r="H92" s="5"/>
       <c r="I92" s="6"/>
@@ -3696,10 +3700,10 @@
     </row>
     <row r="93" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="5">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D93" s="6">
         <v>39904</v>
@@ -3707,7 +3711,9 @@
       <c r="E93" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F93" s="5"/>
+      <c r="F93" s="5" t="s">
+        <v>329</v>
+      </c>
       <c r="G93" s="6"/>
       <c r="H93" s="5"/>
       <c r="I93" s="6"/>
@@ -3715,10 +3721,10 @@
     </row>
     <row r="94" spans="2:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="5">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D94" s="6">
         <v>39904</v>
@@ -4408,26 +4414,22 @@
       <c r="I122" s="6"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B123" s="5">
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>313</v>
+        <v>151</v>
       </c>
       <c r="D123" s="6">
-        <v>39479</v>
+        <v>39904</v>
       </c>
       <c r="E123" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F123" s="5" t="s">
-        <v>314</v>
-      </c>
+      <c r="F123" s="5"/>
       <c r="G123" s="6"/>
-      <c r="H123" s="5" t="s">
-        <v>312</v>
-      </c>
+      <c r="H123" s="5"/>
       <c r="I123" s="6"/>
       <c r="J123" s="5"/>
     </row>
@@ -5179,33 +5181,35 @@
       <c r="I157" s="6"/>
       <c r="J157" s="5"/>
     </row>
-    <row r="158" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B158" s="5">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="C158" s="5" t="s">
-        <v>269</v>
+        <v>313</v>
       </c>
       <c r="D158" s="6">
-        <v>39122</v>
+        <v>39479</v>
       </c>
       <c r="E158" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F158" s="5" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="G158" s="6"/>
-      <c r="H158" s="5"/>
+      <c r="H158" s="5" t="s">
+        <v>312</v>
+      </c>
       <c r="I158" s="6"/>
       <c r="J158" s="5"/>
     </row>
     <row r="159" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B159" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C159" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D159" s="6">
         <v>39122</v>
@@ -5214,24 +5218,32 @@
         <v>59</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>271</v>
+        <v>324</v>
       </c>
       <c r="G159" s="6"/>
       <c r="H159" s="5"/>
       <c r="I159" s="6"/>
       <c r="J159" s="5"/>
     </row>
-    <row r="160" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B160" s="5">
-        <v>158</v>
-      </c>
-      <c r="C160" s="5"/>
-      <c r="D160" s="6"/>
-      <c r="E160" s="5"/>
-      <c r="F160" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D160" s="6">
+        <v>39122</v>
+      </c>
+      <c r="E160" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F160" s="5" t="s">
+        <v>271</v>
+      </c>
       <c r="G160" s="6"/>
       <c r="H160" s="5"/>
-      <c r="I160" s="5"/>
+      <c r="I160" s="6"/>
       <c r="J160" s="5"/>
     </row>
     <row r="161" spans="2:10" x14ac:dyDescent="0.2">
@@ -6378,8 +6390,8 @@
     <filterColumn colId="7">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="B4:J189">
-      <sortCondition descending="1" ref="D3:D164"/>
+    <sortState ref="B5:J189">
+      <sortCondition descending="1" ref="D3:D189"/>
     </sortState>
   </autoFilter>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Issue no. 61 @1379161847
</commit_message>
<xml_diff>
--- a/fare.xlsx
+++ b/fare.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="10410" windowHeight="7335"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="10410" windowHeight="7335" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="fare" sheetId="15" r:id="rId1"/>
-    <sheet name="Template" sheetId="5" r:id="rId2"/>
+    <sheet name="Template" sheetId="5" r:id="rId1"/>
+    <sheet name="fare" sheetId="15" r:id="rId2"/>
+    <sheet name="ds9" sheetId="16" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fare!$B$3:$J$189</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">fare!$B$3:$J$189</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="359">
   <si>
     <t>Konzept</t>
   </si>
@@ -1068,10 +1069,6 @@
     <t>Werte durch BodyPlanet, ... in Registry speichern, mit substitute in DialDay auswerten.</t>
   </si>
   <si>
-    <t>Linienstärke oder -helligkeit prüfen, Umsetzung anlalog mag bei BodyStellar.
-Auch für CatalogWDBII.</t>
-  </si>
-  <si>
     <t>Hauptstädtekatalog einführen</t>
   </si>
   <si>
@@ -1128,13 +1125,70 @@
   <si>
     <t>07.06.2013: Artwork umgesetzt; schwache Performance.
 30.07.2013: Durch Verwendung on PS:image Performance verbessert.</t>
+  </si>
+  <si>
+    <t>Linienstärke oder -helligkeit prüfen, Umsetzung anlalog mag bei BodyStellar.
+Auch für CatalogWDBII.
+BodyArea-Attribut authentic prüfen, node mit level-Wert einführen.
+BodyAreal-Attribute nature optional (Änderung in BodyAreal beachten), Helligkeit/ Farbe als CatalogDS9-Attribut einführen; auch für 7118, 7237.</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>linewidth</t>
+  </si>
+  <si>
+    <t>0..255</t>
+  </si>
+  <si>
+    <t>dark</t>
+  </si>
+  <si>
+    <t>bright</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>setlinewidth</t>
+  </si>
+  <si>
+    <t>setrgbcolor</t>
+  </si>
+  <si>
+    <t>setgray</t>
+  </si>
+  <si>
+    <t>BodyAreal-Attribut nature optional.
+PS aus Preferences in DS9, 7118, 7237, Referenz URL, Type bzw. OType.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
+    <numFmt numFmtId="172" formatCode="0.00000000000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1149,6 +1203,10 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1241,10 +1299,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1291,6 +1350,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1306,12 +1377,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEEF5FF"/>
+      <color rgb="FFCCFFFF"/>
+      <color rgb="FFEFE5FE"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1607,6 +1690,314 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="0.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="11.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="24"/>
+      <c r="I2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="5">
+        <f t="shared" ref="B4:B19" si="0">ROW(B2)-1</f>
+        <v>1</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="5">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B10" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B11" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B15" s="5">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="B1:J258"/>
   <sheetViews>
@@ -1614,7 +2005,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G83" sqref="G83"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1653,14 +2044,14 @@
       <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="23"/>
+      <c r="I2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="11"/>
@@ -1686,7 +2077,7 @@
         <v>157</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D4" s="6">
         <v>41373</v>
@@ -1695,13 +2086,13 @@
         <v>60</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G4" s="6">
         <v>41374</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -1711,7 +2102,7 @@
         <v>158</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D5" s="6">
         <v>41484</v>
@@ -1730,7 +2121,7 @@
         <v>154</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D6" s="6">
         <v>41362</v>
@@ -1751,7 +2142,7 @@
         <v>156</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D7" s="6">
         <v>41363</v>
@@ -1760,7 +2151,7 @@
         <v>59</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
@@ -1772,7 +2163,7 @@
         <v>155</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D8" s="6">
         <v>41362</v>
@@ -1781,7 +2172,7 @@
         <v>60</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="5"/>
@@ -1793,7 +2184,7 @@
         <v>152</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D9" s="6">
         <v>41229</v>
@@ -1802,7 +2193,7 @@
         <v>59</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5"/>
@@ -1814,7 +2205,7 @@
         <v>153</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D10" s="6">
         <v>41229</v>
@@ -1823,14 +2214,14 @@
         <v>59</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:10" ht="101.25" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
         <v>151</v>
       </c>
@@ -1844,10 +2235,14 @@
         <v>59</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="5"/>
+        <v>343</v>
+      </c>
+      <c r="G11" s="6">
+        <v>41518</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>358</v>
+      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
@@ -1986,7 +2381,7 @@
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -2139,7 +2534,7 @@
         <v>59</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="5"/>
@@ -3112,13 +3507,13 @@
         <v>59</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G67" s="6">
         <v>41485</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="I67" s="6"/>
       <c r="J67" s="5"/>
@@ -3712,7 +4107,7 @@
         <v>59</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G93" s="6"/>
       <c r="H93" s="5"/>
@@ -6405,310 +6800,802 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J19"/>
+  <dimension ref="C4:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K12" sqref="K12:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="0.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="36.5703125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="5" width="10.7109375" customWidth="1"/>
+    <col min="11" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="3" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="E4" s="27" t="s">
+        <v>351</v>
+      </c>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+    </row>
+    <row r="5" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="E5" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="O5"/>
+      <c r="P5" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C6" s="21"/>
+      <c r="D6" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6">
+        <v>245</v>
+      </c>
+      <c r="F6">
+        <v>239</v>
+      </c>
+      <c r="G6">
+        <v>245</v>
+      </c>
+      <c r="H6">
+        <v>255</v>
+      </c>
+      <c r="I6" s="18">
+        <f>E6/255</f>
+        <v>0.96078431372549022</v>
+      </c>
+      <c r="J6" s="18"/>
+      <c r="K6" s="28">
+        <f>F6/255</f>
+        <v>0.93725490196078431</v>
+      </c>
+      <c r="L6" s="28">
+        <f>G6/255</f>
+        <v>0.96078431372549022</v>
+      </c>
+      <c r="M6" s="28">
+        <f>H6/255</f>
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>350</v>
+      </c>
+      <c r="P6">
+        <v>0.8</v>
+      </c>
+      <c r="Q6" s="19">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="C7" s="21"/>
+      <c r="D7" t="s">
+        <v>352</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>71</v>
+      </c>
+      <c r="H7">
+        <v>172</v>
+      </c>
+      <c r="I7" s="18">
+        <f>E7/255</f>
+        <v>0.12549019607843137</v>
+      </c>
+      <c r="J7" s="18"/>
+      <c r="K7" s="28">
+        <f t="shared" ref="K7" si="0">F7/255</f>
+        <v>3.9215686274509803E-3</v>
+      </c>
+      <c r="L7" s="28">
+        <f>G7/255</f>
+        <v>0.27843137254901962</v>
+      </c>
+      <c r="M7" s="28">
+        <f>H7/255</f>
+        <v>0.67450980392156867</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" s="19">
+        <f>(E6/E7)^(1/D23)-1</f>
+        <v>0.20327557333048119</v>
+      </c>
+      <c r="F8" s="19">
+        <f>(F6/F7)^(1/D23)-1</f>
+        <v>0.6451973109700686</v>
+      </c>
+      <c r="G8" s="19">
+        <f>(G6/G7)^(1/D23)-1</f>
+        <v>0.11918196529982739</v>
+      </c>
+      <c r="H8" s="19">
+        <f>(H6/H7)^(1/D23)-1</f>
+        <v>3.6445621596678857E-2</v>
+      </c>
+      <c r="I8" s="19">
+        <f>(I6/I7)^(1/D23)-1</f>
+        <v>0.20327557333048119</v>
+      </c>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19">
+        <f>(K6/K7)^(1/D23)-1</f>
+        <v>0.6451973109700686</v>
+      </c>
+      <c r="L8" s="19">
+        <f>(L6/L7)^(1/D23)-1</f>
+        <v>0.11918196529982739</v>
+      </c>
+      <c r="M8" s="19">
+        <f>(M6/M7)^(1/D23)-1</f>
+        <v>3.6445621596678857E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <f>$E$7*(1+$E$8)^D12</f>
+        <v>32</v>
+      </c>
+      <c r="F12" s="20">
+        <f>$F$7*(1+$F$8)^D12</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="20">
+        <f>$G$7*(1+$G$8)^D12</f>
+        <v>71</v>
+      </c>
+      <c r="H12" s="20">
+        <f>$H$7*(1+$H$8)^D12</f>
+        <v>172</v>
+      </c>
+      <c r="I12" s="18">
+        <f>E12/255</f>
+        <v>0.12549019607843137</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K12" s="28">
+        <f>F12/255</f>
+        <v>3.9215686274509803E-3</v>
+      </c>
+      <c r="L12" s="28">
+        <f t="shared" ref="L12:L23" si="1">G12/255</f>
+        <v>0.27843137254901962</v>
+      </c>
+      <c r="M12" s="28">
+        <f t="shared" ref="M12:M23" si="2">H12/255</f>
+        <v>0.67450980392156867</v>
+      </c>
+      <c r="N12" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O12" s="18">
+        <f>$P$6*(1+$Q$6)^D12</f>
+        <v>0.8</v>
+      </c>
+      <c r="P12" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="20">
+        <f t="shared" ref="E13:E23" si="3">$E$7*(1+$E$8)^D13</f>
+        <v>38.504818346575398</v>
+      </c>
+      <c r="F13" s="20">
+        <f>$F$7*(1+$F$8)^D13</f>
+        <v>1.6451973109700686</v>
+      </c>
+      <c r="G13" s="20">
+        <f>$G$7*(1+$G$8)^D13</f>
+        <v>79.461919536287738</v>
+      </c>
+      <c r="H13" s="20">
+        <f>$H$7*(1+$H$8)^D13</f>
+        <v>178.26864691462876</v>
+      </c>
+      <c r="I13" s="18">
+        <f>E13/255</f>
+        <v>0.15099928763362902</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K13" s="28">
+        <f t="shared" ref="K13:K23" si="4">F13/255</f>
+        <v>6.451754160666936E-3</v>
+      </c>
+      <c r="L13" s="28">
+        <f t="shared" si="1"/>
+        <v>0.31161537073054013</v>
+      </c>
+      <c r="M13" s="28">
+        <f t="shared" si="2"/>
+        <v>0.69909273299854413</v>
+      </c>
+      <c r="N13" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O13" s="18">
+        <f t="shared" ref="O13:O23" si="5">$P$6*(1+$Q$6)^D13</f>
+        <v>0.93759999999999999</v>
+      </c>
+      <c r="P13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" s="20">
+        <f t="shared" si="3"/>
+        <v>46.331907371961542</v>
+      </c>
+      <c r="F14" s="20">
+        <f>$F$7*(1+$F$8)^D14</f>
+        <v>2.7066741920231445</v>
+      </c>
+      <c r="G14" s="20">
+        <f>$G$7*(1+$G$8)^D14</f>
+        <v>88.932347273119262</v>
+      </c>
+      <c r="H14" s="20">
+        <f>$H$7*(1+$H$8)^D14</f>
+        <v>184.76575856263128</v>
+      </c>
+      <c r="I14" s="18">
+        <f>E14/255</f>
+        <v>0.18169375439984919</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K14" s="28">
+        <f t="shared" si="4"/>
+        <v>1.0614408596169194E-2</v>
+      </c>
+      <c r="L14" s="28">
+        <f t="shared" si="1"/>
+        <v>0.34875430303184024</v>
+      </c>
+      <c r="M14" s="28">
+        <f t="shared" si="2"/>
+        <v>0.72457160220639716</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O14" s="18">
+        <f t="shared" si="5"/>
+        <v>1.0988671999999999</v>
+      </c>
+      <c r="P14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="20">
+        <f t="shared" si="3"/>
+        <v>55.750052406491768</v>
+      </c>
+      <c r="F15" s="20">
+        <f>$F$7*(1+$F$8)^D15</f>
+        <v>4.4530131023885602</v>
+      </c>
+      <c r="G15" s="20">
+        <f>$G$7*(1+$G$8)^D15</f>
+        <v>99.531479199856363</v>
+      </c>
+      <c r="H15" s="20">
+        <f>$H$7*(1+$H$8)^D15</f>
+        <v>191.49966148322827</v>
+      </c>
+      <c r="I15" s="18">
+        <f>E15/255</f>
+        <v>0.21862765649604615</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K15" s="28">
+        <f t="shared" si="4"/>
+        <v>1.7462796479955137E-2</v>
+      </c>
+      <c r="L15" s="28">
+        <f t="shared" si="1"/>
+        <v>0.3903195262739465</v>
+      </c>
+      <c r="M15" s="28">
+        <f t="shared" si="2"/>
+        <v>0.75097906464011088</v>
+      </c>
+      <c r="N15" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O15" s="18">
+        <f t="shared" si="5"/>
+        <v>1.2878723583999998</v>
+      </c>
+      <c r="P15" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16" s="20">
+        <f t="shared" si="3"/>
+        <v>67.082676272625761</v>
+      </c>
+      <c r="F16" s="20">
+        <f>$F$7*(1+$F$8)^D16</f>
+        <v>7.3260851817641424</v>
+      </c>
+      <c r="G16" s="20">
+        <f>$G$7*(1+$G$8)^D16</f>
+        <v>111.39383650009412</v>
+      </c>
+      <c r="H16" s="20">
+        <f>$H$7*(1+$H$8)^D16</f>
+        <v>198.47898568153812</v>
+      </c>
+      <c r="I16" s="18">
+        <f>E16/255</f>
+        <v>0.26306931871617945</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K16" s="28">
+        <f t="shared" si="4"/>
+        <v>2.8729745810839775E-2</v>
+      </c>
+      <c r="L16" s="28">
+        <f t="shared" si="1"/>
+        <v>0.43683857451017305</v>
+      </c>
+      <c r="M16" s="28">
+        <f t="shared" si="2"/>
+        <v>0.77834896345701221</v>
+      </c>
+      <c r="N16" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O16" s="18">
+        <f t="shared" si="5"/>
+        <v>1.5093864040448</v>
+      </c>
+      <c r="P16" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="3"/>
+        <v>80.718945752486832</v>
+      </c>
+      <c r="F17" s="20">
+        <f>$F$7*(1+$F$8)^D17</f>
+        <v>12.052855640976034</v>
+      </c>
+      <c r="G17" s="20">
+        <f>$G$7*(1+$G$8)^D17</f>
+        <v>124.66997285646299</v>
+      </c>
+      <c r="H17" s="20">
+        <f>$H$7*(1+$H$8)^D17</f>
+        <v>205.71267568858008</v>
+      </c>
+      <c r="I17" s="18">
+        <f>E17/255</f>
+        <v>0.31654488530386993</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K17" s="28">
+        <f t="shared" si="4"/>
+        <v>4.726610055284719E-2</v>
+      </c>
+      <c r="L17" s="28">
+        <f t="shared" si="1"/>
+        <v>0.48890185433907057</v>
+      </c>
+      <c r="M17" s="28">
+        <f t="shared" si="2"/>
+        <v>0.80671637524933359</v>
+      </c>
+      <c r="N17" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O17" s="18">
+        <f t="shared" si="5"/>
+        <v>1.7690008655405052</v>
+      </c>
+      <c r="P17" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18" s="20">
+        <f t="shared" si="3"/>
+        <v>97.127135728955594</v>
+      </c>
+      <c r="F18" s="20">
+        <f>$F$7*(1+$F$8)^D18</f>
+        <v>19.829325690044193</v>
+      </c>
+      <c r="G18" s="20">
+        <f>$G$7*(1+$G$8)^D18</f>
+        <v>139.52838523537238</v>
+      </c>
+      <c r="H18" s="20">
+        <f>$H$7*(1+$H$8)^D18</f>
+        <v>213.21000202436642</v>
+      </c>
+      <c r="I18" s="18">
+        <f>E18/255</f>
+        <v>0.38089072834884546</v>
+      </c>
+      <c r="J18" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K18" s="28">
+        <f t="shared" si="4"/>
+        <v>7.7762061529585078E-2</v>
+      </c>
+      <c r="L18" s="28">
+        <f t="shared" si="1"/>
+        <v>0.54717013817793092</v>
+      </c>
+      <c r="M18" s="28">
+        <f t="shared" si="2"/>
+        <v>0.83611765499751534</v>
+      </c>
+      <c r="N18" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O18" s="18">
+        <f t="shared" si="5"/>
+        <v>2.0732690144134724</v>
+      </c>
+      <c r="P18" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19" s="20">
+        <f t="shared" si="3"/>
+        <v>116.8707099302065</v>
+      </c>
+      <c r="F19" s="20">
+        <f>$F$7*(1+$F$8)^D19</f>
+        <v>32.623153303610401</v>
+      </c>
+      <c r="G19" s="20">
+        <f>$G$7*(1+$G$8)^D19</f>
+        <v>156.15765240283548</v>
+      </c>
+      <c r="H19" s="20">
+        <f>$H$7*(1+$H$8)^D19</f>
+        <v>220.98057307877357</v>
+      </c>
+      <c r="I19" s="18">
+        <f>E19/255</f>
+        <v>0.45831650953022157</v>
+      </c>
+      <c r="J19" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K19" s="28">
+        <f t="shared" si="4"/>
+        <v>0.12793393452396234</v>
+      </c>
+      <c r="L19" s="28">
+        <f t="shared" si="1"/>
+        <v>0.61238295059935488</v>
+      </c>
+      <c r="M19" s="28">
+        <f t="shared" si="2"/>
+        <v>0.86659048266185712</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O19" s="18">
+        <f t="shared" si="5"/>
+        <v>2.4298712848925894</v>
+      </c>
+      <c r="P19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D20">
         <v>8</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="18"/>
-    </row>
-    <row r="3" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="5">
-        <f t="shared" ref="B4:B19" si="0">ROW(B2)-1</f>
-        <v>1</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="5">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="5">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="5">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="5">
-        <f t="shared" si="0"/>
+      <c r="E20" s="20">
+        <f t="shared" si="3"/>
+        <v>140.6276704968096</v>
+      </c>
+      <c r="F20" s="20">
+        <f>$F$7*(1+$F$8)^D20</f>
+        <v>53.671524090464146</v>
+      </c>
+      <c r="G20" s="20">
+        <f>$G$7*(1+$G$8)^D20</f>
+        <v>174.76882831281273</v>
+      </c>
+      <c r="H20" s="20">
+        <f>$H$7*(1+$H$8)^D20</f>
+        <v>229.03434742541981</v>
+      </c>
+      <c r="I20" s="18">
+        <f>E20/255</f>
+        <v>0.55148106077180237</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K20" s="28">
+        <f t="shared" si="4"/>
+        <v>0.21047656506064372</v>
+      </c>
+      <c r="L20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.68536795416789309</v>
+      </c>
+      <c r="M20" s="28">
+        <f t="shared" si="2"/>
+        <v>0.89817391147223458</v>
+      </c>
+      <c r="N20" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O20" s="18">
+        <f t="shared" si="5"/>
+        <v>2.8478091458941148</v>
+      </c>
+      <c r="P20" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D21">
         <v>9</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="5">
-        <f t="shared" si="0"/>
+      <c r="E21" s="20">
+        <f t="shared" si="3"/>
+        <v>169.21384084317856</v>
+      </c>
+      <c r="F21" s="20">
+        <f>$F$7*(1+$F$8)^D21</f>
+        <v>88.300247109296876</v>
+      </c>
+      <c r="G21" s="20">
+        <f>$G$7*(1+$G$8)^D21</f>
+        <v>195.59812074428189</v>
+      </c>
+      <c r="H21" s="20">
+        <f>$H$7*(1+$H$8)^D21</f>
+        <v>237.38164658432893</v>
+      </c>
+      <c r="I21" s="18">
+        <f>E21/255</f>
+        <v>0.66358368958109237</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K21" s="28">
+        <f t="shared" si="4"/>
+        <v>0.34627547885998777</v>
+      </c>
+      <c r="L21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.76705145389914464</v>
+      </c>
+      <c r="M21" s="28">
+        <f t="shared" si="2"/>
+        <v>0.93090841797776047</v>
+      </c>
+      <c r="N21" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O21" s="18">
+        <f t="shared" si="5"/>
+        <v>3.3376323189879025</v>
+      </c>
+      <c r="P21" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D22">
         <v>10</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="5">
-        <f t="shared" si="0"/>
+      <c r="E22" s="20">
+        <f t="shared" si="3"/>
+        <v>203.61088135602847</v>
+      </c>
+      <c r="F22" s="20">
+        <f>$F$7*(1+$F$8)^D22</f>
+        <v>145.27132910220777</v>
+      </c>
+      <c r="G22" s="20">
+        <f>$G$7*(1+$G$8)^D22</f>
+        <v>218.90988918353833</v>
+      </c>
+      <c r="H22" s="20">
+        <f>$H$7*(1+$H$8)^D22</f>
+        <v>246.033168249738</v>
+      </c>
+      <c r="I22" s="18">
+        <f>E22/255</f>
+        <v>0.79847404453344495</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K22" s="28">
+        <f t="shared" si="4"/>
+        <v>0.56969148667532454</v>
+      </c>
+      <c r="L22" s="28">
+        <f t="shared" si="1"/>
+        <v>0.8584701536609346</v>
+      </c>
+      <c r="M22" s="28">
+        <f t="shared" si="2"/>
+        <v>0.96483595392054111</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O22" s="18">
+        <f t="shared" si="5"/>
+        <v>3.9117050778538216</v>
+      </c>
+      <c r="P22" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D23">
         <v>11</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="5">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="5">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="5">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="5">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="5">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="E23" s="20">
+        <f t="shared" si="3"/>
+        <v>244.99999999999974</v>
+      </c>
+      <c r="F23" s="20">
+        <f>$F$7*(1+$F$8)^D23</f>
+        <v>239.00000000000009</v>
+      </c>
+      <c r="G23" s="20">
+        <f>$G$7*(1+$G$8)^D23</f>
+        <v>244.99999999999983</v>
+      </c>
+      <c r="H23" s="20">
+        <f>$H$7*(1+$H$8)^D23</f>
+        <v>254.99999999999991</v>
+      </c>
+      <c r="I23" s="18">
+        <f>E23/255</f>
+        <v>0.96078431372548923</v>
+      </c>
+      <c r="J23" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="K23" s="28">
+        <f t="shared" si="4"/>
+        <v>0.93725490196078465</v>
+      </c>
+      <c r="L23" s="28">
+        <f t="shared" si="1"/>
+        <v>0.96078431372548956</v>
+      </c>
+      <c r="M23" s="28">
+        <f t="shared" si="2"/>
+        <v>0.99999999999999967</v>
+      </c>
+      <c r="N23" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="O23" s="18">
+        <f t="shared" si="5"/>
+        <v>4.5845183512446779</v>
+      </c>
+      <c r="P23" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="E24" s="18"/>
+      <c r="F24" s="20"/>
+      <c r="N24" s="18"/>
+      <c r="P24"/>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="N25" s="18"/>
+      <c r="P25"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
+  <mergeCells count="2">
+    <mergeCell ref="E4:H4"/>
+    <mergeCell ref="I4:M4"/>
   </mergeCells>
-  <phoneticPr fontId="0" type="noConversion"/>
-  <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>